<commit_message>
currently working but is not dynamic and not fitting with other sets. Will need modifications
</commit_message>
<xml_diff>
--- a/Expected Value and Cost Ratio Calculator Pokemon/excelDocs/scarletAndViolet151/pokemon_data.xlsx
+++ b/Expected Value and Cost Ratio Calculator Pokemon/excelDocs/scarletAndViolet151/pokemon_data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1350" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="797" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-27375" yWindow="90" windowWidth="25260" windowHeight="11385" tabRatio="797" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data'!$A$1:$N$210</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data'!$A$1:$K$210</definedName>
   </definedNames>
   <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
@@ -21,7 +21,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,10 +41,15 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -53,16 +58,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00D9D9D9"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -90,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -114,6 +139,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -481,10 +518,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1263"/>
+  <dimension ref="A1:K1263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -498,9 +535,6 @@
     <col width="33.5703125" customWidth="1" min="7" max="8"/>
     <col width="32.42578125" customWidth="1" min="9" max="10"/>
     <col width="39.42578125" customWidth="1" min="11" max="11"/>
-    <col width="16.85546875" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="6" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -559,21 +593,6 @@
           <t>Current Market Price of ETB Promo Card</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>EV Component</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Total EV</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>EVR</t>
-        </is>
-      </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
@@ -590,21 +609,21 @@
         <v>46</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>0.15</v>
       </c>
       <c r="F2" s="3">
-        <f>IF(B2="common", 4, IF(B2="uncommon", 3, IF(B2="rare", 1.22, 1)))</f>
+        <f>IF(B2="common", 4, IF(B2="uncommon", 3, IF(B2="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="G2">
-        <f>SUMPRODUCT(F2:F210, D2:D210/ C2:C210)</f>
+        <f>SUM(H2:H10)</f>
         <v/>
       </c>
       <c r="H2">
-        <f>SUMPRODUCT((B2:B210="Common") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>SUMPRODUCT((B2:B217="Common") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
       <c r="I2" s="3" t="n">
@@ -632,21 +651,17 @@
         <v>21</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.7</v>
+        <v>0.55</v>
       </c>
       <c r="F3" s="3">
-        <f>IF(B3="common", 4, IF(B3="uncommon", 3, IF(B3="rare", 1.22, 1)))</f>
-        <v/>
-      </c>
-      <c r="G3">
-        <f>SUM(H2:H9)</f>
+        <f>IF(B3="common", 4, IF(B3="uncommon", 3, IF(B3="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H3">
-        <f>SUMPRODUCT((B2:B210="Uncommon") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>SUMPRODUCT((B2:B217="Uncommon") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -665,11 +680,11 @@
         <v>90</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.74</v>
+        <v>1.12</v>
       </c>
       <c r="E4" s="3" t="inlineStr"/>
       <c r="F4" s="3">
-        <f>IF(B4="common", 4, IF(B4="uncommon", 3, IF(B4="rare", 1.22, 1)))</f>
+        <f>IF(B4="common", 4, IF(B4="uncommon", 3, IF(B4="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H4">
@@ -692,15 +707,15 @@
         <v>248</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>7.64</v>
+        <v>7.46</v>
       </c>
       <c r="E5" s="3" t="inlineStr"/>
       <c r="F5" s="3">
-        <f>IF(B5="common", 4, IF(B5="uncommon", 3, IF(B5="rare", 1.22, 1)))</f>
+        <f>IF(B5="common", 4, IF(B5="uncommon", 3, IF(B5="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H5">
-        <f>SUMPRODUCT((B2:B210="Double Rare") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>SUMPRODUCT((B2:B217="Double Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -719,11 +734,11 @@
         <v>225</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>39.98</v>
+        <v>43.34</v>
       </c>
       <c r="E6" s="3" t="inlineStr"/>
       <c r="F6" s="3">
-        <f>IF(B6="common", 4, IF(B6="uncommon", 3, IF(B6="rare", 1.22, 1)))</f>
+        <f>IF(B6="common", 4, IF(B6="uncommon", 3, IF(B6="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H6">
@@ -746,17 +761,17 @@
         <v>46</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>0.64</v>
       </c>
       <c r="F7" s="3">
-        <f>IF(B7="common", 4, IF(B7="uncommon", 3, IF(B7="rare", 1.22, 1)))</f>
+        <f>IF(B7="common", 4, IF(B7="uncommon", 3, IF(B7="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H7">
-        <f>SUMPRODUCT((B2:B210="Illustration Rare") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>SUMPRODUCT((B2:B217="Illustration Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -775,17 +790,17 @@
         <v>46</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>1.39</v>
+        <v>1.06</v>
       </c>
       <c r="F8" s="3">
-        <f>IF(B8="common", 4, IF(B8="uncommon", 3, IF(B8="rare", 1.22, 1)))</f>
+        <f>IF(B8="common", 4, IF(B8="uncommon", 3, IF(B8="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H8">
-        <f>SUMPRODUCT((B2:B210="Special Illustration Rare") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>SUMPRODUCT((B2:B217="Special Illustration Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -804,17 +819,17 @@
         <v>46</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="F9" s="3">
-        <f>IF(B9="common", 4, IF(B9="uncommon", 3, IF(B9="rare", 1.22, 1)))</f>
+        <f>IF(B9="common", 4, IF(B9="uncommon", 3, IF(B9="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H9">
-        <f>SUMPRODUCT((B2:B210="Ultra Rare") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>SUMPRODUCT((B2:B217="Ultra Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -833,11 +848,15 @@
         <v>90</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="E10" s="3" t="inlineStr"/>
       <c r="F10" s="3">
-        <f>IF(B10="common", 4, IF(B10="uncommon", 3, IF(B10="rare", 1.22, 1)))</f>
+        <f>IF(B10="common", 4, IF(B10="uncommon", 3, IF(B10="rare", 1.74127216869152, 1)))</f>
+        <v/>
+      </c>
+      <c r="H10">
+        <f>1.88 * SUMPRODUCT((C2:C217&lt;&gt;"") * (E2:E217&lt;&gt;"") * (E2:E217 / C2:C217))</f>
         <v/>
       </c>
     </row>
@@ -856,11 +875,11 @@
         <v>248</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>5.46</v>
+        <v>4.89</v>
       </c>
       <c r="E11" s="3" t="inlineStr"/>
       <c r="F11" s="3">
-        <f>IF(B11="common", 4, IF(B11="uncommon", 3, IF(B11="rare", 1.22, 1)))</f>
+        <f>IF(B11="common", 4, IF(B11="uncommon", 3, IF(B11="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -879,13 +898,13 @@
         <v>33</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="F12" s="3">
-        <f>IF(B12="common", 4, IF(B12="uncommon", 3, IF(B12="rare", 1.22, 1)))</f>
+        <f>IF(B12="common", 4, IF(B12="uncommon", 3, IF(B12="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -904,13 +923,13 @@
         <v>21</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>0.88</v>
+        <v>0.74</v>
       </c>
       <c r="F13" s="3">
-        <f>IF(B13="common", 4, IF(B13="uncommon", 3, IF(B13="rare", 1.22, 1)))</f>
+        <f>IF(B13="common", 4, IF(B13="uncommon", 3, IF(B13="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -929,11 +948,11 @@
         <v>154</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>5.36</v>
+        <v>4.95</v>
       </c>
       <c r="E14" s="3" t="inlineStr"/>
       <c r="F14" s="3">
-        <f>IF(B14="common", 4, IF(B14="uncommon", 3, IF(B14="rare", 1.22, 1)))</f>
+        <f>IF(B14="common", 4, IF(B14="uncommon", 3, IF(B14="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -952,13 +971,13 @@
         <v>21</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="F15" s="3">
-        <f>IF(B15="common", 4, IF(B15="uncommon", 3, IF(B15="rare", 1.22, 1)))</f>
+        <f>IF(B15="common", 4, IF(B15="uncommon", 3, IF(B15="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -977,13 +996,13 @@
         <v>46</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>0.14</v>
       </c>
       <c r="F16" s="3">
-        <f>IF(B16="common", 4, IF(B16="uncommon", 3, IF(B16="rare", 1.22, 1)))</f>
+        <f>IF(B16="common", 4, IF(B16="uncommon", 3, IF(B16="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1002,13 +1021,13 @@
         <v>33</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>0.12</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>1.25</v>
+        <v>1.12</v>
       </c>
       <c r="F17" s="3">
-        <f>IF(B17="common", 4, IF(B17="uncommon", 3, IF(B17="rare", 1.22, 1)))</f>
+        <f>IF(B17="common", 4, IF(B17="uncommon", 3, IF(B17="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1027,13 +1046,13 @@
         <v>33</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F18" s="3">
-        <f>IF(B18="common", 4, IF(B18="uncommon", 3, IF(B18="rare", 1.22, 1)))</f>
+        <f>IF(B18="common", 4, IF(B18="uncommon", 3, IF(B18="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1052,11 +1071,11 @@
         <v>248</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>2.77</v>
+        <v>3.05</v>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
       <c r="F19" s="3">
-        <f>IF(B19="common", 4, IF(B19="uncommon", 3, IF(B19="rare", 1.22, 1)))</f>
+        <f>IF(B19="common", 4, IF(B19="uncommon", 3, IF(B19="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1075,11 +1094,11 @@
         <v>90</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>0.66</v>
+        <v>1.18</v>
       </c>
       <c r="E20" s="3" t="inlineStr"/>
       <c r="F20" s="3">
-        <f>IF(B20="common", 4, IF(B20="uncommon", 3, IF(B20="rare", 1.22, 1)))</f>
+        <f>IF(B20="common", 4, IF(B20="uncommon", 3, IF(B20="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1098,11 +1117,11 @@
         <v>248</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>14.54</v>
+        <v>14.89</v>
       </c>
       <c r="E21" s="3" t="inlineStr"/>
       <c r="F21" s="3">
-        <f>IF(B21="common", 4, IF(B21="uncommon", 3, IF(B21="rare", 1.22, 1)))</f>
+        <f>IF(B21="common", 4, IF(B21="uncommon", 3, IF(B21="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1121,11 +1140,11 @@
         <v>225</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>70.20999999999999</v>
+        <v>73.55</v>
       </c>
       <c r="E22" s="3" t="inlineStr"/>
       <c r="F22" s="3">
-        <f>IF(B22="common", 4, IF(B22="uncommon", 3, IF(B22="rare", 1.22, 1)))</f>
+        <f>IF(B22="common", 4, IF(B22="uncommon", 3, IF(B22="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1144,13 +1163,13 @@
         <v>46</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>0.12</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="F23" s="3">
-        <f>IF(B23="common", 4, IF(B23="uncommon", 3, IF(B23="rare", 1.22, 1)))</f>
+        <f>IF(B23="common", 4, IF(B23="uncommon", 3, IF(B23="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1169,11 +1188,11 @@
         <v>188</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>37.17</v>
+        <v>37.52</v>
       </c>
       <c r="E24" s="3" t="inlineStr"/>
       <c r="F24" s="3">
-        <f>IF(B24="common", 4, IF(B24="uncommon", 3, IF(B24="rare", 1.22, 1)))</f>
+        <f>IF(B24="common", 4, IF(B24="uncommon", 3, IF(B24="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1192,13 +1211,13 @@
         <v>33</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F25" s="3">
-        <f>IF(B25="common", 4, IF(B25="uncommon", 3, IF(B25="rare", 1.22, 1)))</f>
+        <f>IF(B25="common", 4, IF(B25="uncommon", 3, IF(B25="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1217,13 +1236,13 @@
         <v>46</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>0.13</v>
+        <v>0.21</v>
       </c>
       <c r="F26" s="3">
-        <f>IF(B26="common", 4, IF(B26="uncommon", 3, IF(B26="rare", 1.22, 1)))</f>
+        <f>IF(B26="common", 4, IF(B26="uncommon", 3, IF(B26="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1242,11 +1261,11 @@
         <v>188</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>9.66</v>
+        <v>9.56</v>
       </c>
       <c r="E27" s="3" t="inlineStr"/>
       <c r="F27" s="3">
-        <f>IF(B27="common", 4, IF(B27="uncommon", 3, IF(B27="rare", 1.22, 1)))</f>
+        <f>IF(B27="common", 4, IF(B27="uncommon", 3, IF(B27="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1265,13 +1284,13 @@
         <v>21</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>0.86</v>
+        <v>0.65</v>
       </c>
       <c r="F28" s="3">
-        <f>IF(B28="common", 4, IF(B28="uncommon", 3, IF(B28="rare", 1.22, 1)))</f>
+        <f>IF(B28="common", 4, IF(B28="uncommon", 3, IF(B28="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1290,11 +1309,11 @@
         <v>90</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>4.54</v>
+        <v>4.71</v>
       </c>
       <c r="E29" s="3" t="inlineStr"/>
       <c r="F29" s="3">
-        <f>IF(B29="common", 4, IF(B29="uncommon", 3, IF(B29="rare", 1.22, 1)))</f>
+        <f>IF(B29="common", 4, IF(B29="uncommon", 3, IF(B29="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1313,11 +1332,11 @@
         <v>248</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>29.54</v>
+        <v>31.27</v>
       </c>
       <c r="E30" s="3" t="inlineStr"/>
       <c r="F30" s="3">
-        <f>IF(B30="common", 4, IF(B30="uncommon", 3, IF(B30="rare", 1.22, 1)))</f>
+        <f>IF(B30="common", 4, IF(B30="uncommon", 3, IF(B30="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1336,11 +1355,11 @@
         <v>225</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>210.03</v>
+        <v>210.14</v>
       </c>
       <c r="E31" s="3" t="inlineStr"/>
       <c r="F31" s="3">
-        <f>IF(B31="common", 4, IF(B31="uncommon", 3, IF(B31="rare", 1.22, 1)))</f>
+        <f>IF(B31="common", 4, IF(B31="uncommon", 3, IF(B31="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1359,13 +1378,13 @@
         <v>46</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>0.19</v>
       </c>
       <c r="F32" s="3">
-        <f>IF(B32="common", 4, IF(B32="uncommon", 3, IF(B32="rare", 1.22, 1)))</f>
+        <f>IF(B32="common", 4, IF(B32="uncommon", 3, IF(B32="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1384,11 +1403,11 @@
         <v>188</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>46.71</v>
+        <v>52.06</v>
       </c>
       <c r="E33" s="3" t="inlineStr"/>
       <c r="F33" s="3">
-        <f>IF(B33="common", 4, IF(B33="uncommon", 3, IF(B33="rare", 1.22, 1)))</f>
+        <f>IF(B33="common", 4, IF(B33="uncommon", 3, IF(B33="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1410,10 +1429,10 @@
         <v>0.1</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="F34" s="3">
-        <f>IF(B34="common", 4, IF(B34="uncommon", 3, IF(B34="rare", 1.22, 1)))</f>
+        <f>IF(B34="common", 4, IF(B34="uncommon", 3, IF(B34="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1432,11 +1451,11 @@
         <v>188</v>
       </c>
       <c r="D35" s="3" t="n">
-        <v>32.96</v>
+        <v>34.86</v>
       </c>
       <c r="E35" s="3" t="inlineStr"/>
       <c r="F35" s="3">
-        <f>IF(B35="common", 4, IF(B35="uncommon", 3, IF(B35="rare", 1.22, 1)))</f>
+        <f>IF(B35="common", 4, IF(B35="uncommon", 3, IF(B35="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1455,13 +1474,13 @@
         <v>33</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E36" s="3" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="F36" s="3">
-        <f>IF(B36="common", 4, IF(B36="uncommon", 3, IF(B36="rare", 1.22, 1)))</f>
+        <f>IF(B36="common", 4, IF(B36="uncommon", 3, IF(B36="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1480,13 +1499,13 @@
         <v>46</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="F37" s="3">
-        <f>IF(B37="common", 4, IF(B37="uncommon", 3, IF(B37="rare", 1.22, 1)))</f>
+        <f>IF(B37="common", 4, IF(B37="uncommon", 3, IF(B37="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1505,13 +1524,13 @@
         <v>33</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E38" s="3" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="F38" s="3">
-        <f>IF(B38="common", 4, IF(B38="uncommon", 3, IF(B38="rare", 1.22, 1)))</f>
+        <f>IF(B38="common", 4, IF(B38="uncommon", 3, IF(B38="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1530,13 +1549,13 @@
         <v>46</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>0.18</v>
+        <v>0.14</v>
       </c>
       <c r="F39" s="3">
-        <f>IF(B39="common", 4, IF(B39="uncommon", 3, IF(B39="rare", 1.22, 1)))</f>
+        <f>IF(B39="common", 4, IF(B39="uncommon", 3, IF(B39="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1555,13 +1574,13 @@
         <v>33</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E40" s="3" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="F40" s="3">
-        <f>IF(B40="common", 4, IF(B40="uncommon", 3, IF(B40="rare", 1.22, 1)))</f>
+        <f>IF(B40="common", 4, IF(B40="uncommon", 3, IF(B40="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1583,10 +1602,10 @@
         <v>0.09</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="F41" s="3">
-        <f>IF(B41="common", 4, IF(B41="uncommon", 3, IF(B41="rare", 1.22, 1)))</f>
+        <f>IF(B41="common", 4, IF(B41="uncommon", 3, IF(B41="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1605,11 +1624,11 @@
         <v>248</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>3.42</v>
+        <v>4.04</v>
       </c>
       <c r="E42" s="3" t="inlineStr"/>
       <c r="F42" s="3">
-        <f>IF(B42="common", 4, IF(B42="uncommon", 3, IF(B42="rare", 1.22, 1)))</f>
+        <f>IF(B42="common", 4, IF(B42="uncommon", 3, IF(B42="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1631,10 +1650,10 @@
         <v>0.06</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F43" s="3">
-        <f>IF(B43="common", 4, IF(B43="uncommon", 3, IF(B43="rare", 1.22, 1)))</f>
+        <f>IF(B43="common", 4, IF(B43="uncommon", 3, IF(B43="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1656,10 +1675,10 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E44" s="3" t="n">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="F44" s="3">
-        <f>IF(B44="common", 4, IF(B44="uncommon", 3, IF(B44="rare", 1.22, 1)))</f>
+        <f>IF(B44="common", 4, IF(B44="uncommon", 3, IF(B44="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1678,13 +1697,13 @@
         <v>21</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>0.28</v>
+        <v>0.26</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>0.84</v>
+        <v>0.64</v>
       </c>
       <c r="F45" s="3">
-        <f>IF(B45="common", 4, IF(B45="uncommon", 3, IF(B45="rare", 1.22, 1)))</f>
+        <f>IF(B45="common", 4, IF(B45="uncommon", 3, IF(B45="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1703,11 +1722,11 @@
         <v>21</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="E46" s="3" t="inlineStr"/>
       <c r="F46" s="3">
-        <f>IF(B46="common", 4, IF(B46="uncommon", 3, IF(B46="rare", 1.22, 1)))</f>
+        <f>IF(B46="common", 4, IF(B46="uncommon", 3, IF(B46="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1729,10 +1748,10 @@
         <v>0.14</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>0.68</v>
+        <v>0.63</v>
       </c>
       <c r="F47" s="3">
-        <f>IF(B47="common", 4, IF(B47="uncommon", 3, IF(B47="rare", 1.22, 1)))</f>
+        <f>IF(B47="common", 4, IF(B47="uncommon", 3, IF(B47="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1754,10 +1773,10 @@
         <v>0.06</v>
       </c>
       <c r="E48" s="3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="F48" s="3">
-        <f>IF(B48="common", 4, IF(B48="uncommon", 3, IF(B48="rare", 1.22, 1)))</f>
+        <f>IF(B48="common", 4, IF(B48="uncommon", 3, IF(B48="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1779,10 +1798,10 @@
         <v>0.11</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>1.86</v>
+        <v>2</v>
       </c>
       <c r="F49" s="3">
-        <f>IF(B49="common", 4, IF(B49="uncommon", 3, IF(B49="rare", 1.22, 1)))</f>
+        <f>IF(B49="common", 4, IF(B49="uncommon", 3, IF(B49="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1801,11 +1820,11 @@
         <v>188</v>
       </c>
       <c r="D50" s="3" t="n">
-        <v>22.83</v>
+        <v>25.78</v>
       </c>
       <c r="E50" s="3" t="inlineStr"/>
       <c r="F50" s="3">
-        <f>IF(B50="common", 4, IF(B50="uncommon", 3, IF(B50="rare", 1.22, 1)))</f>
+        <f>IF(B50="common", 4, IF(B50="uncommon", 3, IF(B50="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1824,13 +1843,13 @@
         <v>21</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>0.32</v>
+        <v>0.41</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>1.54</v>
+        <v>1.32</v>
       </c>
       <c r="F51" s="3">
-        <f>IF(B51="common", 4, IF(B51="uncommon", 3, IF(B51="rare", 1.22, 1)))</f>
+        <f>IF(B51="common", 4, IF(B51="uncommon", 3, IF(B51="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1849,13 +1868,13 @@
         <v>46</v>
       </c>
       <c r="D52" s="3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="F52" s="3">
-        <f>IF(B52="common", 4, IF(B52="uncommon", 3, IF(B52="rare", 1.22, 1)))</f>
+        <f>IF(B52="common", 4, IF(B52="uncommon", 3, IF(B52="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1874,13 +1893,13 @@
         <v>46</v>
       </c>
       <c r="D53" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F53" s="3">
-        <f>IF(B53="common", 4, IF(B53="uncommon", 3, IF(B53="rare", 1.22, 1)))</f>
+        <f>IF(B53="common", 4, IF(B53="uncommon", 3, IF(B53="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1902,10 +1921,10 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>0.31</v>
+        <v>0.13</v>
       </c>
       <c r="F54" s="3">
-        <f>IF(B54="common", 4, IF(B54="uncommon", 3, IF(B54="rare", 1.22, 1)))</f>
+        <f>IF(B54="common", 4, IF(B54="uncommon", 3, IF(B54="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1924,13 +1943,13 @@
         <v>46</v>
       </c>
       <c r="D55" s="3" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
       <c r="F55" s="3">
-        <f>IF(B55="common", 4, IF(B55="uncommon", 3, IF(B55="rare", 1.22, 1)))</f>
+        <f>IF(B55="common", 4, IF(B55="uncommon", 3, IF(B55="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1949,13 +1968,13 @@
         <v>46</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E56" s="3" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="F56" s="3">
-        <f>IF(B56="common", 4, IF(B56="uncommon", 3, IF(B56="rare", 1.22, 1)))</f>
+        <f>IF(B56="common", 4, IF(B56="uncommon", 3, IF(B56="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -1974,13 +1993,13 @@
         <v>46</v>
       </c>
       <c r="D57" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="F57" s="3">
-        <f>IF(B57="common", 4, IF(B57="uncommon", 3, IF(B57="rare", 1.22, 1)))</f>
+        <f>IF(B57="common", 4, IF(B57="uncommon", 3, IF(B57="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2002,10 +2021,10 @@
         <v>0.13</v>
       </c>
       <c r="E58" s="3" t="n">
-        <v>1.68</v>
+        <v>1.27</v>
       </c>
       <c r="F58" s="3">
-        <f>IF(B58="common", 4, IF(B58="uncommon", 3, IF(B58="rare", 1.22, 1)))</f>
+        <f>IF(B58="common", 4, IF(B58="uncommon", 3, IF(B58="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2024,13 +2043,13 @@
         <v>33</v>
       </c>
       <c r="D59" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="F59" s="3">
-        <f>IF(B59="common", 4, IF(B59="uncommon", 3, IF(B59="rare", 1.22, 1)))</f>
+        <f>IF(B59="common", 4, IF(B59="uncommon", 3, IF(B59="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2049,13 +2068,13 @@
         <v>33</v>
       </c>
       <c r="D60" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>0.92</v>
+        <v>0.8</v>
       </c>
       <c r="F60" s="3">
-        <f>IF(B60="common", 4, IF(B60="uncommon", 3, IF(B60="rare", 1.22, 1)))</f>
+        <f>IF(B60="common", 4, IF(B60="uncommon", 3, IF(B60="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2074,11 +2093,11 @@
         <v>248</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>6.39</v>
+        <v>6.99</v>
       </c>
       <c r="E61" s="3" t="inlineStr"/>
       <c r="F61" s="3">
-        <f>IF(B61="common", 4, IF(B61="uncommon", 3, IF(B61="rare", 1.22, 1)))</f>
+        <f>IF(B61="common", 4, IF(B61="uncommon", 3, IF(B61="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2097,11 +2116,11 @@
         <v>225</v>
       </c>
       <c r="D62" s="3" t="n">
-        <v>14.75</v>
+        <v>14.98</v>
       </c>
       <c r="E62" s="3" t="inlineStr"/>
       <c r="F62" s="3">
-        <f>IF(B62="common", 4, IF(B62="uncommon", 3, IF(B62="rare", 1.22, 1)))</f>
+        <f>IF(B62="common", 4, IF(B62="uncommon", 3, IF(B62="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2123,10 +2142,10 @@
         <v>0.05</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="F63" s="3">
-        <f>IF(B63="common", 4, IF(B63="uncommon", 3, IF(B63="rare", 1.22, 1)))</f>
+        <f>IF(B63="common", 4, IF(B63="uncommon", 3, IF(B63="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2145,13 +2164,13 @@
         <v>33</v>
       </c>
       <c r="D64" s="3" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E64" s="3" t="n">
-        <v>1.46</v>
+        <v>1.26</v>
       </c>
       <c r="F64" s="3">
-        <f>IF(B64="common", 4, IF(B64="uncommon", 3, IF(B64="rare", 1.22, 1)))</f>
+        <f>IF(B64="common", 4, IF(B64="uncommon", 3, IF(B64="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2170,13 +2189,13 @@
         <v>46</v>
       </c>
       <c r="D65" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F65" s="3">
-        <f>IF(B65="common", 4, IF(B65="uncommon", 3, IF(B65="rare", 1.22, 1)))</f>
+        <f>IF(B65="common", 4, IF(B65="uncommon", 3, IF(B65="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2195,13 +2214,13 @@
         <v>33</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="F66" s="3">
-        <f>IF(B66="common", 4, IF(B66="uncommon", 3, IF(B66="rare", 1.22, 1)))</f>
+        <f>IF(B66="common", 4, IF(B66="uncommon", 3, IF(B66="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2220,13 +2239,13 @@
         <v>21</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>1.11</v>
+        <v>1.08</v>
       </c>
       <c r="F67" s="3">
-        <f>IF(B67="common", 4, IF(B67="uncommon", 3, IF(B67="rare", 1.22, 1)))</f>
+        <f>IF(B67="common", 4, IF(B67="uncommon", 3, IF(B67="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2245,13 +2264,13 @@
         <v>46</v>
       </c>
       <c r="D68" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F68" s="3">
-        <f>IF(B68="common", 4, IF(B68="uncommon", 3, IF(B68="rare", 1.22, 1)))</f>
+        <f>IF(B68="common", 4, IF(B68="uncommon", 3, IF(B68="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2270,13 +2289,13 @@
         <v>21</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>0.38</v>
+        <v>0.27</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>1.89</v>
+        <v>1.78</v>
       </c>
       <c r="F69" s="3">
-        <f>IF(B69="common", 4, IF(B69="uncommon", 3, IF(B69="rare", 1.22, 1)))</f>
+        <f>IF(B69="common", 4, IF(B69="uncommon", 3, IF(B69="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2301,7 +2320,7 @@
         <v>0.15</v>
       </c>
       <c r="F70" s="3">
-        <f>IF(B70="common", 4, IF(B70="uncommon", 3, IF(B70="rare", 1.22, 1)))</f>
+        <f>IF(B70="common", 4, IF(B70="uncommon", 3, IF(B70="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2320,13 +2339,13 @@
         <v>33</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>1.34</v>
+        <v>1.03</v>
       </c>
       <c r="F71" s="3">
-        <f>IF(B71="common", 4, IF(B71="uncommon", 3, IF(B71="rare", 1.22, 1)))</f>
+        <f>IF(B71="common", 4, IF(B71="uncommon", 3, IF(B71="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2345,11 +2364,11 @@
         <v>248</v>
       </c>
       <c r="D72" s="3" t="n">
-        <v>4.81</v>
+        <v>4.99</v>
       </c>
       <c r="E72" s="3" t="inlineStr"/>
       <c r="F72" s="3">
-        <f>IF(B72="common", 4, IF(B72="uncommon", 3, IF(B72="rare", 1.22, 1)))</f>
+        <f>IF(B72="common", 4, IF(B72="uncommon", 3, IF(B72="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2368,11 +2387,11 @@
         <v>225</v>
       </c>
       <c r="D73" s="3" t="n">
-        <v>13.81</v>
+        <v>15.6</v>
       </c>
       <c r="E73" s="3" t="inlineStr"/>
       <c r="F73" s="3">
-        <f>IF(B73="common", 4, IF(B73="uncommon", 3, IF(B73="rare", 1.22, 1)))</f>
+        <f>IF(B73="common", 4, IF(B73="uncommon", 3, IF(B73="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2391,13 +2410,13 @@
         <v>33</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="F74" s="3">
-        <f>IF(B74="common", 4, IF(B74="uncommon", 3, IF(B74="rare", 1.22, 1)))</f>
+        <f>IF(B74="common", 4, IF(B74="uncommon", 3, IF(B74="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2422,7 +2441,7 @@
         <v>0.18</v>
       </c>
       <c r="F75" s="3">
-        <f>IF(B75="common", 4, IF(B75="uncommon", 3, IF(B75="rare", 1.22, 1)))</f>
+        <f>IF(B75="common", 4, IF(B75="uncommon", 3, IF(B75="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2441,13 +2460,13 @@
         <v>46</v>
       </c>
       <c r="D76" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E76" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F76" s="3">
-        <f>IF(B76="common", 4, IF(B76="uncommon", 3, IF(B76="rare", 1.22, 1)))</f>
+        <f>IF(B76="common", 4, IF(B76="uncommon", 3, IF(B76="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2466,13 +2485,13 @@
         <v>33</v>
       </c>
       <c r="D77" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="F77" s="3">
-        <f>IF(B77="common", 4, IF(B77="uncommon", 3, IF(B77="rare", 1.22, 1)))</f>
+        <f>IF(B77="common", 4, IF(B77="uncommon", 3, IF(B77="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2491,11 +2510,11 @@
         <v>90</v>
       </c>
       <c r="D78" s="3" t="n">
-        <v>0.8</v>
+        <v>0.62</v>
       </c>
       <c r="E78" s="3" t="inlineStr"/>
       <c r="F78" s="3">
-        <f>IF(B78="common", 4, IF(B78="uncommon", 3, IF(B78="rare", 1.22, 1)))</f>
+        <f>IF(B78="common", 4, IF(B78="uncommon", 3, IF(B78="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2514,11 +2533,11 @@
         <v>248</v>
       </c>
       <c r="D79" s="3" t="n">
-        <v>5.64</v>
+        <v>5.18</v>
       </c>
       <c r="E79" s="3" t="inlineStr"/>
       <c r="F79" s="3">
-        <f>IF(B79="common", 4, IF(B79="uncommon", 3, IF(B79="rare", 1.22, 1)))</f>
+        <f>IF(B79="common", 4, IF(B79="uncommon", 3, IF(B79="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2537,13 +2556,13 @@
         <v>33</v>
       </c>
       <c r="D80" s="3" t="n">
-        <v>0.15</v>
+        <v>0.26</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>0.84</v>
+        <v>0.73</v>
       </c>
       <c r="F80" s="3">
-        <f>IF(B80="common", 4, IF(B80="uncommon", 3, IF(B80="rare", 1.22, 1)))</f>
+        <f>IF(B80="common", 4, IF(B80="uncommon", 3, IF(B80="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2562,13 +2581,13 @@
         <v>33</v>
       </c>
       <c r="D81" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E81" s="3" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="F81" s="3">
-        <f>IF(B81="common", 4, IF(B81="uncommon", 3, IF(B81="rare", 1.22, 1)))</f>
+        <f>IF(B81="common", 4, IF(B81="uncommon", 3, IF(B81="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2587,13 +2606,13 @@
         <v>46</v>
       </c>
       <c r="D82" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E82" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F82" s="3">
-        <f>IF(B82="common", 4, IF(B82="uncommon", 3, IF(B82="rare", 1.22, 1)))</f>
+        <f>IF(B82="common", 4, IF(B82="uncommon", 3, IF(B82="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2612,13 +2631,13 @@
         <v>46</v>
       </c>
       <c r="D83" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>0.22</v>
+        <v>0.14</v>
       </c>
       <c r="F83" s="3">
-        <f>IF(B83="common", 4, IF(B83="uncommon", 3, IF(B83="rare", 1.22, 1)))</f>
+        <f>IF(B83="common", 4, IF(B83="uncommon", 3, IF(B83="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2637,13 +2656,13 @@
         <v>21</v>
       </c>
       <c r="D84" s="3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="F84" s="3">
-        <f>IF(B84="common", 4, IF(B84="uncommon", 3, IF(B84="rare", 1.22, 1)))</f>
+        <f>IF(B84="common", 4, IF(B84="uncommon", 3, IF(B84="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2665,10 +2684,10 @@
         <v>0.1</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="F85" s="3">
-        <f>IF(B85="common", 4, IF(B85="uncommon", 3, IF(B85="rare", 1.22, 1)))</f>
+        <f>IF(B85="common", 4, IF(B85="uncommon", 3, IF(B85="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2687,13 +2706,13 @@
         <v>33</v>
       </c>
       <c r="D86" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>1.73</v>
+        <v>1.5</v>
       </c>
       <c r="F86" s="3">
-        <f>IF(B86="common", 4, IF(B86="uncommon", 3, IF(B86="rare", 1.22, 1)))</f>
+        <f>IF(B86="common", 4, IF(B86="uncommon", 3, IF(B86="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2715,10 +2734,10 @@
         <v>0.08</v>
       </c>
       <c r="E87" s="3" t="n">
-        <v>1.46</v>
+        <v>1.12</v>
       </c>
       <c r="F87" s="3">
-        <f>IF(B87="common", 4, IF(B87="uncommon", 3, IF(B87="rare", 1.22, 1)))</f>
+        <f>IF(B87="common", 4, IF(B87="uncommon", 3, IF(B87="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2737,13 +2756,13 @@
         <v>46</v>
       </c>
       <c r="D88" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E88" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F88" s="3">
-        <f>IF(B88="common", 4, IF(B88="uncommon", 3, IF(B88="rare", 1.22, 1)))</f>
+        <f>IF(B88="common", 4, IF(B88="uncommon", 3, IF(B88="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2762,13 +2781,13 @@
         <v>33</v>
       </c>
       <c r="D89" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>1.59</v>
+        <v>1.3</v>
       </c>
       <c r="F89" s="3">
-        <f>IF(B89="common", 4, IF(B89="uncommon", 3, IF(B89="rare", 1.22, 1)))</f>
+        <f>IF(B89="common", 4, IF(B89="uncommon", 3, IF(B89="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2787,13 +2806,13 @@
         <v>33</v>
       </c>
       <c r="D90" s="3" t="n">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
       <c r="F90" s="3">
-        <f>IF(B90="common", 4, IF(B90="uncommon", 3, IF(B90="rare", 1.22, 1)))</f>
+        <f>IF(B90="common", 4, IF(B90="uncommon", 3, IF(B90="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2812,11 +2831,11 @@
         <v>188</v>
       </c>
       <c r="D91" s="3" t="n">
-        <v>26.54</v>
+        <v>26.26</v>
       </c>
       <c r="E91" s="3" t="inlineStr"/>
       <c r="F91" s="3">
-        <f>IF(B91="common", 4, IF(B91="uncommon", 3, IF(B91="rare", 1.22, 1)))</f>
+        <f>IF(B91="common", 4, IF(B91="uncommon", 3, IF(B91="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2835,13 +2854,13 @@
         <v>46</v>
       </c>
       <c r="D92" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E92" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F92" s="3">
-        <f>IF(B92="common", 4, IF(B92="uncommon", 3, IF(B92="rare", 1.22, 1)))</f>
+        <f>IF(B92="common", 4, IF(B92="uncommon", 3, IF(B92="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2860,13 +2879,13 @@
         <v>21</v>
       </c>
       <c r="D93" s="3" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="E93" s="3" t="n">
-        <v>1.66</v>
+        <v>2.24</v>
       </c>
       <c r="F93" s="3">
-        <f>IF(B93="common", 4, IF(B93="uncommon", 3, IF(B93="rare", 1.22, 1)))</f>
+        <f>IF(B93="common", 4, IF(B93="uncommon", 3, IF(B93="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2885,11 +2904,11 @@
         <v>90</v>
       </c>
       <c r="D94" s="3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E94" s="3" t="inlineStr"/>
       <c r="F94" s="3">
-        <f>IF(B94="common", 4, IF(B94="uncommon", 3, IF(B94="rare", 1.22, 1)))</f>
+        <f>IF(B94="common", 4, IF(B94="uncommon", 3, IF(B94="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2908,11 +2927,11 @@
         <v>248</v>
       </c>
       <c r="D95" s="3" t="n">
-        <v>4.76</v>
+        <v>5.3</v>
       </c>
       <c r="E95" s="3" t="inlineStr"/>
       <c r="F95" s="3">
-        <f>IF(B95="common", 4, IF(B95="uncommon", 3, IF(B95="rare", 1.22, 1)))</f>
+        <f>IF(B95="common", 4, IF(B95="uncommon", 3, IF(B95="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2931,13 +2950,13 @@
         <v>33</v>
       </c>
       <c r="D96" s="3" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="E96" s="3" t="n">
-        <v>1.37</v>
+        <v>1.12</v>
       </c>
       <c r="F96" s="3">
-        <f>IF(B96="common", 4, IF(B96="uncommon", 3, IF(B96="rare", 1.22, 1)))</f>
+        <f>IF(B96="common", 4, IF(B96="uncommon", 3, IF(B96="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2959,10 +2978,10 @@
         <v>0.13</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>0.87</v>
+        <v>0.89</v>
       </c>
       <c r="F97" s="3">
-        <f>IF(B97="common", 4, IF(B97="uncommon", 3, IF(B97="rare", 1.22, 1)))</f>
+        <f>IF(B97="common", 4, IF(B97="uncommon", 3, IF(B97="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -2981,13 +3000,13 @@
         <v>33</v>
       </c>
       <c r="D98" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E98" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="F98" s="3">
-        <f>IF(B98="common", 4, IF(B98="uncommon", 3, IF(B98="rare", 1.22, 1)))</f>
+        <f>IF(B98="common", 4, IF(B98="uncommon", 3, IF(B98="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3006,13 +3025,13 @@
         <v>46</v>
       </c>
       <c r="D99" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E99" s="3" t="n">
-        <v>2.13</v>
+        <v>2.01</v>
       </c>
       <c r="F99" s="3">
-        <f>IF(B99="common", 4, IF(B99="uncommon", 3, IF(B99="rare", 1.22, 1)))</f>
+        <f>IF(B99="common", 4, IF(B99="uncommon", 3, IF(B99="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3031,11 +3050,11 @@
         <v>90</v>
       </c>
       <c r="D100" s="3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="E100" s="3" t="inlineStr"/>
       <c r="F100" s="3">
-        <f>IF(B100="common", 4, IF(B100="uncommon", 3, IF(B100="rare", 1.22, 1)))</f>
+        <f>IF(B100="common", 4, IF(B100="uncommon", 3, IF(B100="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3054,11 +3073,11 @@
         <v>248</v>
       </c>
       <c r="D101" s="3" t="n">
-        <v>5.53</v>
+        <v>5.8</v>
       </c>
       <c r="E101" s="3" t="inlineStr"/>
       <c r="F101" s="3">
-        <f>IF(B101="common", 4, IF(B101="uncommon", 3, IF(B101="rare", 1.22, 1)))</f>
+        <f>IF(B101="common", 4, IF(B101="uncommon", 3, IF(B101="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3077,13 +3096,13 @@
         <v>33</v>
       </c>
       <c r="D102" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E102" s="3" t="n">
-        <v>1.47</v>
+        <v>1.26</v>
       </c>
       <c r="F102" s="3">
-        <f>IF(B102="common", 4, IF(B102="uncommon", 3, IF(B102="rare", 1.22, 1)))</f>
+        <f>IF(B102="common", 4, IF(B102="uncommon", 3, IF(B102="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3105,10 +3124,10 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E103" s="3" t="n">
-        <v>0.18</v>
+        <v>0.14</v>
       </c>
       <c r="F103" s="3">
-        <f>IF(B103="common", 4, IF(B103="uncommon", 3, IF(B103="rare", 1.22, 1)))</f>
+        <f>IF(B103="common", 4, IF(B103="uncommon", 3, IF(B103="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3127,13 +3146,13 @@
         <v>46</v>
       </c>
       <c r="D104" s="3" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="E104" s="3" t="n">
-        <v>0.13</v>
+        <v>0.17</v>
       </c>
       <c r="F104" s="3">
-        <f>IF(B104="common", 4, IF(B104="uncommon", 3, IF(B104="rare", 1.22, 1)))</f>
+        <f>IF(B104="common", 4, IF(B104="uncommon", 3, IF(B104="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3155,10 +3174,10 @@
         <v>0.08</v>
       </c>
       <c r="E105" s="3" t="n">
-        <v>1.51</v>
+        <v>1.65</v>
       </c>
       <c r="F105" s="3">
-        <f>IF(B105="common", 4, IF(B105="uncommon", 3, IF(B105="rare", 1.22, 1)))</f>
+        <f>IF(B105="common", 4, IF(B105="uncommon", 3, IF(B105="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3177,13 +3196,13 @@
         <v>33</v>
       </c>
       <c r="D106" s="3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="E106" s="3" t="n">
-        <v>0.57</v>
+        <v>0.52</v>
       </c>
       <c r="F106" s="3">
-        <f>IF(B106="common", 4, IF(B106="uncommon", 3, IF(B106="rare", 1.22, 1)))</f>
+        <f>IF(B106="common", 4, IF(B106="uncommon", 3, IF(B106="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3202,13 +3221,13 @@
         <v>46</v>
       </c>
       <c r="D107" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E107" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F107" s="3">
-        <f>IF(B107="common", 4, IF(B107="uncommon", 3, IF(B107="rare", 1.22, 1)))</f>
+        <f>IF(B107="common", 4, IF(B107="uncommon", 3, IF(B107="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3227,13 +3246,13 @@
         <v>21</v>
       </c>
       <c r="D108" s="3" t="n">
-        <v>0.14</v>
+        <v>0.17</v>
       </c>
       <c r="E108" s="3" t="n">
-        <v>0.58</v>
+        <v>0.66</v>
       </c>
       <c r="F108" s="3">
-        <f>IF(B108="common", 4, IF(B108="uncommon", 3, IF(B108="rare", 1.22, 1)))</f>
+        <f>IF(B108="common", 4, IF(B108="uncommon", 3, IF(B108="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3252,13 +3271,13 @@
         <v>33</v>
       </c>
       <c r="D109" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E109" s="3" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="F109" s="3">
-        <f>IF(B109="common", 4, IF(B109="uncommon", 3, IF(B109="rare", 1.22, 1)))</f>
+        <f>IF(B109="common", 4, IF(B109="uncommon", 3, IF(B109="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3277,11 +3296,11 @@
         <v>188</v>
       </c>
       <c r="D110" s="3" t="n">
-        <v>10.04</v>
+        <v>11.24</v>
       </c>
       <c r="E110" s="3" t="inlineStr"/>
       <c r="F110" s="3">
-        <f>IF(B110="common", 4, IF(B110="uncommon", 3, IF(B110="rare", 1.22, 1)))</f>
+        <f>IF(B110="common", 4, IF(B110="uncommon", 3, IF(B110="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3303,10 +3322,10 @@
         <v>0.06</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="F111" s="3">
-        <f>IF(B111="common", 4, IF(B111="uncommon", 3, IF(B111="rare", 1.22, 1)))</f>
+        <f>IF(B111="common", 4, IF(B111="uncommon", 3, IF(B111="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3325,13 +3344,13 @@
         <v>46</v>
       </c>
       <c r="D112" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E112" s="3" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="F112" s="3">
-        <f>IF(B112="common", 4, IF(B112="uncommon", 3, IF(B112="rare", 1.22, 1)))</f>
+        <f>IF(B112="common", 4, IF(B112="uncommon", 3, IF(B112="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3350,13 +3369,13 @@
         <v>46</v>
       </c>
       <c r="D113" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E113" s="3" t="n">
-        <v>1.26</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F113" s="3">
-        <f>IF(B113="common", 4, IF(B113="uncommon", 3, IF(B113="rare", 1.22, 1)))</f>
+        <f>IF(B113="common", 4, IF(B113="uncommon", 3, IF(B113="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3375,13 +3394,13 @@
         <v>46</v>
       </c>
       <c r="D114" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E114" s="3" t="n">
         <v>0.15</v>
       </c>
       <c r="F114" s="3">
-        <f>IF(B114="common", 4, IF(B114="uncommon", 3, IF(B114="rare", 1.22, 1)))</f>
+        <f>IF(B114="common", 4, IF(B114="uncommon", 3, IF(B114="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3400,13 +3419,13 @@
         <v>33</v>
       </c>
       <c r="D115" s="3" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="E115" s="3" t="n">
-        <v>0.17</v>
+        <v>0.13</v>
       </c>
       <c r="F115" s="3">
-        <f>IF(B115="common", 4, IF(B115="uncommon", 3, IF(B115="rare", 1.22, 1)))</f>
+        <f>IF(B115="common", 4, IF(B115="uncommon", 3, IF(B115="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3425,13 +3444,13 @@
         <v>46</v>
       </c>
       <c r="D116" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E116" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F116" s="3">
-        <f>IF(B116="common", 4, IF(B116="uncommon", 3, IF(B116="rare", 1.22, 1)))</f>
+        <f>IF(B116="common", 4, IF(B116="uncommon", 3, IF(B116="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3450,13 +3469,13 @@
         <v>21</v>
       </c>
       <c r="D117" s="3" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="E117" s="3" t="n">
-        <v>0.71</v>
+        <v>0.54</v>
       </c>
       <c r="F117" s="3">
-        <f>IF(B117="common", 4, IF(B117="uncommon", 3, IF(B117="rare", 1.22, 1)))</f>
+        <f>IF(B117="common", 4, IF(B117="uncommon", 3, IF(B117="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3475,13 +3494,13 @@
         <v>46</v>
       </c>
       <c r="D118" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E118" s="3" t="n">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="F118" s="3">
-        <f>IF(B118="common", 4, IF(B118="uncommon", 3, IF(B118="rare", 1.22, 1)))</f>
+        <f>IF(B118="common", 4, IF(B118="uncommon", 3, IF(B118="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3500,13 +3519,13 @@
         <v>46</v>
       </c>
       <c r="D119" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>2.15</v>
+        <v>2.22</v>
       </c>
       <c r="F119" s="3">
-        <f>IF(B119="common", 4, IF(B119="uncommon", 3, IF(B119="rare", 1.22, 1)))</f>
+        <f>IF(B119="common", 4, IF(B119="uncommon", 3, IF(B119="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3525,11 +3544,11 @@
         <v>90</v>
       </c>
       <c r="D120" s="3" t="n">
-        <v>6.89</v>
+        <v>7.21</v>
       </c>
       <c r="E120" s="3" t="inlineStr"/>
       <c r="F120" s="3">
-        <f>IF(B120="common", 4, IF(B120="uncommon", 3, IF(B120="rare", 1.22, 1)))</f>
+        <f>IF(B120="common", 4, IF(B120="uncommon", 3, IF(B120="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3548,11 +3567,11 @@
         <v>248</v>
       </c>
       <c r="D121" s="3" t="n">
-        <v>18.01</v>
+        <v>19.11</v>
       </c>
       <c r="E121" s="3" t="inlineStr"/>
       <c r="F121" s="3">
-        <f>IF(B121="common", 4, IF(B121="uncommon", 3, IF(B121="rare", 1.22, 1)))</f>
+        <f>IF(B121="common", 4, IF(B121="uncommon", 3, IF(B121="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3571,11 +3590,11 @@
         <v>154</v>
       </c>
       <c r="D122" s="3" t="n">
-        <v>13.15</v>
+        <v>13.27</v>
       </c>
       <c r="E122" s="3" t="inlineStr"/>
       <c r="F122" s="3">
-        <f>IF(B122="common", 4, IF(B122="uncommon", 3, IF(B122="rare", 1.22, 1)))</f>
+        <f>IF(B122="common", 4, IF(B122="uncommon", 3, IF(B122="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3594,11 +3613,11 @@
         <v>90</v>
       </c>
       <c r="D123" s="3" t="n">
-        <v>9.84</v>
+        <v>9.75</v>
       </c>
       <c r="E123" s="3" t="inlineStr"/>
       <c r="F123" s="3">
-        <f>IF(B123="common", 4, IF(B123="uncommon", 3, IF(B123="rare", 1.22, 1)))</f>
+        <f>IF(B123="common", 4, IF(B123="uncommon", 3, IF(B123="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3617,13 +3636,13 @@
         <v>21</v>
       </c>
       <c r="D124" s="3" t="n">
-        <v>0.54</v>
+        <v>0.51</v>
       </c>
       <c r="E124" s="3" t="n">
-        <v>1.62</v>
+        <v>1.58</v>
       </c>
       <c r="F124" s="3">
-        <f>IF(B124="common", 4, IF(B124="uncommon", 3, IF(B124="rare", 1.22, 1)))</f>
+        <f>IF(B124="common", 4, IF(B124="uncommon", 3, IF(B124="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3642,13 +3661,13 @@
         <v>21</v>
       </c>
       <c r="D125" s="3" t="n">
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="E125" s="3" t="n">
-        <v>1.01</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F125" s="3">
-        <f>IF(B125="common", 4, IF(B125="uncommon", 3, IF(B125="rare", 1.22, 1)))</f>
+        <f>IF(B125="common", 4, IF(B125="uncommon", 3, IF(B125="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3667,13 +3686,13 @@
         <v>21</v>
       </c>
       <c r="D126" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="E126" s="3" t="n">
-        <v>0.54</v>
+        <v>0.51</v>
       </c>
       <c r="F126" s="3">
-        <f>IF(B126="common", 4, IF(B126="uncommon", 3, IF(B126="rare", 1.22, 1)))</f>
+        <f>IF(B126="common", 4, IF(B126="uncommon", 3, IF(B126="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3692,11 +3711,11 @@
         <v>188</v>
       </c>
       <c r="D127" s="3" t="n">
-        <v>6.68</v>
+        <v>5.79</v>
       </c>
       <c r="E127" s="3" t="inlineStr"/>
       <c r="F127" s="3">
-        <f>IF(B127="common", 4, IF(B127="uncommon", 3, IF(B127="rare", 1.22, 1)))</f>
+        <f>IF(B127="common", 4, IF(B127="uncommon", 3, IF(B127="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3715,13 +3734,13 @@
         <v>33</v>
       </c>
       <c r="D128" s="3" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="E128" s="3" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
       <c r="F128" s="3">
-        <f>IF(B128="common", 4, IF(B128="uncommon", 3, IF(B128="rare", 1.22, 1)))</f>
+        <f>IF(B128="common", 4, IF(B128="uncommon", 3, IF(B128="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3740,13 +3759,13 @@
         <v>21</v>
       </c>
       <c r="D129" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="E129" s="3" t="n">
-        <v>0.92</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F129" s="3">
-        <f>IF(B129="common", 4, IF(B129="uncommon", 3, IF(B129="rare", 1.22, 1)))</f>
+        <f>IF(B129="common", 4, IF(B129="uncommon", 3, IF(B129="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3765,11 +3784,11 @@
         <v>188</v>
       </c>
       <c r="D130" s="3" t="n">
-        <v>10.45</v>
+        <v>9.58</v>
       </c>
       <c r="E130" s="3" t="inlineStr"/>
       <c r="F130" s="3">
-        <f>IF(B130="common", 4, IF(B130="uncommon", 3, IF(B130="rare", 1.22, 1)))</f>
+        <f>IF(B130="common", 4, IF(B130="uncommon", 3, IF(B130="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3788,13 +3807,13 @@
         <v>33</v>
       </c>
       <c r="D131" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E131" s="3" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="F131" s="3">
-        <f>IF(B131="common", 4, IF(B131="uncommon", 3, IF(B131="rare", 1.22, 1)))</f>
+        <f>IF(B131="common", 4, IF(B131="uncommon", 3, IF(B131="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3813,13 +3832,13 @@
         <v>46</v>
       </c>
       <c r="D132" s="3" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="E132" s="3" t="n">
-        <v>1.95</v>
+        <v>1.98</v>
       </c>
       <c r="F132" s="3">
-        <f>IF(B132="common", 4, IF(B132="uncommon", 3, IF(B132="rare", 1.22, 1)))</f>
+        <f>IF(B132="common", 4, IF(B132="uncommon", 3, IF(B132="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3838,13 +3857,13 @@
         <v>46</v>
       </c>
       <c r="D133" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="E133" s="3" t="n">
-        <v>2.12</v>
+        <v>1.56</v>
       </c>
       <c r="F133" s="3">
-        <f>IF(B133="common", 4, IF(B133="uncommon", 3, IF(B133="rare", 1.22, 1)))</f>
+        <f>IF(B133="common", 4, IF(B133="uncommon", 3, IF(B133="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3866,10 +3885,10 @@
         <v>0.08</v>
       </c>
       <c r="E134" s="3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="F134" s="3">
-        <f>IF(B134="common", 4, IF(B134="uncommon", 3, IF(B134="rare", 1.22, 1)))</f>
+        <f>IF(B134="common", 4, IF(B134="uncommon", 3, IF(B134="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3888,13 +3907,13 @@
         <v>33</v>
       </c>
       <c r="D135" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E135" s="3" t="n">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="F135" s="3">
-        <f>IF(B135="common", 4, IF(B135="uncommon", 3, IF(B135="rare", 1.22, 1)))</f>
+        <f>IF(B135="common", 4, IF(B135="uncommon", 3, IF(B135="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3913,11 +3932,11 @@
         <v>90</v>
       </c>
       <c r="D136" s="3" t="n">
-        <v>0.59</v>
+        <v>0.83</v>
       </c>
       <c r="E136" s="3" t="inlineStr"/>
       <c r="F136" s="3">
-        <f>IF(B136="common", 4, IF(B136="uncommon", 3, IF(B136="rare", 1.22, 1)))</f>
+        <f>IF(B136="common", 4, IF(B136="uncommon", 3, IF(B136="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3936,11 +3955,11 @@
         <v>248</v>
       </c>
       <c r="D137" s="3" t="n">
-        <v>9.24</v>
+        <v>7.87</v>
       </c>
       <c r="E137" s="3" t="inlineStr"/>
       <c r="F137" s="3">
-        <f>IF(B137="common", 4, IF(B137="uncommon", 3, IF(B137="rare", 1.22, 1)))</f>
+        <f>IF(B137="common", 4, IF(B137="uncommon", 3, IF(B137="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3959,13 +3978,13 @@
         <v>46</v>
       </c>
       <c r="D138" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E138" s="3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="F138" s="3">
-        <f>IF(B138="common", 4, IF(B138="uncommon", 3, IF(B138="rare", 1.22, 1)))</f>
+        <f>IF(B138="common", 4, IF(B138="uncommon", 3, IF(B138="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -3984,13 +4003,13 @@
         <v>33</v>
       </c>
       <c r="D139" s="3" t="n">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>2.34</v>
+        <v>2.36</v>
       </c>
       <c r="F139" s="3">
-        <f>IF(B139="common", 4, IF(B139="uncommon", 3, IF(B139="rare", 1.22, 1)))</f>
+        <f>IF(B139="common", 4, IF(B139="uncommon", 3, IF(B139="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4009,11 +4028,11 @@
         <v>188</v>
       </c>
       <c r="D140" s="3" t="n">
-        <v>7.26</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="inlineStr"/>
       <c r="F140" s="3">
-        <f>IF(B140="common", 4, IF(B140="uncommon", 3, IF(B140="rare", 1.22, 1)))</f>
+        <f>IF(B140="common", 4, IF(B140="uncommon", 3, IF(B140="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4032,13 +4051,13 @@
         <v>21</v>
       </c>
       <c r="D141" s="3" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="E141" s="3" t="n">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
       <c r="F141" s="3">
-        <f>IF(B141="common", 4, IF(B141="uncommon", 3, IF(B141="rare", 1.22, 1)))</f>
+        <f>IF(B141="common", 4, IF(B141="uncommon", 3, IF(B141="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4057,13 +4076,13 @@
         <v>33</v>
       </c>
       <c r="D142" s="3" t="n">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E142" s="3" t="n">
-        <v>1.28</v>
+        <v>1.36</v>
       </c>
       <c r="F142" s="3">
-        <f>IF(B142="common", 4, IF(B142="uncommon", 3, IF(B142="rare", 1.22, 1)))</f>
+        <f>IF(B142="common", 4, IF(B142="uncommon", 3, IF(B142="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4082,13 +4101,13 @@
         <v>46</v>
       </c>
       <c r="D143" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E143" s="3" t="n">
         <v>0.16</v>
       </c>
       <c r="F143" s="3">
-        <f>IF(B143="common", 4, IF(B143="uncommon", 3, IF(B143="rare", 1.22, 1)))</f>
+        <f>IF(B143="common", 4, IF(B143="uncommon", 3, IF(B143="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4107,13 +4126,13 @@
         <v>33</v>
       </c>
       <c r="D144" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E144" s="3" t="n">
-        <v>0.13</v>
+        <v>0.19</v>
       </c>
       <c r="F144" s="3">
-        <f>IF(B144="common", 4, IF(B144="uncommon", 3, IF(B144="rare", 1.22, 1)))</f>
+        <f>IF(B144="common", 4, IF(B144="uncommon", 3, IF(B144="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4132,13 +4151,13 @@
         <v>33</v>
       </c>
       <c r="D145" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>0.13</v>
+        <v>0.21</v>
       </c>
       <c r="F145" s="3">
-        <f>IF(B145="common", 4, IF(B145="uncommon", 3, IF(B145="rare", 1.22, 1)))</f>
+        <f>IF(B145="common", 4, IF(B145="uncommon", 3, IF(B145="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4157,13 +4176,13 @@
         <v>33</v>
       </c>
       <c r="D146" s="3" t="n">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="E146" s="3" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="F146" s="3">
-        <f>IF(B146="common", 4, IF(B146="uncommon", 3, IF(B146="rare", 1.22, 1)))</f>
+        <f>IF(B146="common", 4, IF(B146="uncommon", 3, IF(B146="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4182,13 +4201,13 @@
         <v>46</v>
       </c>
       <c r="D147" s="3" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>3.16</v>
+        <v>2.19</v>
       </c>
       <c r="F147" s="3">
-        <f>IF(B147="common", 4, IF(B147="uncommon", 3, IF(B147="rare", 1.22, 1)))</f>
+        <f>IF(B147="common", 4, IF(B147="uncommon", 3, IF(B147="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4207,13 +4226,13 @@
         <v>46</v>
       </c>
       <c r="D148" s="3" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="E148" s="3" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="F148" s="3">
-        <f>IF(B148="common", 4, IF(B148="uncommon", 3, IF(B148="rare", 1.22, 1)))</f>
+        <f>IF(B148="common", 4, IF(B148="uncommon", 3, IF(B148="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4235,10 +4254,10 @@
         <v>0.1</v>
       </c>
       <c r="E149" s="3" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="F149" s="3">
-        <f>IF(B149="common", 4, IF(B149="uncommon", 3, IF(B149="rare", 1.22, 1)))</f>
+        <f>IF(B149="common", 4, IF(B149="uncommon", 3, IF(B149="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4257,11 +4276,11 @@
         <v>188</v>
       </c>
       <c r="D150" s="3" t="n">
-        <v>28.19</v>
+        <v>28.89</v>
       </c>
       <c r="E150" s="3" t="inlineStr"/>
       <c r="F150" s="3">
-        <f>IF(B150="common", 4, IF(B150="uncommon", 3, IF(B150="rare", 1.22, 1)))</f>
+        <f>IF(B150="common", 4, IF(B150="uncommon", 3, IF(B150="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4280,13 +4299,13 @@
         <v>33</v>
       </c>
       <c r="D151" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>1.36</v>
+        <v>1.65</v>
       </c>
       <c r="F151" s="3">
-        <f>IF(B151="common", 4, IF(B151="uncommon", 3, IF(B151="rare", 1.22, 1)))</f>
+        <f>IF(B151="common", 4, IF(B151="uncommon", 3, IF(B151="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4308,10 +4327,10 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E152" s="3" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="F152" s="3">
-        <f>IF(B152="common", 4, IF(B152="uncommon", 3, IF(B152="rare", 1.22, 1)))</f>
+        <f>IF(B152="common", 4, IF(B152="uncommon", 3, IF(B152="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4333,10 +4352,10 @@
         <v>0.1</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>1.44</v>
+        <v>1.14</v>
       </c>
       <c r="F153" s="3">
-        <f>IF(B153="common", 4, IF(B153="uncommon", 3, IF(B153="rare", 1.22, 1)))</f>
+        <f>IF(B153="common", 4, IF(B153="uncommon", 3, IF(B153="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4355,11 +4374,11 @@
         <v>188</v>
       </c>
       <c r="D154" s="3" t="n">
-        <v>15.76</v>
+        <v>18.96</v>
       </c>
       <c r="E154" s="3" t="inlineStr"/>
       <c r="F154" s="3">
-        <f>IF(B154="common", 4, IF(B154="uncommon", 3, IF(B154="rare", 1.22, 1)))</f>
+        <f>IF(B154="common", 4, IF(B154="uncommon", 3, IF(B154="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4378,13 +4397,13 @@
         <v>33</v>
       </c>
       <c r="D155" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E155" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F155" s="3">
-        <f>IF(B155="common", 4, IF(B155="uncommon", 3, IF(B155="rare", 1.22, 1)))</f>
+        <f>IF(B155="common", 4, IF(B155="uncommon", 3, IF(B155="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4403,13 +4422,13 @@
         <v>46</v>
       </c>
       <c r="D156" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E156" s="3" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="F156" s="3">
-        <f>IF(B156="common", 4, IF(B156="uncommon", 3, IF(B156="rare", 1.22, 1)))</f>
+        <f>IF(B156="common", 4, IF(B156="uncommon", 3, IF(B156="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4428,13 +4447,13 @@
         <v>46</v>
       </c>
       <c r="D157" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E157" s="3" t="n">
-        <v>0.14</v>
+        <v>0.17</v>
       </c>
       <c r="F157" s="3">
-        <f>IF(B157="common", 4, IF(B157="uncommon", 3, IF(B157="rare", 1.22, 1)))</f>
+        <f>IF(B157="common", 4, IF(B157="uncommon", 3, IF(B157="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4453,13 +4472,13 @@
         <v>33</v>
       </c>
       <c r="D158" s="3" t="n">
-        <v>0.05</v>
+        <v>0.09</v>
       </c>
       <c r="E158" s="3" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="F158" s="3">
-        <f>IF(B158="common", 4, IF(B158="uncommon", 3, IF(B158="rare", 1.22, 1)))</f>
+        <f>IF(B158="common", 4, IF(B158="uncommon", 3, IF(B158="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4478,13 +4497,13 @@
         <v>33</v>
       </c>
       <c r="D159" s="3" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="F159" s="3">
-        <f>IF(B159="common", 4, IF(B159="uncommon", 3, IF(B159="rare", 1.22, 1)))</f>
+        <f>IF(B159="common", 4, IF(B159="uncommon", 3, IF(B159="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4503,13 +4522,13 @@
         <v>46</v>
       </c>
       <c r="D160" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E160" s="3" t="n">
-        <v>0.34</v>
+        <v>0.22</v>
       </c>
       <c r="F160" s="3">
-        <f>IF(B160="common", 4, IF(B160="uncommon", 3, IF(B160="rare", 1.22, 1)))</f>
+        <f>IF(B160="common", 4, IF(B160="uncommon", 3, IF(B160="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4528,11 +4547,11 @@
         <v>188</v>
       </c>
       <c r="D161" s="3" t="n">
-        <v>20.61</v>
+        <v>21.1</v>
       </c>
       <c r="E161" s="3" t="inlineStr"/>
       <c r="F161" s="3">
-        <f>IF(B161="common", 4, IF(B161="uncommon", 3, IF(B161="rare", 1.22, 1)))</f>
+        <f>IF(B161="common", 4, IF(B161="uncommon", 3, IF(B161="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4554,10 +4573,10 @@
         <v>0.14</v>
       </c>
       <c r="E162" s="3" t="n">
-        <v>0.95</v>
+        <v>0.86</v>
       </c>
       <c r="F162" s="3">
-        <f>IF(B162="common", 4, IF(B162="uncommon", 3, IF(B162="rare", 1.22, 1)))</f>
+        <f>IF(B162="common", 4, IF(B162="uncommon", 3, IF(B162="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4579,10 +4598,10 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F163" s="3">
-        <f>IF(B163="common", 4, IF(B163="uncommon", 3, IF(B163="rare", 1.22, 1)))</f>
+        <f>IF(B163="common", 4, IF(B163="uncommon", 3, IF(B163="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4601,13 +4620,13 @@
         <v>33</v>
       </c>
       <c r="D164" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E164" s="3" t="n">
         <v>0.17</v>
       </c>
       <c r="F164" s="3">
-        <f>IF(B164="common", 4, IF(B164="uncommon", 3, IF(B164="rare", 1.22, 1)))</f>
+        <f>IF(B164="common", 4, IF(B164="uncommon", 3, IF(B164="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4629,10 +4648,10 @@
         <v>0.06</v>
       </c>
       <c r="E165" s="3" t="n">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
       <c r="F165" s="3">
-        <f>IF(B165="common", 4, IF(B165="uncommon", 3, IF(B165="rare", 1.22, 1)))</f>
+        <f>IF(B165="common", 4, IF(B165="uncommon", 3, IF(B165="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4651,13 +4670,13 @@
         <v>33</v>
       </c>
       <c r="D166" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E166" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F166" s="3">
-        <f>IF(B166="common", 4, IF(B166="uncommon", 3, IF(B166="rare", 1.22, 1)))</f>
+        <f>IF(B166="common", 4, IF(B166="uncommon", 3, IF(B166="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4676,13 +4695,13 @@
         <v>46</v>
       </c>
       <c r="D167" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E167" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F167" s="3">
-        <f>IF(B167="common", 4, IF(B167="uncommon", 3, IF(B167="rare", 1.22, 1)))</f>
+        <f>IF(B167="common", 4, IF(B167="uncommon", 3, IF(B167="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4701,13 +4720,13 @@
         <v>33</v>
       </c>
       <c r="D168" s="3" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="E168" s="3" t="n">
-        <v>1.43</v>
+        <v>1.08</v>
       </c>
       <c r="F168" s="3">
-        <f>IF(B168="common", 4, IF(B168="uncommon", 3, IF(B168="rare", 1.22, 1)))</f>
+        <f>IF(B168="common", 4, IF(B168="uncommon", 3, IF(B168="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4726,13 +4745,13 @@
         <v>46</v>
       </c>
       <c r="D169" s="3" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="E169" s="3" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="F169" s="3">
-        <f>IF(B169="common", 4, IF(B169="uncommon", 3, IF(B169="rare", 1.22, 1)))</f>
+        <f>IF(B169="common", 4, IF(B169="uncommon", 3, IF(B169="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4751,13 +4770,13 @@
         <v>33</v>
       </c>
       <c r="D170" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E170" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F170" s="3">
-        <f>IF(B170="common", 4, IF(B170="uncommon", 3, IF(B170="rare", 1.22, 1)))</f>
+        <f>IF(B170="common", 4, IF(B170="uncommon", 3, IF(B170="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4776,13 +4795,13 @@
         <v>33</v>
       </c>
       <c r="D171" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>2.57</v>
+        <v>2.4</v>
       </c>
       <c r="F171" s="3">
-        <f>IF(B171="common", 4, IF(B171="uncommon", 3, IF(B171="rare", 1.22, 1)))</f>
+        <f>IF(B171="common", 4, IF(B171="uncommon", 3, IF(B171="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4801,13 +4820,13 @@
         <v>33</v>
       </c>
       <c r="D172" s="3" t="n">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E172" s="3" t="n">
         <v>0.14</v>
       </c>
       <c r="F172" s="3">
-        <f>IF(B172="common", 4, IF(B172="uncommon", 3, IF(B172="rare", 1.22, 1)))</f>
+        <f>IF(B172="common", 4, IF(B172="uncommon", 3, IF(B172="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4826,13 +4845,13 @@
         <v>33</v>
       </c>
       <c r="D173" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>1.02</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F173" s="3">
-        <f>IF(B173="common", 4, IF(B173="uncommon", 3, IF(B173="rare", 1.22, 1)))</f>
+        <f>IF(B173="common", 4, IF(B173="uncommon", 3, IF(B173="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4854,10 +4873,10 @@
         <v>0.08</v>
       </c>
       <c r="E174" s="3" t="n">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="F174" s="3">
-        <f>IF(B174="common", 4, IF(B174="uncommon", 3, IF(B174="rare", 1.22, 1)))</f>
+        <f>IF(B174="common", 4, IF(B174="uncommon", 3, IF(B174="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4879,10 +4898,10 @@
         <v>0.06</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F175" s="3">
-        <f>IF(B175="common", 4, IF(B175="uncommon", 3, IF(B175="rare", 1.22, 1)))</f>
+        <f>IF(B175="common", 4, IF(B175="uncommon", 3, IF(B175="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4901,13 +4920,13 @@
         <v>33</v>
       </c>
       <c r="D176" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E176" s="3" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="F176" s="3">
-        <f>IF(B176="common", 4, IF(B176="uncommon", 3, IF(B176="rare", 1.22, 1)))</f>
+        <f>IF(B176="common", 4, IF(B176="uncommon", 3, IF(B176="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4926,13 +4945,13 @@
         <v>46</v>
       </c>
       <c r="D177" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="F177" s="3">
-        <f>IF(B177="common", 4, IF(B177="uncommon", 3, IF(B177="rare", 1.22, 1)))</f>
+        <f>IF(B177="common", 4, IF(B177="uncommon", 3, IF(B177="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4951,13 +4970,13 @@
         <v>33</v>
       </c>
       <c r="D178" s="3" t="n">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
       <c r="E178" s="3" t="n">
-        <v>1.96</v>
+        <v>1.27</v>
       </c>
       <c r="F178" s="3">
-        <f>IF(B178="common", 4, IF(B178="uncommon", 3, IF(B178="rare", 1.22, 1)))</f>
+        <f>IF(B178="common", 4, IF(B178="uncommon", 3, IF(B178="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -4976,13 +4995,13 @@
         <v>46</v>
       </c>
       <c r="D179" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="F179" s="3">
-        <f>IF(B179="common", 4, IF(B179="uncommon", 3, IF(B179="rare", 1.22, 1)))</f>
+        <f>IF(B179="common", 4, IF(B179="uncommon", 3, IF(B179="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5001,13 +5020,13 @@
         <v>46</v>
       </c>
       <c r="D180" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E180" s="3" t="n">
-        <v>0.16</v>
+        <v>0.23</v>
       </c>
       <c r="F180" s="3">
-        <f>IF(B180="common", 4, IF(B180="uncommon", 3, IF(B180="rare", 1.22, 1)))</f>
+        <f>IF(B180="common", 4, IF(B180="uncommon", 3, IF(B180="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5026,11 +5045,11 @@
         <v>188</v>
       </c>
       <c r="D181" s="3" t="n">
-        <v>45.51</v>
+        <v>46.05</v>
       </c>
       <c r="E181" s="3" t="inlineStr"/>
       <c r="F181" s="3">
-        <f>IF(B181="common", 4, IF(B181="uncommon", 3, IF(B181="rare", 1.22, 1)))</f>
+        <f>IF(B181="common", 4, IF(B181="uncommon", 3, IF(B181="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5049,13 +5068,13 @@
         <v>21</v>
       </c>
       <c r="D182" s="3" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="E182" s="3" t="n">
-        <v>0.75</v>
+        <v>0.64</v>
       </c>
       <c r="F182" s="3">
-        <f>IF(B182="common", 4, IF(B182="uncommon", 3, IF(B182="rare", 1.22, 1)))</f>
+        <f>IF(B182="common", 4, IF(B182="uncommon", 3, IF(B182="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5074,13 +5093,13 @@
         <v>46</v>
       </c>
       <c r="D183" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E183" s="3" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="F183" s="3">
-        <f>IF(B183="common", 4, IF(B183="uncommon", 3, IF(B183="rare", 1.22, 1)))</f>
+        <f>IF(B183="common", 4, IF(B183="uncommon", 3, IF(B183="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5099,11 +5118,11 @@
         <v>154</v>
       </c>
       <c r="D184" s="3" t="n">
-        <v>2.38</v>
+        <v>2.56</v>
       </c>
       <c r="E184" s="3" t="inlineStr"/>
       <c r="F184" s="3">
-        <f>IF(B184="common", 4, IF(B184="uncommon", 3, IF(B184="rare", 1.22, 1)))</f>
+        <f>IF(B184="common", 4, IF(B184="uncommon", 3, IF(B184="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5122,13 +5141,13 @@
         <v>46</v>
       </c>
       <c r="D185" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E185" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F185" s="3">
-        <f>IF(B185="common", 4, IF(B185="uncommon", 3, IF(B185="rare", 1.22, 1)))</f>
+        <f>IF(B185="common", 4, IF(B185="uncommon", 3, IF(B185="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5147,11 +5166,11 @@
         <v>188</v>
       </c>
       <c r="D186" s="3" t="n">
-        <v>7.57</v>
+        <v>7.68</v>
       </c>
       <c r="E186" s="3" t="inlineStr"/>
       <c r="F186" s="3">
-        <f>IF(B186="common", 4, IF(B186="uncommon", 3, IF(B186="rare", 1.22, 1)))</f>
+        <f>IF(B186="common", 4, IF(B186="uncommon", 3, IF(B186="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5170,13 +5189,13 @@
         <v>33</v>
       </c>
       <c r="D187" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>0.7</v>
+        <v>0.77</v>
       </c>
       <c r="F187" s="3">
-        <f>IF(B187="common", 4, IF(B187="uncommon", 3, IF(B187="rare", 1.22, 1)))</f>
+        <f>IF(B187="common", 4, IF(B187="uncommon", 3, IF(B187="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5195,13 +5214,13 @@
         <v>46</v>
       </c>
       <c r="D188" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E188" s="3" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="F188" s="3">
-        <f>IF(B188="common", 4, IF(B188="uncommon", 3, IF(B188="rare", 1.22, 1)))</f>
+        <f>IF(B188="common", 4, IF(B188="uncommon", 3, IF(B188="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5220,13 +5239,13 @@
         <v>33</v>
       </c>
       <c r="D189" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E189" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F189" s="3">
-        <f>IF(B189="common", 4, IF(B189="uncommon", 3, IF(B189="rare", 1.22, 1)))</f>
+        <f>IF(B189="common", 4, IF(B189="uncommon", 3, IF(B189="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5248,10 +5267,10 @@
         <v>0.28</v>
       </c>
       <c r="E190" s="3" t="n">
-        <v>1.44</v>
+        <v>1.28</v>
       </c>
       <c r="F190" s="3">
-        <f>IF(B190="common", 4, IF(B190="uncommon", 3, IF(B190="rare", 1.22, 1)))</f>
+        <f>IF(B190="common", 4, IF(B190="uncommon", 3, IF(B190="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5273,10 +5292,10 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F191" s="3">
-        <f>IF(B191="common", 4, IF(B191="uncommon", 3, IF(B191="rare", 1.22, 1)))</f>
+        <f>IF(B191="common", 4, IF(B191="uncommon", 3, IF(B191="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5295,13 +5314,13 @@
         <v>46</v>
       </c>
       <c r="D192" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E192" s="3" t="n">
         <v>0.14</v>
       </c>
       <c r="F192" s="3">
-        <f>IF(B192="common", 4, IF(B192="uncommon", 3, IF(B192="rare", 1.22, 1)))</f>
+        <f>IF(B192="common", 4, IF(B192="uncommon", 3, IF(B192="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5320,11 +5339,11 @@
         <v>90</v>
       </c>
       <c r="D193" s="3" t="n">
-        <v>0.58</v>
+        <v>0.77</v>
       </c>
       <c r="E193" s="3" t="inlineStr"/>
       <c r="F193" s="3">
-        <f>IF(B193="common", 4, IF(B193="uncommon", 3, IF(B193="rare", 1.22, 1)))</f>
+        <f>IF(B193="common", 4, IF(B193="uncommon", 3, IF(B193="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5343,11 +5362,11 @@
         <v>248</v>
       </c>
       <c r="D194" s="3" t="n">
-        <v>11.85</v>
+        <v>11.82</v>
       </c>
       <c r="E194" s="3" t="inlineStr"/>
       <c r="F194" s="3">
-        <f>IF(B194="common", 4, IF(B194="uncommon", 3, IF(B194="rare", 1.22, 1)))</f>
+        <f>IF(B194="common", 4, IF(B194="uncommon", 3, IF(B194="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5366,11 +5385,11 @@
         <v>225</v>
       </c>
       <c r="D195" s="3" t="n">
-        <v>66.20999999999999</v>
+        <v>68.69</v>
       </c>
       <c r="E195" s="3" t="inlineStr"/>
       <c r="F195" s="3">
-        <f>IF(B195="common", 4, IF(B195="uncommon", 3, IF(B195="rare", 1.22, 1)))</f>
+        <f>IF(B195="common", 4, IF(B195="uncommon", 3, IF(B195="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5392,10 +5411,10 @@
         <v>0.05</v>
       </c>
       <c r="E196" s="3" t="n">
-        <v>0.31</v>
+        <v>0.17</v>
       </c>
       <c r="F196" s="3">
-        <f>IF(B196="common", 4, IF(B196="uncommon", 3, IF(B196="rare", 1.22, 1)))</f>
+        <f>IF(B196="common", 4, IF(B196="uncommon", 3, IF(B196="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5414,13 +5433,13 @@
         <v>21</v>
       </c>
       <c r="D197" s="3" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E197" s="3" t="n">
-        <v>0.88</v>
+        <v>0.93</v>
       </c>
       <c r="F197" s="3">
-        <f>IF(B197="common", 4, IF(B197="uncommon", 3, IF(B197="rare", 1.22, 1)))</f>
+        <f>IF(B197="common", 4, IF(B197="uncommon", 3, IF(B197="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5439,13 +5458,13 @@
         <v>46</v>
       </c>
       <c r="D198" s="3" t="n">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E198" s="3" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="F198" s="3">
-        <f>IF(B198="common", 4, IF(B198="uncommon", 3, IF(B198="rare", 1.22, 1)))</f>
+        <f>IF(B198="common", 4, IF(B198="uncommon", 3, IF(B198="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5464,13 +5483,13 @@
         <v>46</v>
       </c>
       <c r="D199" s="3" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="E199" s="3" t="n">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="F199" s="3">
-        <f>IF(B199="common", 4, IF(B199="uncommon", 3, IF(B199="rare", 1.22, 1)))</f>
+        <f>IF(B199="common", 4, IF(B199="uncommon", 3, IF(B199="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5492,10 +5511,10 @@
         <v>0.12</v>
       </c>
       <c r="E200" s="3" t="n">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="F200" s="3">
-        <f>IF(B200="common", 4, IF(B200="uncommon", 3, IF(B200="rare", 1.22, 1)))</f>
+        <f>IF(B200="common", 4, IF(B200="uncommon", 3, IF(B200="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5514,11 +5533,11 @@
         <v>188</v>
       </c>
       <c r="D201" s="3" t="n">
-        <v>29.75</v>
+        <v>30.34</v>
       </c>
       <c r="E201" s="3" t="inlineStr"/>
       <c r="F201" s="3">
-        <f>IF(B201="common", 4, IF(B201="uncommon", 3, IF(B201="rare", 1.22, 1)))</f>
+        <f>IF(B201="common", 4, IF(B201="uncommon", 3, IF(B201="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5537,13 +5556,13 @@
         <v>46</v>
       </c>
       <c r="D202" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E202" s="3" t="n">
-        <v>0.16</v>
+        <v>0.11</v>
       </c>
       <c r="F202" s="3">
-        <f>IF(B202="common", 4, IF(B202="uncommon", 3, IF(B202="rare", 1.22, 1)))</f>
+        <f>IF(B202="common", 4, IF(B202="uncommon", 3, IF(B202="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5562,13 +5581,13 @@
         <v>46</v>
       </c>
       <c r="D203" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E203" s="3" t="n">
-        <v>1.85</v>
+        <v>1.51</v>
       </c>
       <c r="F203" s="3">
-        <f>IF(B203="common", 4, IF(B203="uncommon", 3, IF(B203="rare", 1.22, 1)))</f>
+        <f>IF(B203="common", 4, IF(B203="uncommon", 3, IF(B203="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5587,13 +5606,13 @@
         <v>21</v>
       </c>
       <c r="D204" s="3" t="n">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="E204" s="3" t="n">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="F204" s="3">
-        <f>IF(B204="common", 4, IF(B204="uncommon", 3, IF(B204="rare", 1.22, 1)))</f>
+        <f>IF(B204="common", 4, IF(B204="uncommon", 3, IF(B204="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5612,11 +5631,11 @@
         <v>90</v>
       </c>
       <c r="D205" s="3" t="n">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
       <c r="E205" s="3" t="inlineStr"/>
       <c r="F205" s="3">
-        <f>IF(B205="common", 4, IF(B205="uncommon", 3, IF(B205="rare", 1.22, 1)))</f>
+        <f>IF(B205="common", 4, IF(B205="uncommon", 3, IF(B205="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5635,11 +5654,11 @@
         <v>248</v>
       </c>
       <c r="D206" s="3" t="n">
-        <v>6.95</v>
+        <v>7.9</v>
       </c>
       <c r="E206" s="3" t="inlineStr"/>
       <c r="F206" s="3">
-        <f>IF(B206="common", 4, IF(B206="uncommon", 3, IF(B206="rare", 1.22, 1)))</f>
+        <f>IF(B206="common", 4, IF(B206="uncommon", 3, IF(B206="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5658,11 +5677,11 @@
         <v>90</v>
       </c>
       <c r="D207" s="3" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="E207" s="3" t="inlineStr"/>
       <c r="F207" s="3">
-        <f>IF(B207="common", 4, IF(B207="uncommon", 3, IF(B207="rare", 1.22, 1)))</f>
+        <f>IF(B207="common", 4, IF(B207="uncommon", 3, IF(B207="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5681,11 +5700,11 @@
         <v>248</v>
       </c>
       <c r="D208" s="3" t="n">
-        <v>7.9</v>
+        <v>8.06</v>
       </c>
       <c r="E208" s="3" t="inlineStr"/>
       <c r="F208" s="3">
-        <f>IF(B208="common", 4, IF(B208="uncommon", 3, IF(B208="rare", 1.22, 1)))</f>
+        <f>IF(B208="common", 4, IF(B208="uncommon", 3, IF(B208="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5704,11 +5723,11 @@
         <v>225</v>
       </c>
       <c r="D209" s="3" t="n">
-        <v>52.05</v>
+        <v>55.36</v>
       </c>
       <c r="E209" s="3" t="inlineStr"/>
       <c r="F209" s="3">
-        <f>IF(B209="common", 4, IF(B209="uncommon", 3, IF(B209="rare", 1.22, 1)))</f>
+        <f>IF(B209="common", 4, IF(B209="uncommon", 3, IF(B209="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5730,10 +5749,10 @@
         <v>0.06</v>
       </c>
       <c r="E210" s="3" t="n">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="F210" s="3">
-        <f>IF(B210="common", 4, IF(B210="uncommon", 3, IF(B210="rare", 1.22, 1)))</f>
+        <f>IF(B210="common", 4, IF(B210="uncommon", 3, IF(B210="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5758,7 +5777,7 @@
         <v>0.59</v>
       </c>
       <c r="F211" s="3">
-        <f>IF(B211="common", 4, IF(B211="uncommon", 3, IF(B211="rare", 1.22, 1)))</f>
+        <f>IF(B211="common", 4, IF(B211="uncommon", 3, IF(B211="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5781,7 +5800,7 @@
       </c>
       <c r="E212" s="3" t="n"/>
       <c r="F212" s="3">
-        <f>IF(B212="common", 4, IF(B212="uncommon", 3, IF(B212="rare", 1.22, 1)))</f>
+        <f>IF(B212="common", 4, IF(B212="uncommon", 3, IF(B212="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5804,7 +5823,7 @@
       </c>
       <c r="E213" s="3" t="n"/>
       <c r="F213" s="3">
-        <f>IF(B213="common", 4, IF(B213="uncommon", 3, IF(B213="rare", 1.22, 1)))</f>
+        <f>IF(B213="common", 4, IF(B213="uncommon", 3, IF(B213="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5827,7 +5846,7 @@
       </c>
       <c r="E214" s="3" t="n"/>
       <c r="F214" s="3">
-        <f>IF(B214="common", 4, IF(B214="uncommon", 3, IF(B214="rare", 1.22, 1)))</f>
+        <f>IF(B214="common", 4, IF(B214="uncommon", 3, IF(B214="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5850,7 +5869,7 @@
       </c>
       <c r="E215" s="3" t="n"/>
       <c r="F215" s="3">
-        <f>IF(B215="common", 4, IF(B215="uncommon", 3, IF(B215="rare", 1.22, 1)))</f>
+        <f>IF(B215="common", 4, IF(B215="uncommon", 3, IF(B215="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5873,7 +5892,7 @@
       </c>
       <c r="E216" s="3" t="n"/>
       <c r="F216" s="3">
-        <f>IF(B216="common", 4, IF(B216="uncommon", 3, IF(B216="rare", 1.22, 1)))</f>
+        <f>IF(B216="common", 4, IF(B216="uncommon", 3, IF(B216="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -5898,7 +5917,7 @@
         <v>0.14</v>
       </c>
       <c r="F217" s="3">
-        <f>IF(B217="common", 4, IF(B217="uncommon", 3, IF(B217="rare", 1.22, 1)))</f>
+        <f>IF(B217="common", 4, IF(B217="uncommon", 3, IF(B217="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
     </row>
@@ -12446,7 +12465,7 @@
       <c r="E1263" s="3" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N210"/>
+  <autoFilter ref="A1:K210"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -12457,7 +12476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12470,194 +12489,224 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>Metric</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="10" t="inlineStr">
         <is>
           <t>ev_common_total</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>0.1093478260869565</v>
+      <c r="B2" s="11" t="n">
+        <v>0.1123913043478261</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>ev_uncommon_total</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>0.1560606060606061</v>
+      <c r="B3" s="11" t="n">
+        <v>0.1696969696969697</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>ev_rare_total</t>
         </is>
       </c>
-      <c r="B4" s="7" t="n">
-        <v>0.2604761904761905</v>
+      <c r="B4" s="11" t="n">
+        <v>0.2695238095238095</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>ev_double_rare_total</t>
         </is>
       </c>
-      <c r="B5" s="7" t="n">
-        <v>0.3288888888888888</v>
+      <c r="B5" s="11" t="n">
+        <v>0.3478888888888889</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>ev_pokeball_total</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>ev_master_ball_total</t>
+        </is>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>ev_hyper_rare_total</t>
         </is>
       </c>
-      <c r="B6" s="7" t="n">
-        <v>0.1356493506493506</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="B8" s="11" t="n">
+        <v>0.1349350649350649</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>ev_ultra_rare_total</t>
         </is>
       </c>
-      <c r="B7" s="7" t="n">
-        <v>0.6429435483870968</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="B9" s="11" t="n">
+        <v>0.6597580645161291</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>ev_SIR_total</t>
         </is>
       </c>
-      <c r="B8" s="7" t="n">
-        <v>2.301644444444444</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="B10" s="11" t="n">
+        <v>2.366622222222222</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>ev_IR_total</t>
         </is>
       </c>
-      <c r="B9" s="7" t="n">
-        <v>1.902606382978723</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="B11" s="11" t="n">
+        <v>1.987606382978723</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>ev_reverse_total</t>
         </is>
       </c>
-      <c r="B10" s="7" t="n">
-        <v>3.066667607754564</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="B12" s="11" t="n">
+        <v>2.824572746094485</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>reverse_multiplier</t>
         </is>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B13" s="11" t="n">
         <v>1.879338061465721</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="6" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>rare_multiplier</t>
         </is>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B14" s="10" t="n">
         <v>1.741272168691524</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="6" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="10" t="inlineStr">
         <is>
           <t>ev_total_for_hits</t>
         </is>
       </c>
-      <c r="B13" s="7" t="n">
-        <v>4.982843726459615</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="inlineStr">
+      <c r="B15" s="11" t="n">
+        <v>5.14892173465214</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="inlineStr">
         <is>
           <t>ev_hits_total</t>
         </is>
       </c>
-      <c r="B14" s="7" t="n">
-        <v>5.311732615348505</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="inlineStr">
+      <c r="B16" s="11" t="n">
+        <v>5.496810623541029</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>total_ev</t>
         </is>
       </c>
-      <c r="B15" s="7" t="n">
-        <v>12.43417083607831</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="inlineStr">
+      <c r="B17" s="11" t="n">
+        <v>11.07690299510566</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>net_value</t>
         </is>
       </c>
-      <c r="B16" s="7" t="n">
-        <v>1.544170836078312</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="inlineStr">
+      <c r="B18" s="11" t="n">
+        <v>0.1869029951056582</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>roi</t>
         </is>
       </c>
-      <c r="B17" s="8" t="n">
-        <v>0.1417971382992023</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="inlineStr">
+      <c r="B19" s="12" t="n">
+        <v>0.01716280946792081</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>roi_percent</t>
         </is>
       </c>
-      <c r="B18" s="8" t="n">
-        <v>13.17971382992023</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="inlineStr">
-        <is>
-          <t>hit_prob_pct</t>
-        </is>
-      </c>
-      <c r="B19" s="8" t="n">
+      <c r="B20" s="12" t="n">
+        <v>0.7162809467920814</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>no_hit_probability_percentage</t>
+        </is>
+      </c>
+      <c r="B21" s="12" t="n">
+        <v>68.32877110235633</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>hit_probability_percentage</t>
+        </is>
+      </c>
+      <c r="B22" s="12" t="n">
         <v>31.67122889764367</v>
       </c>
     </row>

</xml_diff>

<commit_message>
now works for 2 sets. Need to automate price pulling
</commit_message>
<xml_diff>
--- a/Expected Value and Cost Ratio Calculator Pokemon/excelDocs/scarletAndViolet151/pokemon_data.xlsx
+++ b/Expected Value and Cost Ratio Calculator Pokemon/excelDocs/scarletAndViolet151/pokemon_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-27375" yWindow="90" windowWidth="25260" windowHeight="11385" tabRatio="797" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3450" yWindow="825" windowWidth="25260" windowHeight="11385" tabRatio="797" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -115,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -138,6 +138,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -148,6 +151,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -520,8 +526,8 @@
   </sheetPr>
   <dimension ref="A1:K1263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -602,7 +608,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
@@ -612,7 +618,7 @@
         <v>0.06</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F2" s="3">
         <f>IF(B2="common", 4, IF(B2="uncommon", 3, IF(B2="rare", 1.74127216869152, 1)))</f>
@@ -644,17 +650,17 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.55</v>
+        <v>0.53</v>
       </c>
       <c r="F3" s="3">
         <f>IF(B3="common", 4, IF(B3="uncommon", 3, IF(B3="rare", 1.74127216869152, 1)))</f>
@@ -673,14 +679,14 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>1.12</v>
+        <v>1.13</v>
       </c>
       <c r="E4" s="3" t="inlineStr"/>
       <c r="F4" s="3">
@@ -688,7 +694,7 @@
         <v/>
       </c>
       <c r="H4">
-        <f>SUMPRODUCT((B2:B210="Rare") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>0.792892156862745*SUMPRODUCT((B2:B217="Rare") * D2:D217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -700,14 +706,14 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>7.46</v>
+        <v>7.37</v>
       </c>
       <c r="E5" s="3" t="inlineStr"/>
       <c r="F5" s="3">
@@ -715,7 +721,7 @@
         <v/>
       </c>
       <c r="H5">
-        <f>SUMPRODUCT((B2:B217="Double Rare") * D2:D217 * F2:F217 / C2:C217)</f>
+        <f>1.88541666666666* SUMPRODUCT((C2:C217&lt;&gt;"") * (E2:E217&lt;&gt;"") * (E2:E217 / C2:C217))</f>
         <v/>
       </c>
     </row>
@@ -727,14 +733,14 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
         <v>225</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>43.34</v>
+        <v>43.91</v>
       </c>
       <c r="E6" s="3" t="inlineStr"/>
       <c r="F6" s="3">
@@ -742,7 +748,7 @@
         <v/>
       </c>
       <c r="H6">
-        <f>SUMPRODUCT((B2:B210="Hyper Rare") * D2:D210 * F2:F210 / C2:C210)</f>
+        <f>SUMPRODUCT((B2:B217="Illustration Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -754,7 +760,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C7" s="3" t="n">
@@ -764,14 +770,14 @@
         <v>0.08</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="F7" s="3">
         <f>IF(B7="common", 4, IF(B7="uncommon", 3, IF(B7="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H7">
-        <f>SUMPRODUCT((B2:B217="Illustration Rare") * D2:D217 * F2:F217 / C2:C217)</f>
+        <f>SUMPRODUCT((B2:B217="Special Illustration Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -783,24 +789,24 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C8" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>1.06</v>
+        <v>0.95</v>
       </c>
       <c r="F8" s="3">
         <f>IF(B8="common", 4, IF(B8="uncommon", 3, IF(B8="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H8">
-        <f>SUMPRODUCT((B2:B217="Special Illustration Rare") * D2:D217 * F2:F217 / C2:C217)</f>
+        <f>SUMPRODUCT((B2:B217="Double Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -812,24 +818,24 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C9" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="F9" s="3">
         <f>IF(B9="common", 4, IF(B9="uncommon", 3, IF(B9="rare", 1.74127216869152, 1)))</f>
         <v/>
       </c>
       <c r="H9">
-        <f>SUMPRODUCT((B2:B217="Ultra Rare") * D2:D217 * F2:F217 / C2:C217)</f>
+        <f>SUMPRODUCT((B2:B217="Hyper Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -841,14 +847,14 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.76</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E10" s="3" t="inlineStr"/>
       <c r="F10" s="3">
@@ -856,7 +862,7 @@
         <v/>
       </c>
       <c r="H10">
-        <f>1.88 * SUMPRODUCT((C2:C217&lt;&gt;"") * (E2:E217&lt;&gt;"") * (E2:E217 / C2:C217))</f>
+        <f>SUMPRODUCT((B2:B217="Ultra Rare") * D2:D217 * F2:F217 / C2:C217)</f>
         <v/>
       </c>
     </row>
@@ -868,14 +874,14 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>4.89</v>
+        <v>4.98</v>
       </c>
       <c r="E11" s="3" t="inlineStr"/>
       <c r="F11" s="3">
@@ -891,17 +897,17 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C12" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F12" s="3">
         <f>IF(B12="common", 4, IF(B12="uncommon", 3, IF(B12="rare", 1.74127216869152, 1)))</f>
@@ -916,17 +922,17 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C13" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>0.74</v>
+        <v>0.71</v>
       </c>
       <c r="F13" s="3">
         <f>IF(B13="common", 4, IF(B13="uncommon", 3, IF(B13="rare", 1.74127216869152, 1)))</f>
@@ -941,14 +947,14 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Hyper Rare</t>
+          <t>hyper rare</t>
         </is>
       </c>
       <c r="C14" s="3" t="n">
         <v>154</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>4.95</v>
+        <v>4.7</v>
       </c>
       <c r="E14" s="3" t="inlineStr"/>
       <c r="F14" s="3">
@@ -964,7 +970,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C15" s="3" t="n">
@@ -989,7 +995,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C16" s="3" t="n">
@@ -999,7 +1005,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F16" s="3">
         <f>IF(B16="common", 4, IF(B16="uncommon", 3, IF(B16="rare", 1.74127216869152, 1)))</f>
@@ -1014,17 +1020,17 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C17" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>1.12</v>
+        <v>1.22</v>
       </c>
       <c r="F17" s="3">
         <f>IF(B17="common", 4, IF(B17="uncommon", 3, IF(B17="rare", 1.74127216869152, 1)))</f>
@@ -1039,7 +1045,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C18" s="3" t="n">
@@ -1049,7 +1055,7 @@
         <v>0.12</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="F18" s="3">
         <f>IF(B18="common", 4, IF(B18="uncommon", 3, IF(B18="rare", 1.74127216869152, 1)))</f>
@@ -1064,14 +1070,14 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C19" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>3.05</v>
+        <v>3.07</v>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
       <c r="F19" s="3">
@@ -1087,14 +1093,14 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C20" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>1.18</v>
+        <v>0.96</v>
       </c>
       <c r="E20" s="3" t="inlineStr"/>
       <c r="F20" s="3">
@@ -1110,14 +1116,14 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C21" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>14.89</v>
+        <v>14.5</v>
       </c>
       <c r="E21" s="3" t="inlineStr"/>
       <c r="F21" s="3">
@@ -1133,14 +1139,14 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C22" s="3" t="n">
         <v>225</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>73.55</v>
+        <v>73.09999999999999</v>
       </c>
       <c r="E22" s="3" t="inlineStr"/>
       <c r="F22" s="3">
@@ -1156,17 +1162,17 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C23" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="F23" s="3">
         <f>IF(B23="common", 4, IF(B23="uncommon", 3, IF(B23="rare", 1.74127216869152, 1)))</f>
@@ -1181,14 +1187,14 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C24" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>37.52</v>
+        <v>37.01</v>
       </c>
       <c r="E24" s="3" t="inlineStr"/>
       <c r="F24" s="3">
@@ -1204,7 +1210,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C25" s="3" t="n">
@@ -1214,7 +1220,7 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F25" s="3">
         <f>IF(B25="common", 4, IF(B25="uncommon", 3, IF(B25="rare", 1.74127216869152, 1)))</f>
@@ -1229,14 +1235,14 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C26" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>0.21</v>
@@ -1254,14 +1260,14 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C27" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>9.56</v>
+        <v>9.460000000000001</v>
       </c>
       <c r="E27" s="3" t="inlineStr"/>
       <c r="F27" s="3">
@@ -1277,17 +1283,17 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C28" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>0.65</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F28" s="3">
         <f>IF(B28="common", 4, IF(B28="uncommon", 3, IF(B28="rare", 1.74127216869152, 1)))</f>
@@ -1302,14 +1308,14 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C29" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>4.71</v>
+        <v>5.05</v>
       </c>
       <c r="E29" s="3" t="inlineStr"/>
       <c r="F29" s="3">
@@ -1325,14 +1331,14 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C30" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>31.27</v>
+        <v>31.25</v>
       </c>
       <c r="E30" s="3" t="inlineStr"/>
       <c r="F30" s="3">
@@ -1348,14 +1354,14 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C31" s="3" t="n">
         <v>225</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>210.14</v>
+        <v>214.14</v>
       </c>
       <c r="E31" s="3" t="inlineStr"/>
       <c r="F31" s="3">
@@ -1371,14 +1377,14 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C32" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>0.19</v>
@@ -1396,14 +1402,14 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C33" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>52.06</v>
+        <v>51.42</v>
       </c>
       <c r="E33" s="3" t="inlineStr"/>
       <c r="F33" s="3">
@@ -1419,7 +1425,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C34" s="3" t="n">
@@ -1429,7 +1435,7 @@
         <v>0.1</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="F34" s="3">
         <f>IF(B34="common", 4, IF(B34="uncommon", 3, IF(B34="rare", 1.74127216869152, 1)))</f>
@@ -1444,14 +1450,14 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C35" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D35" s="3" t="n">
-        <v>34.86</v>
+        <v>34.16</v>
       </c>
       <c r="E35" s="3" t="inlineStr"/>
       <c r="F35" s="3">
@@ -1467,7 +1473,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C36" s="3" t="n">
@@ -1492,7 +1498,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C37" s="3" t="n">
@@ -1517,17 +1523,17 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C38" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E38" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F38" s="3">
         <f>IF(B38="common", 4, IF(B38="uncommon", 3, IF(B38="rare", 1.74127216869152, 1)))</f>
@@ -1542,17 +1548,17 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C39" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F39" s="3">
         <f>IF(B39="common", 4, IF(B39="uncommon", 3, IF(B39="rare", 1.74127216869152, 1)))</f>
@@ -1567,17 +1573,17 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C40" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E40" s="3" t="n">
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="F40" s="3">
         <f>IF(B40="common", 4, IF(B40="uncommon", 3, IF(B40="rare", 1.74127216869152, 1)))</f>
@@ -1592,17 +1598,17 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C41" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="F41" s="3">
         <f>IF(B41="common", 4, IF(B41="uncommon", 3, IF(B41="rare", 1.74127216869152, 1)))</f>
@@ -1617,14 +1623,14 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C42" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>4.04</v>
+        <v>3.92</v>
       </c>
       <c r="E42" s="3" t="inlineStr"/>
       <c r="F42" s="3">
@@ -1640,17 +1646,17 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C43" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D43" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F43" s="3">
         <f>IF(B43="common", 4, IF(B43="uncommon", 3, IF(B43="rare", 1.74127216869152, 1)))</f>
@@ -1665,14 +1671,14 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C44" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D44" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E44" s="3" t="n">
         <v>0.15</v>
@@ -1690,17 +1696,17 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C45" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="F45" s="3">
         <f>IF(B45="common", 4, IF(B45="uncommon", 3, IF(B45="rare", 1.74127216869152, 1)))</f>
@@ -1715,14 +1721,14 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C46" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>0.34</v>
+        <v>0.47</v>
       </c>
       <c r="E46" s="3" t="inlineStr"/>
       <c r="F46" s="3">
@@ -1738,17 +1744,17 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C47" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D47" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="F47" s="3">
         <f>IF(B47="common", 4, IF(B47="uncommon", 3, IF(B47="rare", 1.74127216869152, 1)))</f>
@@ -1763,7 +1769,7 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C48" s="3" t="n">
@@ -1788,17 +1794,17 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C49" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D49" s="3" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>2</v>
+        <v>2.18</v>
       </c>
       <c r="F49" s="3">
         <f>IF(B49="common", 4, IF(B49="uncommon", 3, IF(B49="rare", 1.74127216869152, 1)))</f>
@@ -1813,14 +1819,14 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C50" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D50" s="3" t="n">
-        <v>25.78</v>
+        <v>25.53</v>
       </c>
       <c r="E50" s="3" t="inlineStr"/>
       <c r="F50" s="3">
@@ -1836,17 +1842,17 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C51" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>0.41</v>
+        <v>0.37</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>1.32</v>
+        <v>1.3</v>
       </c>
       <c r="F51" s="3">
         <f>IF(B51="common", 4, IF(B51="uncommon", 3, IF(B51="rare", 1.74127216869152, 1)))</f>
@@ -1861,17 +1867,17 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C52" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D52" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F52" s="3">
         <f>IF(B52="common", 4, IF(B52="uncommon", 3, IF(B52="rare", 1.74127216869152, 1)))</f>
@@ -1886,7 +1892,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C53" s="3" t="n">
@@ -1896,7 +1902,7 @@
         <v>0.05</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F53" s="3">
         <f>IF(B53="common", 4, IF(B53="uncommon", 3, IF(B53="rare", 1.74127216869152, 1)))</f>
@@ -1911,7 +1917,7 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C54" s="3" t="n">
@@ -1936,17 +1942,17 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C55" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D55" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="F55" s="3">
         <f>IF(B55="common", 4, IF(B55="uncommon", 3, IF(B55="rare", 1.74127216869152, 1)))</f>
@@ -1961,7 +1967,7 @@
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C56" s="3" t="n">
@@ -1971,7 +1977,7 @@
         <v>0.05</v>
       </c>
       <c r="E56" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F56" s="3">
         <f>IF(B56="common", 4, IF(B56="uncommon", 3, IF(B56="rare", 1.74127216869152, 1)))</f>
@@ -1986,7 +1992,7 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C57" s="3" t="n">
@@ -1996,7 +2002,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="F57" s="3">
         <f>IF(B57="common", 4, IF(B57="uncommon", 3, IF(B57="rare", 1.74127216869152, 1)))</f>
@@ -2011,7 +2017,7 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C58" s="3" t="n">
@@ -2021,7 +2027,7 @@
         <v>0.13</v>
       </c>
       <c r="E58" s="3" t="n">
-        <v>1.27</v>
+        <v>1.23</v>
       </c>
       <c r="F58" s="3">
         <f>IF(B58="common", 4, IF(B58="uncommon", 3, IF(B58="rare", 1.74127216869152, 1)))</f>
@@ -2036,7 +2042,7 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C59" s="3" t="n">
@@ -2046,7 +2052,7 @@
         <v>0.16</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>1.41</v>
+        <v>1.43</v>
       </c>
       <c r="F59" s="3">
         <f>IF(B59="common", 4, IF(B59="uncommon", 3, IF(B59="rare", 1.74127216869152, 1)))</f>
@@ -2061,17 +2067,17 @@
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C60" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D60" s="3" t="n">
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>0.8</v>
+        <v>0.84</v>
       </c>
       <c r="F60" s="3">
         <f>IF(B60="common", 4, IF(B60="uncommon", 3, IF(B60="rare", 1.74127216869152, 1)))</f>
@@ -2086,14 +2092,14 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C61" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>6.99</v>
+        <v>6.92</v>
       </c>
       <c r="E61" s="3" t="inlineStr"/>
       <c r="F61" s="3">
@@ -2109,14 +2115,14 @@
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C62" s="3" t="n">
         <v>225</v>
       </c>
       <c r="D62" s="3" t="n">
-        <v>14.98</v>
+        <v>14.48</v>
       </c>
       <c r="E62" s="3" t="inlineStr"/>
       <c r="F62" s="3">
@@ -2132,7 +2138,7 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C63" s="3" t="n">
@@ -2157,7 +2163,7 @@
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C64" s="3" t="n">
@@ -2167,7 +2173,7 @@
         <v>0.1</v>
       </c>
       <c r="E64" s="3" t="n">
-        <v>1.26</v>
+        <v>1.31</v>
       </c>
       <c r="F64" s="3">
         <f>IF(B64="common", 4, IF(B64="uncommon", 3, IF(B64="rare", 1.74127216869152, 1)))</f>
@@ -2182,7 +2188,7 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C65" s="3" t="n">
@@ -2192,7 +2198,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="F65" s="3">
         <f>IF(B65="common", 4, IF(B65="uncommon", 3, IF(B65="rare", 1.74127216869152, 1)))</f>
@@ -2207,17 +2213,17 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C66" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F66" s="3">
         <f>IF(B66="common", 4, IF(B66="uncommon", 3, IF(B66="rare", 1.74127216869152, 1)))</f>
@@ -2232,14 +2238,14 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C67" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>0.25</v>
+        <v>0.29</v>
       </c>
       <c r="E67" s="3" t="n">
         <v>1.08</v>
@@ -2257,14 +2263,14 @@
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C68" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D68" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E68" s="3" t="n">
         <v>0.18</v>
@@ -2282,17 +2288,17 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C69" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>0.27</v>
+        <v>0.3</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>1.78</v>
+        <v>1.82</v>
       </c>
       <c r="F69" s="3">
         <f>IF(B69="common", 4, IF(B69="uncommon", 3, IF(B69="rare", 1.74127216869152, 1)))</f>
@@ -2307,7 +2313,7 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C70" s="3" t="n">
@@ -2332,17 +2338,17 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C71" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>1.03</v>
+        <v>0.98</v>
       </c>
       <c r="F71" s="3">
         <f>IF(B71="common", 4, IF(B71="uncommon", 3, IF(B71="rare", 1.74127216869152, 1)))</f>
@@ -2357,14 +2363,14 @@
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C72" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D72" s="3" t="n">
-        <v>4.99</v>
+        <v>5.05</v>
       </c>
       <c r="E72" s="3" t="inlineStr"/>
       <c r="F72" s="3">
@@ -2380,14 +2386,14 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C73" s="3" t="n">
         <v>225</v>
       </c>
       <c r="D73" s="3" t="n">
-        <v>15.6</v>
+        <v>13.93</v>
       </c>
       <c r="E73" s="3" t="inlineStr"/>
       <c r="F73" s="3">
@@ -2403,14 +2409,14 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C74" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E74" s="3" t="n">
         <v>0.21</v>
@@ -2428,7 +2434,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C75" s="3" t="n">
@@ -2453,17 +2459,17 @@
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C76" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D76" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E76" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F76" s="3">
         <f>IF(B76="common", 4, IF(B76="uncommon", 3, IF(B76="rare", 1.74127216869152, 1)))</f>
@@ -2478,7 +2484,7 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C77" s="3" t="n">
@@ -2503,14 +2509,14 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C78" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D78" s="3" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="E78" s="3" t="inlineStr"/>
       <c r="F78" s="3">
@@ -2526,14 +2532,14 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C79" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D79" s="3" t="n">
-        <v>5.18</v>
+        <v>4.83</v>
       </c>
       <c r="E79" s="3" t="inlineStr"/>
       <c r="F79" s="3">
@@ -2549,17 +2555,17 @@
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C80" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D80" s="3" t="n">
-        <v>0.26</v>
+        <v>0.14</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="F80" s="3">
         <f>IF(B80="common", 4, IF(B80="uncommon", 3, IF(B80="rare", 1.74127216869152, 1)))</f>
@@ -2574,7 +2580,7 @@
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C81" s="3" t="n">
@@ -2599,14 +2605,14 @@
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C82" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D82" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E82" s="3" t="n">
         <v>0.15</v>
@@ -2624,7 +2630,7 @@
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C83" s="3" t="n">
@@ -2649,17 +2655,17 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C84" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D84" s="3" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="F84" s="3">
         <f>IF(B84="common", 4, IF(B84="uncommon", 3, IF(B84="rare", 1.74127216869152, 1)))</f>
@@ -2674,17 +2680,17 @@
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C85" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D85" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="F85" s="3">
         <f>IF(B85="common", 4, IF(B85="uncommon", 3, IF(B85="rare", 1.74127216869152, 1)))</f>
@@ -2699,17 +2705,17 @@
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C86" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D86" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>1.5</v>
+        <v>1.51</v>
       </c>
       <c r="F86" s="3">
         <f>IF(B86="common", 4, IF(B86="uncommon", 3, IF(B86="rare", 1.74127216869152, 1)))</f>
@@ -2724,17 +2730,17 @@
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C87" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D87" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E87" s="3" t="n">
-        <v>1.12</v>
+        <v>1.26</v>
       </c>
       <c r="F87" s="3">
         <f>IF(B87="common", 4, IF(B87="uncommon", 3, IF(B87="rare", 1.74127216869152, 1)))</f>
@@ -2749,7 +2755,7 @@
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C88" s="3" t="n">
@@ -2759,7 +2765,7 @@
         <v>0.06</v>
       </c>
       <c r="E88" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F88" s="3">
         <f>IF(B88="common", 4, IF(B88="uncommon", 3, IF(B88="rare", 1.74127216869152, 1)))</f>
@@ -2774,7 +2780,7 @@
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C89" s="3" t="n">
@@ -2784,7 +2790,7 @@
         <v>0.1</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>1.3</v>
+        <v>1.32</v>
       </c>
       <c r="F89" s="3">
         <f>IF(B89="common", 4, IF(B89="uncommon", 3, IF(B89="rare", 1.74127216869152, 1)))</f>
@@ -2799,7 +2805,7 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C90" s="3" t="n">
@@ -2824,14 +2830,14 @@
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C91" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D91" s="3" t="n">
-        <v>26.26</v>
+        <v>26.78</v>
       </c>
       <c r="E91" s="3" t="inlineStr"/>
       <c r="F91" s="3">
@@ -2847,17 +2853,17 @@
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C92" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D92" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="F92" s="3">
         <f>IF(B92="common", 4, IF(B92="uncommon", 3, IF(B92="rare", 1.74127216869152, 1)))</f>
@@ -2872,17 +2878,17 @@
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C93" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D93" s="3" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="E93" s="3" t="n">
-        <v>2.24</v>
+        <v>2.36</v>
       </c>
       <c r="F93" s="3">
         <f>IF(B93="common", 4, IF(B93="uncommon", 3, IF(B93="rare", 1.74127216869152, 1)))</f>
@@ -2897,14 +2903,14 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C94" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D94" s="3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="E94" s="3" t="inlineStr"/>
       <c r="F94" s="3">
@@ -2920,14 +2926,14 @@
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C95" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D95" s="3" t="n">
-        <v>5.3</v>
+        <v>5.09</v>
       </c>
       <c r="E95" s="3" t="inlineStr"/>
       <c r="F95" s="3">
@@ -2943,7 +2949,7 @@
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C96" s="3" t="n">
@@ -2953,7 +2959,7 @@
         <v>0.09</v>
       </c>
       <c r="E96" s="3" t="n">
-        <v>1.12</v>
+        <v>1.06</v>
       </c>
       <c r="F96" s="3">
         <f>IF(B96="common", 4, IF(B96="uncommon", 3, IF(B96="rare", 1.74127216869152, 1)))</f>
@@ -2968,17 +2974,17 @@
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C97" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D97" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="F97" s="3">
         <f>IF(B97="common", 4, IF(B97="uncommon", 3, IF(B97="rare", 1.74127216869152, 1)))</f>
@@ -2993,17 +2999,17 @@
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C98" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D98" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E98" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F98" s="3">
         <f>IF(B98="common", 4, IF(B98="uncommon", 3, IF(B98="rare", 1.74127216869152, 1)))</f>
@@ -3018,7 +3024,7 @@
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C99" s="3" t="n">
@@ -3028,7 +3034,7 @@
         <v>0.1</v>
       </c>
       <c r="E99" s="3" t="n">
-        <v>2.01</v>
+        <v>2.1</v>
       </c>
       <c r="F99" s="3">
         <f>IF(B99="common", 4, IF(B99="uncommon", 3, IF(B99="rare", 1.74127216869152, 1)))</f>
@@ -3043,14 +3049,14 @@
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C100" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D100" s="3" t="n">
-        <v>0.59</v>
+        <v>0.7</v>
       </c>
       <c r="E100" s="3" t="inlineStr"/>
       <c r="F100" s="3">
@@ -3066,14 +3072,14 @@
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C101" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D101" s="3" t="n">
-        <v>5.8</v>
+        <v>5.55</v>
       </c>
       <c r="E101" s="3" t="inlineStr"/>
       <c r="F101" s="3">
@@ -3089,17 +3095,17 @@
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C102" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D102" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E102" s="3" t="n">
-        <v>1.26</v>
+        <v>1.3</v>
       </c>
       <c r="F102" s="3">
         <f>IF(B102="common", 4, IF(B102="uncommon", 3, IF(B102="rare", 1.74127216869152, 1)))</f>
@@ -3114,7 +3120,7 @@
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C103" s="3" t="n">
@@ -3139,7 +3145,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C104" s="3" t="n">
@@ -3164,7 +3170,7 @@
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C105" s="3" t="n">
@@ -3174,7 +3180,7 @@
         <v>0.08</v>
       </c>
       <c r="E105" s="3" t="n">
-        <v>1.65</v>
+        <v>1.63</v>
       </c>
       <c r="F105" s="3">
         <f>IF(B105="common", 4, IF(B105="uncommon", 3, IF(B105="rare", 1.74127216869152, 1)))</f>
@@ -3189,17 +3195,17 @@
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C106" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D106" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E106" s="3" t="n">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="F106" s="3">
         <f>IF(B106="common", 4, IF(B106="uncommon", 3, IF(B106="rare", 1.74127216869152, 1)))</f>
@@ -3214,17 +3220,17 @@
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C107" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D107" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E107" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F107" s="3">
         <f>IF(B107="common", 4, IF(B107="uncommon", 3, IF(B107="rare", 1.74127216869152, 1)))</f>
@@ -3239,17 +3245,17 @@
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C108" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D108" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="E108" s="3" t="n">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="F108" s="3">
         <f>IF(B108="common", 4, IF(B108="uncommon", 3, IF(B108="rare", 1.74127216869152, 1)))</f>
@@ -3264,17 +3270,17 @@
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C109" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D109" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E109" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F109" s="3">
         <f>IF(B109="common", 4, IF(B109="uncommon", 3, IF(B109="rare", 1.74127216869152, 1)))</f>
@@ -3289,14 +3295,14 @@
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C110" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D110" s="3" t="n">
-        <v>11.24</v>
+        <v>11.22</v>
       </c>
       <c r="E110" s="3" t="inlineStr"/>
       <c r="F110" s="3">
@@ -3312,17 +3318,17 @@
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C111" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D111" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F111" s="3">
         <f>IF(B111="common", 4, IF(B111="uncommon", 3, IF(B111="rare", 1.74127216869152, 1)))</f>
@@ -3337,7 +3343,7 @@
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C112" s="3" t="n">
@@ -3347,7 +3353,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E112" s="3" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="F112" s="3">
         <f>IF(B112="common", 4, IF(B112="uncommon", 3, IF(B112="rare", 1.74127216869152, 1)))</f>
@@ -3362,14 +3368,14 @@
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C113" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D113" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E113" s="3" t="n">
         <v>0.9399999999999999</v>
@@ -3387,7 +3393,7 @@
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C114" s="3" t="n">
@@ -3397,7 +3403,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E114" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F114" s="3">
         <f>IF(B114="common", 4, IF(B114="uncommon", 3, IF(B114="rare", 1.74127216869152, 1)))</f>
@@ -3412,14 +3418,14 @@
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C115" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D115" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E115" s="3" t="n">
         <v>0.13</v>
@@ -3437,14 +3443,14 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C116" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D116" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E116" s="3" t="n">
         <v>0.13</v>
@@ -3462,7 +3468,7 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C117" s="3" t="n">
@@ -3472,7 +3478,7 @@
         <v>0.16</v>
       </c>
       <c r="E117" s="3" t="n">
-        <v>0.54</v>
+        <v>0.58</v>
       </c>
       <c r="F117" s="3">
         <f>IF(B117="common", 4, IF(B117="uncommon", 3, IF(B117="rare", 1.74127216869152, 1)))</f>
@@ -3487,7 +3493,7 @@
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C118" s="3" t="n">
@@ -3497,7 +3503,7 @@
         <v>0.06</v>
       </c>
       <c r="E118" s="3" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="F118" s="3">
         <f>IF(B118="common", 4, IF(B118="uncommon", 3, IF(B118="rare", 1.74127216869152, 1)))</f>
@@ -3512,17 +3518,17 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C119" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D119" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>2.22</v>
+        <v>2.31</v>
       </c>
       <c r="F119" s="3">
         <f>IF(B119="common", 4, IF(B119="uncommon", 3, IF(B119="rare", 1.74127216869152, 1)))</f>
@@ -3537,14 +3543,14 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C120" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D120" s="3" t="n">
-        <v>7.21</v>
+        <v>6.62</v>
       </c>
       <c r="E120" s="3" t="inlineStr"/>
       <c r="F120" s="3">
@@ -3560,14 +3566,14 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C121" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D121" s="3" t="n">
-        <v>19.11</v>
+        <v>18.71</v>
       </c>
       <c r="E121" s="3" t="inlineStr"/>
       <c r="F121" s="3">
@@ -3583,14 +3589,14 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Hyper Rare</t>
+          <t>hyper rare</t>
         </is>
       </c>
       <c r="C122" s="3" t="n">
         <v>154</v>
       </c>
       <c r="D122" s="3" t="n">
-        <v>13.27</v>
+        <v>13.41</v>
       </c>
       <c r="E122" s="3" t="inlineStr"/>
       <c r="F122" s="3">
@@ -3606,14 +3612,14 @@
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C123" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D123" s="3" t="n">
-        <v>9.75</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="E123" s="3" t="inlineStr"/>
       <c r="F123" s="3">
@@ -3629,17 +3635,17 @@
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C124" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D124" s="3" t="n">
-        <v>0.51</v>
+        <v>0.55</v>
       </c>
       <c r="E124" s="3" t="n">
-        <v>1.58</v>
+        <v>1.57</v>
       </c>
       <c r="F124" s="3">
         <f>IF(B124="common", 4, IF(B124="uncommon", 3, IF(B124="rare", 1.74127216869152, 1)))</f>
@@ -3654,7 +3660,7 @@
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C125" s="3" t="n">
@@ -3664,7 +3670,7 @@
         <v>0.21</v>
       </c>
       <c r="E125" s="3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="F125" s="3">
         <f>IF(B125="common", 4, IF(B125="uncommon", 3, IF(B125="rare", 1.74127216869152, 1)))</f>
@@ -3679,7 +3685,7 @@
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C126" s="3" t="n">
@@ -3704,14 +3710,14 @@
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C127" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D127" s="3" t="n">
-        <v>5.79</v>
+        <v>5.49</v>
       </c>
       <c r="E127" s="3" t="inlineStr"/>
       <c r="F127" s="3">
@@ -3727,14 +3733,14 @@
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C128" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D128" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E128" s="3" t="n">
         <v>0.22</v>
@@ -3752,7 +3758,7 @@
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C129" s="3" t="n">
@@ -3762,7 +3768,7 @@
         <v>0.19</v>
       </c>
       <c r="E129" s="3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.77</v>
       </c>
       <c r="F129" s="3">
         <f>IF(B129="common", 4, IF(B129="uncommon", 3, IF(B129="rare", 1.74127216869152, 1)))</f>
@@ -3777,14 +3783,14 @@
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C130" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D130" s="3" t="n">
-        <v>9.58</v>
+        <v>9.9</v>
       </c>
       <c r="E130" s="3" t="inlineStr"/>
       <c r="F130" s="3">
@@ -3800,7 +3806,7 @@
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C131" s="3" t="n">
@@ -3810,7 +3816,7 @@
         <v>0.06</v>
       </c>
       <c r="E131" s="3" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="F131" s="3">
         <f>IF(B131="common", 4, IF(B131="uncommon", 3, IF(B131="rare", 1.74127216869152, 1)))</f>
@@ -3825,17 +3831,17 @@
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C132" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D132" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E132" s="3" t="n">
-        <v>1.98</v>
+        <v>1.95</v>
       </c>
       <c r="F132" s="3">
         <f>IF(B132="common", 4, IF(B132="uncommon", 3, IF(B132="rare", 1.74127216869152, 1)))</f>
@@ -3850,17 +3856,17 @@
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C133" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D133" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E133" s="3" t="n">
-        <v>1.56</v>
+        <v>1.53</v>
       </c>
       <c r="F133" s="3">
         <f>IF(B133="common", 4, IF(B133="uncommon", 3, IF(B133="rare", 1.74127216869152, 1)))</f>
@@ -3875,14 +3881,14 @@
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C134" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D134" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E134" s="3" t="n">
         <v>0.19</v>
@@ -3900,17 +3906,17 @@
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C135" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D135" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E135" s="3" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="F135" s="3">
         <f>IF(B135="common", 4, IF(B135="uncommon", 3, IF(B135="rare", 1.74127216869152, 1)))</f>
@@ -3925,14 +3931,14 @@
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C136" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D136" s="3" t="n">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
       <c r="E136" s="3" t="inlineStr"/>
       <c r="F136" s="3">
@@ -3948,14 +3954,14 @@
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C137" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D137" s="3" t="n">
-        <v>7.87</v>
+        <v>6.83</v>
       </c>
       <c r="E137" s="3" t="inlineStr"/>
       <c r="F137" s="3">
@@ -3971,7 +3977,7 @@
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C138" s="3" t="n">
@@ -3981,7 +3987,7 @@
         <v>0.08</v>
       </c>
       <c r="E138" s="3" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="F138" s="3">
         <f>IF(B138="common", 4, IF(B138="uncommon", 3, IF(B138="rare", 1.74127216869152, 1)))</f>
@@ -3996,7 +4002,7 @@
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C139" s="3" t="n">
@@ -4006,7 +4012,7 @@
         <v>0.06</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>2.36</v>
+        <v>2.33</v>
       </c>
       <c r="F139" s="3">
         <f>IF(B139="common", 4, IF(B139="uncommon", 3, IF(B139="rare", 1.74127216869152, 1)))</f>
@@ -4021,14 +4027,14 @@
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C140" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D140" s="3" t="n">
-        <v>8</v>
+        <v>7.85</v>
       </c>
       <c r="E140" s="3" t="inlineStr"/>
       <c r="F140" s="3">
@@ -4044,14 +4050,14 @@
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C141" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D141" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="E141" s="3" t="n">
         <v>0.59</v>
@@ -4069,7 +4075,7 @@
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C142" s="3" t="n">
@@ -4079,7 +4085,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E142" s="3" t="n">
-        <v>1.36</v>
+        <v>1.29</v>
       </c>
       <c r="F142" s="3">
         <f>IF(B142="common", 4, IF(B142="uncommon", 3, IF(B142="rare", 1.74127216869152, 1)))</f>
@@ -4094,7 +4100,7 @@
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C143" s="3" t="n">
@@ -4119,7 +4125,7 @@
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C144" s="3" t="n">
@@ -4129,7 +4135,7 @@
         <v>0.1</v>
       </c>
       <c r="E144" s="3" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="F144" s="3">
         <f>IF(B144="common", 4, IF(B144="uncommon", 3, IF(B144="rare", 1.74127216869152, 1)))</f>
@@ -4144,17 +4150,17 @@
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C145" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D145" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="F145" s="3">
         <f>IF(B145="common", 4, IF(B145="uncommon", 3, IF(B145="rare", 1.74127216869152, 1)))</f>
@@ -4169,7 +4175,7 @@
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C146" s="3" t="n">
@@ -4179,7 +4185,7 @@
         <v>0.06</v>
       </c>
       <c r="E146" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F146" s="3">
         <f>IF(B146="common", 4, IF(B146="uncommon", 3, IF(B146="rare", 1.74127216869152, 1)))</f>
@@ -4194,17 +4200,17 @@
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C147" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D147" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>2.19</v>
+        <v>2.01</v>
       </c>
       <c r="F147" s="3">
         <f>IF(B147="common", 4, IF(B147="uncommon", 3, IF(B147="rare", 1.74127216869152, 1)))</f>
@@ -4219,7 +4225,7 @@
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C148" s="3" t="n">
@@ -4229,7 +4235,7 @@
         <v>0.09</v>
       </c>
       <c r="E148" s="3" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="F148" s="3">
         <f>IF(B148="common", 4, IF(B148="uncommon", 3, IF(B148="rare", 1.74127216869152, 1)))</f>
@@ -4244,7 +4250,7 @@
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C149" s="3" t="n">
@@ -4254,7 +4260,7 @@
         <v>0.1</v>
       </c>
       <c r="E149" s="3" t="n">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="F149" s="3">
         <f>IF(B149="common", 4, IF(B149="uncommon", 3, IF(B149="rare", 1.74127216869152, 1)))</f>
@@ -4269,14 +4275,14 @@
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C150" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D150" s="3" t="n">
-        <v>28.89</v>
+        <v>28.78</v>
       </c>
       <c r="E150" s="3" t="inlineStr"/>
       <c r="F150" s="3">
@@ -4292,17 +4298,17 @@
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C151" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D151" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>1.65</v>
+        <v>1.61</v>
       </c>
       <c r="F151" s="3">
         <f>IF(B151="common", 4, IF(B151="uncommon", 3, IF(B151="rare", 1.74127216869152, 1)))</f>
@@ -4317,7 +4323,7 @@
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C152" s="3" t="n">
@@ -4327,7 +4333,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E152" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F152" s="3">
         <f>IF(B152="common", 4, IF(B152="uncommon", 3, IF(B152="rare", 1.74127216869152, 1)))</f>
@@ -4342,17 +4348,17 @@
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C153" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D153" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>1.14</v>
+        <v>1.24</v>
       </c>
       <c r="F153" s="3">
         <f>IF(B153="common", 4, IF(B153="uncommon", 3, IF(B153="rare", 1.74127216869152, 1)))</f>
@@ -4367,14 +4373,14 @@
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C154" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D154" s="3" t="n">
-        <v>18.96</v>
+        <v>19.64</v>
       </c>
       <c r="E154" s="3" t="inlineStr"/>
       <c r="F154" s="3">
@@ -4390,7 +4396,7 @@
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C155" s="3" t="n">
@@ -4415,7 +4421,7 @@
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C156" s="3" t="n">
@@ -4425,7 +4431,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E156" s="3" t="n">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="F156" s="3">
         <f>IF(B156="common", 4, IF(B156="uncommon", 3, IF(B156="rare", 1.74127216869152, 1)))</f>
@@ -4440,14 +4446,14 @@
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C157" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D157" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E157" s="3" t="n">
         <v>0.17</v>
@@ -4465,7 +4471,7 @@
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C158" s="3" t="n">
@@ -4475,7 +4481,7 @@
         <v>0.09</v>
       </c>
       <c r="E158" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F158" s="3">
         <f>IF(B158="common", 4, IF(B158="uncommon", 3, IF(B158="rare", 1.74127216869152, 1)))</f>
@@ -4490,17 +4496,17 @@
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C159" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D159" s="3" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="F159" s="3">
         <f>IF(B159="common", 4, IF(B159="uncommon", 3, IF(B159="rare", 1.74127216869152, 1)))</f>
@@ -4515,7 +4521,7 @@
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C160" s="3" t="n">
@@ -4540,14 +4546,14 @@
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C161" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D161" s="3" t="n">
-        <v>21.1</v>
+        <v>20.45</v>
       </c>
       <c r="E161" s="3" t="inlineStr"/>
       <c r="F161" s="3">
@@ -4563,17 +4569,17 @@
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C162" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D162" s="3" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="E162" s="3" t="n">
-        <v>0.86</v>
+        <v>0.83</v>
       </c>
       <c r="F162" s="3">
         <f>IF(B162="common", 4, IF(B162="uncommon", 3, IF(B162="rare", 1.74127216869152, 1)))</f>
@@ -4588,7 +4594,7 @@
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C163" s="3" t="n">
@@ -4598,7 +4604,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F163" s="3">
         <f>IF(B163="common", 4, IF(B163="uncommon", 3, IF(B163="rare", 1.74127216869152, 1)))</f>
@@ -4613,7 +4619,7 @@
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C164" s="3" t="n">
@@ -4638,7 +4644,7 @@
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C165" s="3" t="n">
@@ -4648,7 +4654,7 @@
         <v>0.06</v>
       </c>
       <c r="E165" s="3" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="F165" s="3">
         <f>IF(B165="common", 4, IF(B165="uncommon", 3, IF(B165="rare", 1.74127216869152, 1)))</f>
@@ -4663,17 +4669,17 @@
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C166" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D166" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E166" s="3" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="F166" s="3">
         <f>IF(B166="common", 4, IF(B166="uncommon", 3, IF(B166="rare", 1.74127216869152, 1)))</f>
@@ -4688,7 +4694,7 @@
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C167" s="3" t="n">
@@ -4698,7 +4704,7 @@
         <v>0.06</v>
       </c>
       <c r="E167" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F167" s="3">
         <f>IF(B167="common", 4, IF(B167="uncommon", 3, IF(B167="rare", 1.74127216869152, 1)))</f>
@@ -4713,17 +4719,17 @@
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C168" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D168" s="3" t="n">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="E168" s="3" t="n">
-        <v>1.08</v>
+        <v>1.05</v>
       </c>
       <c r="F168" s="3">
         <f>IF(B168="common", 4, IF(B168="uncommon", 3, IF(B168="rare", 1.74127216869152, 1)))</f>
@@ -4738,17 +4744,17 @@
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C169" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D169" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E169" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F169" s="3">
         <f>IF(B169="common", 4, IF(B169="uncommon", 3, IF(B169="rare", 1.74127216869152, 1)))</f>
@@ -4763,7 +4769,7 @@
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C170" s="3" t="n">
@@ -4773,7 +4779,7 @@
         <v>0.08</v>
       </c>
       <c r="E170" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F170" s="3">
         <f>IF(B170="common", 4, IF(B170="uncommon", 3, IF(B170="rare", 1.74127216869152, 1)))</f>
@@ -4788,7 +4794,7 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C171" s="3" t="n">
@@ -4798,7 +4804,7 @@
         <v>0.11</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>2.4</v>
+        <v>2.25</v>
       </c>
       <c r="F171" s="3">
         <f>IF(B171="common", 4, IF(B171="uncommon", 3, IF(B171="rare", 1.74127216869152, 1)))</f>
@@ -4813,7 +4819,7 @@
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C172" s="3" t="n">
@@ -4823,7 +4829,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E172" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F172" s="3">
         <f>IF(B172="common", 4, IF(B172="uncommon", 3, IF(B172="rare", 1.74127216869152, 1)))</f>
@@ -4838,7 +4844,7 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C173" s="3" t="n">
@@ -4863,7 +4869,7 @@
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C174" s="3" t="n">
@@ -4888,7 +4894,7 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C175" s="3" t="n">
@@ -4898,7 +4904,7 @@
         <v>0.06</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F175" s="3">
         <f>IF(B175="common", 4, IF(B175="uncommon", 3, IF(B175="rare", 1.74127216869152, 1)))</f>
@@ -4913,7 +4919,7 @@
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C176" s="3" t="n">
@@ -4938,7 +4944,7 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C177" s="3" t="n">
@@ -4948,7 +4954,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="F177" s="3">
         <f>IF(B177="common", 4, IF(B177="uncommon", 3, IF(B177="rare", 1.74127216869152, 1)))</f>
@@ -4963,7 +4969,7 @@
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C178" s="3" t="n">
@@ -4973,7 +4979,7 @@
         <v>0.16</v>
       </c>
       <c r="E178" s="3" t="n">
-        <v>1.27</v>
+        <v>1.31</v>
       </c>
       <c r="F178" s="3">
         <f>IF(B178="common", 4, IF(B178="uncommon", 3, IF(B178="rare", 1.74127216869152, 1)))</f>
@@ -4988,7 +4994,7 @@
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C179" s="3" t="n">
@@ -4998,7 +5004,7 @@
         <v>0.06</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="F179" s="3">
         <f>IF(B179="common", 4, IF(B179="uncommon", 3, IF(B179="rare", 1.74127216869152, 1)))</f>
@@ -5013,7 +5019,7 @@
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C180" s="3" t="n">
@@ -5023,7 +5029,7 @@
         <v>0.11</v>
       </c>
       <c r="E180" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="F180" s="3">
         <f>IF(B180="common", 4, IF(B180="uncommon", 3, IF(B180="rare", 1.74127216869152, 1)))</f>
@@ -5038,14 +5044,14 @@
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C181" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D181" s="3" t="n">
-        <v>46.05</v>
+        <v>45.09</v>
       </c>
       <c r="E181" s="3" t="inlineStr"/>
       <c r="F181" s="3">
@@ -5061,17 +5067,17 @@
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C182" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D182" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="E182" s="3" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="F182" s="3">
         <f>IF(B182="common", 4, IF(B182="uncommon", 3, IF(B182="rare", 1.74127216869152, 1)))</f>
@@ -5086,7 +5092,7 @@
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C183" s="3" t="n">
@@ -5111,14 +5117,14 @@
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Hyper Rare</t>
+          <t>hyper rare</t>
         </is>
       </c>
       <c r="C184" s="3" t="n">
         <v>154</v>
       </c>
       <c r="D184" s="3" t="n">
-        <v>2.56</v>
+        <v>2.93</v>
       </c>
       <c r="E184" s="3" t="inlineStr"/>
       <c r="F184" s="3">
@@ -5134,17 +5140,17 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C185" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D185" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E185" s="3" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="F185" s="3">
         <f>IF(B185="common", 4, IF(B185="uncommon", 3, IF(B185="rare", 1.74127216869152, 1)))</f>
@@ -5159,14 +5165,14 @@
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C186" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D186" s="3" t="n">
-        <v>7.68</v>
+        <v>7.56</v>
       </c>
       <c r="E186" s="3" t="inlineStr"/>
       <c r="F186" s="3">
@@ -5182,17 +5188,17 @@
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C187" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D187" s="3" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="F187" s="3">
         <f>IF(B187="common", 4, IF(B187="uncommon", 3, IF(B187="rare", 1.74127216869152, 1)))</f>
@@ -5207,7 +5213,7 @@
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C188" s="3" t="n">
@@ -5217,7 +5223,7 @@
         <v>0.06</v>
       </c>
       <c r="E188" s="3" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="F188" s="3">
         <f>IF(B188="common", 4, IF(B188="uncommon", 3, IF(B188="rare", 1.74127216869152, 1)))</f>
@@ -5232,7 +5238,7 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C189" s="3" t="n">
@@ -5257,17 +5263,17 @@
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C190" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D190" s="3" t="n">
-        <v>0.28</v>
+        <v>0.25</v>
       </c>
       <c r="E190" s="3" t="n">
-        <v>1.28</v>
+        <v>1.25</v>
       </c>
       <c r="F190" s="3">
         <f>IF(B190="common", 4, IF(B190="uncommon", 3, IF(B190="rare", 1.74127216869152, 1)))</f>
@@ -5282,7 +5288,7 @@
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C191" s="3" t="n">
@@ -5292,7 +5298,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="F191" s="3">
         <f>IF(B191="common", 4, IF(B191="uncommon", 3, IF(B191="rare", 1.74127216869152, 1)))</f>
@@ -5307,7 +5313,7 @@
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C192" s="3" t="n">
@@ -5332,14 +5338,14 @@
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C193" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D193" s="3" t="n">
-        <v>0.77</v>
+        <v>0.95</v>
       </c>
       <c r="E193" s="3" t="inlineStr"/>
       <c r="F193" s="3">
@@ -5355,14 +5361,14 @@
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C194" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D194" s="3" t="n">
-        <v>11.82</v>
+        <v>11.58</v>
       </c>
       <c r="E194" s="3" t="inlineStr"/>
       <c r="F194" s="3">
@@ -5378,14 +5384,14 @@
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C195" s="3" t="n">
         <v>225</v>
       </c>
       <c r="D195" s="3" t="n">
-        <v>68.69</v>
+        <v>67.88</v>
       </c>
       <c r="E195" s="3" t="inlineStr"/>
       <c r="F195" s="3">
@@ -5401,7 +5407,7 @@
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C196" s="3" t="n">
@@ -5411,7 +5417,7 @@
         <v>0.05</v>
       </c>
       <c r="E196" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F196" s="3">
         <f>IF(B196="common", 4, IF(B196="uncommon", 3, IF(B196="rare", 1.74127216869152, 1)))</f>
@@ -5426,17 +5432,17 @@
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C197" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D197" s="3" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="E197" s="3" t="n">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
       <c r="F197" s="3">
         <f>IF(B197="common", 4, IF(B197="uncommon", 3, IF(B197="rare", 1.74127216869152, 1)))</f>
@@ -5451,7 +5457,7 @@
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C198" s="3" t="n">
@@ -5461,7 +5467,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E198" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F198" s="3">
         <f>IF(B198="common", 4, IF(B198="uncommon", 3, IF(B198="rare", 1.74127216869152, 1)))</f>
@@ -5476,7 +5482,7 @@
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C199" s="3" t="n">
@@ -5486,7 +5492,7 @@
         <v>0.09</v>
       </c>
       <c r="E199" s="3" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="F199" s="3">
         <f>IF(B199="common", 4, IF(B199="uncommon", 3, IF(B199="rare", 1.74127216869152, 1)))</f>
@@ -5501,17 +5507,17 @@
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Uncommon</t>
+          <t>uncommon</t>
         </is>
       </c>
       <c r="C200" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D200" s="3" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="E200" s="3" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="F200" s="3">
         <f>IF(B200="common", 4, IF(B200="uncommon", 3, IF(B200="rare", 1.74127216869152, 1)))</f>
@@ -5526,14 +5532,14 @@
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Illustration Rare</t>
+          <t>illustration rare</t>
         </is>
       </c>
       <c r="C201" s="3" t="n">
         <v>188</v>
       </c>
       <c r="D201" s="3" t="n">
-        <v>30.34</v>
+        <v>29.96</v>
       </c>
       <c r="E201" s="3" t="inlineStr"/>
       <c r="F201" s="3">
@@ -5549,7 +5555,7 @@
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C202" s="3" t="n">
@@ -5559,7 +5565,7 @@
         <v>0.06</v>
       </c>
       <c r="E202" s="3" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="F202" s="3">
         <f>IF(B202="common", 4, IF(B202="uncommon", 3, IF(B202="rare", 1.74127216869152, 1)))</f>
@@ -5574,17 +5580,17 @@
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C203" s="3" t="n">
         <v>46</v>
       </c>
       <c r="D203" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E203" s="3" t="n">
-        <v>1.51</v>
+        <v>1.54</v>
       </c>
       <c r="F203" s="3">
         <f>IF(B203="common", 4, IF(B203="uncommon", 3, IF(B203="rare", 1.74127216869152, 1)))</f>
@@ -5599,17 +5605,17 @@
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C204" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D204" s="3" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="E204" s="3" t="n">
-        <v>0.58</v>
+        <v>0.57</v>
       </c>
       <c r="F204" s="3">
         <f>IF(B204="common", 4, IF(B204="uncommon", 3, IF(B204="rare", 1.74127216869152, 1)))</f>
@@ -5624,14 +5630,14 @@
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C205" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D205" s="3" t="n">
-        <v>0.77</v>
+        <v>0.84</v>
       </c>
       <c r="E205" s="3" t="inlineStr"/>
       <c r="F205" s="3">
@@ -5647,14 +5653,14 @@
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C206" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D206" s="3" t="n">
-        <v>7.9</v>
+        <v>7.25</v>
       </c>
       <c r="E206" s="3" t="inlineStr"/>
       <c r="F206" s="3">
@@ -5670,14 +5676,14 @@
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C207" s="3" t="n">
         <v>90</v>
       </c>
       <c r="D207" s="3" t="n">
-        <v>0.71</v>
+        <v>0.77</v>
       </c>
       <c r="E207" s="3" t="inlineStr"/>
       <c r="F207" s="3">
@@ -5693,14 +5699,14 @@
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C208" s="3" t="n">
         <v>248</v>
       </c>
       <c r="D208" s="3" t="n">
-        <v>8.06</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="E208" s="3" t="inlineStr"/>
       <c r="F208" s="3">
@@ -5716,14 +5722,14 @@
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C209" s="3" t="n">
         <v>225</v>
       </c>
       <c r="D209" s="3" t="n">
-        <v>55.36</v>
+        <v>55.64</v>
       </c>
       <c r="E209" s="3" t="inlineStr"/>
       <c r="F209" s="3">
@@ -5739,7 +5745,7 @@
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C210" s="3" t="n">
@@ -5764,7 +5770,7 @@
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>rare</t>
         </is>
       </c>
       <c r="C211" s="3" t="n">
@@ -5789,7 +5795,7 @@
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C212" s="3" t="n">
@@ -5812,7 +5818,7 @@
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C213" s="3" t="n">
@@ -5835,7 +5841,7 @@
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Double Rare</t>
+          <t>double rare</t>
         </is>
       </c>
       <c r="C214" s="3" t="n">
@@ -5858,7 +5864,7 @@
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Ultra Rare</t>
+          <t>ultra rare</t>
         </is>
       </c>
       <c r="C215" s="3" t="n">
@@ -5881,7 +5887,7 @@
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Special Illustration Rare</t>
+          <t>special illustration rare</t>
         </is>
       </c>
       <c r="C216" s="3" t="n">
@@ -5904,7 +5910,7 @@
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>common</t>
         </is>
       </c>
       <c r="C217" s="3" t="n">
@@ -12489,225 +12495,225 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>Metric</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>ev_common_total</t>
         </is>
       </c>
-      <c r="B2" s="11" t="n">
-        <v>0.1123913043478261</v>
+      <c r="B2" s="12" t="n">
+        <v>0.451304347826087</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="inlineStr">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>ev_uncommon_total</t>
         </is>
       </c>
-      <c r="B3" s="11" t="n">
-        <v>0.1696969696969697</v>
+      <c r="B3" s="12" t="n">
+        <v>0.5090909090909091</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="11" t="inlineStr">
         <is>
           <t>ev_rare_total</t>
         </is>
       </c>
-      <c r="B4" s="11" t="n">
-        <v>0.2695238095238095</v>
+      <c r="B4" s="12" t="n">
+        <v>0.213703314659197</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>ev_reverse_total</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="n">
+        <v>5.313106295878034</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>ev_ace_spec_total</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="inlineStr">
+        <is>
+          <t>ev_pokeball_total</t>
+        </is>
+      </c>
+      <c r="B7" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="inlineStr">
+        <is>
+          <t>ev_master_ball_total</t>
+        </is>
+      </c>
+      <c r="B8" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>ev_IR_total</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="n">
+        <v>1.96968085106383</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="inlineStr">
+        <is>
+          <t>ev_SIR_total</t>
+        </is>
+      </c>
+      <c r="B10" s="12" t="n">
+        <v>2.372933333333333</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="inlineStr">
         <is>
           <t>ev_double_rare_total</t>
         </is>
       </c>
-      <c r="B5" s="11" t="n">
-        <v>0.3478888888888889</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="10" t="inlineStr">
-        <is>
-          <t>ev_pokeball_total</t>
-        </is>
-      </c>
-      <c r="B6" s="11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="10" t="inlineStr">
-        <is>
-          <t>ev_master_ball_total</t>
-        </is>
-      </c>
-      <c r="B7" s="11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="B11" s="12" t="n">
+        <v>0.3439999999999999</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="inlineStr">
         <is>
           <t>ev_hyper_rare_total</t>
         </is>
       </c>
-      <c r="B8" s="11" t="n">
-        <v>0.1349350649350649</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="10" t="inlineStr">
+      <c r="B12" s="12" t="n">
+        <v>0.1366233766233766</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="inlineStr">
         <is>
           <t>ev_ultra_rare_total</t>
         </is>
       </c>
-      <c r="B9" s="11" t="n">
-        <v>0.6597580645161291</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="10" t="inlineStr">
-        <is>
-          <t>ev_SIR_total</t>
-        </is>
-      </c>
-      <c r="B10" s="11" t="n">
-        <v>2.366622222222222</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="10" t="inlineStr">
-        <is>
-          <t>ev_IR_total</t>
-        </is>
-      </c>
-      <c r="B11" s="11" t="n">
-        <v>1.987606382978723</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="10" t="inlineStr">
-        <is>
-          <t>ev_reverse_total</t>
-        </is>
-      </c>
-      <c r="B12" s="11" t="n">
-        <v>2.824572746094485</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="10" t="inlineStr">
+      <c r="B13" s="12" t="n">
+        <v>0.6449596774193548</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>reverse_multiplier</t>
         </is>
       </c>
-      <c r="B13" s="11" t="n">
-        <v>1.879338061465721</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="10" t="inlineStr">
+      <c r="B14" s="11" t="n">
+        <v>1.885416666666667</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="inlineStr">
         <is>
           <t>rare_multiplier</t>
         </is>
       </c>
-      <c r="B14" s="10" t="n">
-        <v>1.741272168691524</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="10" t="inlineStr">
-        <is>
-          <t>ev_total_for_hits</t>
-        </is>
-      </c>
       <c r="B15" s="11" t="n">
-        <v>5.14892173465214</v>
+        <v>0.7928921568627451</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="inlineStr">
+      <c r="A16" s="11" t="inlineStr">
         <is>
           <t>ev_hits_total</t>
         </is>
       </c>
-      <c r="B16" s="11" t="n">
-        <v>5.496810623541029</v>
+      <c r="B16" s="12" t="n">
+        <v>5.468197238439894</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="inlineStr">
+      <c r="A17" s="11" t="inlineStr">
         <is>
           <t>total_ev</t>
         </is>
       </c>
-      <c r="B17" s="11" t="n">
-        <v>11.07690299510566</v>
+      <c r="B17" s="12" t="n">
+        <v>11.95540210589412</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="inlineStr">
+      <c r="A18" s="11" t="inlineStr">
         <is>
           <t>net_value</t>
         </is>
       </c>
-      <c r="B18" s="11" t="n">
-        <v>0.1869029951056582</v>
+      <c r="B18" s="12" t="n">
+        <v>1.065402105894121</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="inlineStr">
+      <c r="A19" s="11" t="inlineStr">
         <is>
           <t>roi</t>
         </is>
       </c>
-      <c r="B19" s="12" t="n">
-        <v>0.01716280946792081</v>
+      <c r="B19" s="13" t="n">
+        <v>1.097833067575218</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="inlineStr">
+      <c r="A20" s="11" t="inlineStr">
         <is>
           <t>roi_percent</t>
         </is>
       </c>
-      <c r="B20" s="12" t="n">
-        <v>0.7162809467920814</v>
+      <c r="B20" s="14" t="n">
+        <v>0.09783306757521772</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="inlineStr">
+      <c r="A21" s="11" t="inlineStr">
         <is>
           <t>no_hit_probability_percentage</t>
         </is>
       </c>
-      <c r="B21" s="12" t="n">
-        <v>68.32877110235633</v>
+      <c r="B21" s="14" t="n">
+        <v>0.6832877110235632</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="inlineStr">
+      <c r="A22" s="11" t="inlineStr">
         <is>
           <t>hit_probability_percentage</t>
         </is>
       </c>
-      <c r="B22" s="12" t="n">
-        <v>31.67122889764367</v>
+      <c r="B22" s="14" t="n">
+        <v>0.3167122889764367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major refractoring for scaling
</commit_message>
<xml_diff>
--- a/Expected Value and Cost Ratio Calculator Pokemon/excelDocs/scarletAndViolet151/pokemon_data.xlsx
+++ b/Expected Value and Cost Ratio Calculator Pokemon/excelDocs/scarletAndViolet151/pokemon_data.xlsx
@@ -667,7 +667,7 @@
         <v>0.06</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="F2" s="3">
         <f>IF(B2:B210="common", 4, IF(B2:B210="uncommon", 3, IF(B2:B210="rare", 0.792892156862745, 1)))</f>
@@ -682,20 +682,20 @@
         <v/>
       </c>
       <c r="I2" s="3" t="n">
-        <v>9.73</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>65.38</v>
+        <v>65.62</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>232.49</v>
+        <v>232.98</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>5.93</v>
+        <v>6.19</v>
       </c>
       <c r="M2" s="3" t="n"/>
       <c r="N2" s="3" t="n">
-        <v>372.1</v>
+        <v>372.92</v>
       </c>
       <c r="R2" s="3" t="n"/>
       <c r="S2" s="3" t="n"/>
@@ -733,10 +733,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.64</v>
+        <v>0.59</v>
       </c>
       <c r="F3" s="3">
         <f>IF(B3:B211="common", 4, IF(B3:B211="uncommon", 3, IF(B3:B211="rare", 0.792892156862745, 1)))</f>
@@ -843,7 +843,7 @@
         <v>248</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>7.41</v>
+        <v>7.01</v>
       </c>
       <c r="E5" s="3" t="inlineStr"/>
       <c r="F5" s="3">
@@ -897,7 +897,7 @@
         <v>225</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>36.43</v>
+        <v>36.5</v>
       </c>
       <c r="E6" s="3" t="inlineStr"/>
       <c r="F6" s="3">
@@ -951,7 +951,7 @@
         <v>46</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>0.58</v>
@@ -1007,10 +1007,10 @@
         <v>46</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="F8" s="3">
         <f>IF(B8:B216="common", 4, IF(B8:B216="uncommon", 3, IF(B8:B216="rare", 0.792892156862745, 1)))</f>
@@ -1063,10 +1063,10 @@
         <v>46</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
       <c r="F9" s="3">
         <f>IF(B9:B217="common", 4, IF(B9:B217="uncommon", 3, IF(B9:B217="rare", 0.792892156862745, 1)))</f>
@@ -1119,7 +1119,7 @@
         <v>90</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="E10" s="3" t="inlineStr"/>
       <c r="F10" s="3">
@@ -1173,7 +1173,7 @@
         <v>248</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>5.38</v>
+        <v>4.77</v>
       </c>
       <c r="E11" s="3" t="inlineStr"/>
       <c r="F11" s="3">
@@ -1227,7 +1227,7 @@
         <v>0.06</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="F12" s="3">
         <f>IF(B12:B220="common", 4, IF(B12:B220="uncommon", 3, IF(B12:B220="rare", 0.792892156862745, 1)))</f>
@@ -1277,10 +1277,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>1.1</v>
+        <v>0.96</v>
       </c>
       <c r="F13" s="3">
         <f>IF(B13:B221="common", 4, IF(B13:B221="uncommon", 3, IF(B13:B221="rare", 0.792892156862745, 1)))</f>
@@ -1330,7 +1330,7 @@
         <v>154</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>4.61</v>
+        <v>4.45</v>
       </c>
       <c r="E14" s="3" t="inlineStr"/>
       <c r="F14" s="3">
@@ -1381,10 +1381,10 @@
         <v>21</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>0.76</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F15" s="3">
         <f>IF(B15:B223="common", 4, IF(B15:B223="uncommon", 3, IF(B15:B223="rare", 0.792892156862745, 1)))</f>
@@ -1434,7 +1434,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>0.11</v>
@@ -1490,7 +1490,7 @@
         <v>0.09</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.83</v>
+        <v>0.79</v>
       </c>
       <c r="F17" s="3">
         <f>IF(B17:B225="common", 4, IF(B17:B225="uncommon", 3, IF(B17:B225="rare", 0.792892156862745, 1)))</f>
@@ -1543,7 +1543,7 @@
         <v>0.11</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0.47</v>
+        <v>0.38</v>
       </c>
       <c r="F18" s="3">
         <f>IF(B18:B226="common", 4, IF(B18:B226="uncommon", 3, IF(B18:B226="rare", 0.792892156862745, 1)))</f>
@@ -1593,7 +1593,7 @@
         <v>248</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>3.06</v>
+        <v>2.85</v>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
       <c r="F19" s="3">
@@ -1644,7 +1644,7 @@
         <v>90</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="E20" s="3" t="inlineStr"/>
       <c r="F20" s="3">
@@ -1695,7 +1695,7 @@
         <v>248</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>13.25</v>
+        <v>13.09</v>
       </c>
       <c r="E21" s="3" t="inlineStr"/>
       <c r="F21" s="3">
@@ -1746,7 +1746,7 @@
         <v>225</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>65.98</v>
+        <v>65.44</v>
       </c>
       <c r="E22" s="3" t="inlineStr"/>
       <c r="F22" s="3">
@@ -1797,10 +1797,10 @@
         <v>46</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="F23" s="3">
         <f>IF(B23:B231="common", 4, IF(B23:B231="uncommon", 3, IF(B23:B231="rare", 0.792892156862745, 1)))</f>
@@ -1850,7 +1850,7 @@
         <v>188</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>33.97</v>
+        <v>34.54</v>
       </c>
       <c r="E24" s="3" t="inlineStr"/>
       <c r="F24" s="3">
@@ -1901,7 +1901,7 @@
         <v>33</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>0.14</v>
@@ -1954,10 +1954,10 @@
         <v>46</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="F26" s="3">
         <f>IF(B26:B234="common", 4, IF(B26:B234="uncommon", 3, IF(B26:B234="rare", 0.792892156862745, 1)))</f>
@@ -2007,7 +2007,7 @@
         <v>188</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>7.77</v>
+        <v>7.19</v>
       </c>
       <c r="E27" s="3" t="inlineStr"/>
       <c r="F27" s="3">
@@ -2061,7 +2061,7 @@
         <v>0.18</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>0.91</v>
+        <v>0.87</v>
       </c>
       <c r="F28" s="3">
         <f>IF(B28:B236="common", 4, IF(B28:B236="uncommon", 3, IF(B28:B236="rare", 0.792892156862745, 1)))</f>
@@ -2111,7 +2111,7 @@
         <v>90</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>3.86</v>
+        <v>4.25</v>
       </c>
       <c r="E29" s="3" t="inlineStr"/>
       <c r="F29" s="3">
@@ -2162,7 +2162,7 @@
         <v>248</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>25.18</v>
+        <v>26.9</v>
       </c>
       <c r="E30" s="3" t="inlineStr"/>
       <c r="F30" s="3">
@@ -2213,7 +2213,7 @@
         <v>225</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>206.26</v>
+        <v>198.4</v>
       </c>
       <c r="E31" s="3" t="inlineStr"/>
       <c r="F31" s="3">
@@ -2264,10 +2264,10 @@
         <v>46</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="F32" s="3">
         <f>IF(B32:B240="common", 4, IF(B32:B240="uncommon", 3, IF(B32:B240="rare", 0.792892156862745, 1)))</f>
@@ -2317,7 +2317,7 @@
         <v>188</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>42.53</v>
+        <v>42.66</v>
       </c>
       <c r="E33" s="3" t="inlineStr"/>
       <c r="F33" s="3">
@@ -2368,10 +2368,10 @@
         <v>33</v>
       </c>
       <c r="D34" s="3" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="F34" s="3">
         <f>IF(B34:B242="common", 4, IF(B34:B242="uncommon", 3, IF(B34:B242="rare", 0.792892156862745, 1)))</f>
@@ -2421,7 +2421,7 @@
         <v>188</v>
       </c>
       <c r="D35" s="3" t="n">
-        <v>32.92</v>
+        <v>32.18</v>
       </c>
       <c r="E35" s="3" t="inlineStr"/>
       <c r="F35" s="3">
@@ -2472,10 +2472,10 @@
         <v>33</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E36" s="3" t="n">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
       <c r="F36" s="3">
         <f>IF(B36:B244="common", 4, IF(B36:B244="uncommon", 3, IF(B36:B244="rare", 0.792892156862745, 1)))</f>
@@ -2525,7 +2525,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E37" s="3" t="n">
         <v>0.13</v>
@@ -2578,7 +2578,7 @@
         <v>33</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>0.18</v>
@@ -2631,10 +2631,10 @@
         <v>46</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="F39" s="3">
         <f>IF(B39:B247="common", 4, IF(B39:B247="uncommon", 3, IF(B39:B247="rare", 0.792892156862745, 1)))</f>
@@ -2687,7 +2687,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E40" s="3" t="n">
-        <v>0.62</v>
+        <v>0.66</v>
       </c>
       <c r="F40" s="3">
         <f>IF(B40:B248="common", 4, IF(B40:B248="uncommon", 3, IF(B40:B248="rare", 0.792892156862745, 1)))</f>
@@ -2740,7 +2740,7 @@
         <v>0.09</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>0.61</v>
+        <v>0.64</v>
       </c>
       <c r="F41" s="3">
         <f>IF(B41:B249="common", 4, IF(B41:B249="uncommon", 3, IF(B41:B249="rare", 0.792892156862745, 1)))</f>
@@ -2790,7 +2790,7 @@
         <v>248</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>3.18</v>
+        <v>3.26</v>
       </c>
       <c r="E42" s="3" t="inlineStr"/>
       <c r="F42" s="3">
@@ -2841,10 +2841,10 @@
         <v>33</v>
       </c>
       <c r="D43" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="F43" s="3">
         <f>IF(B43:B251="common", 4, IF(B43:B251="uncommon", 3, IF(B43:B251="rare", 0.792892156862745, 1)))</f>
@@ -2894,7 +2894,7 @@
         <v>46</v>
       </c>
       <c r="D44" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E44" s="3" t="n">
         <v>0.14</v>
@@ -2947,10 +2947,10 @@
         <v>21</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>0.28</v>
+        <v>0.32</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="F45" s="3">
         <f>IF(B45:B253="common", 4, IF(B45:B253="uncommon", 3, IF(B45:B253="rare", 0.792892156862745, 1)))</f>
@@ -3000,7 +3000,7 @@
         <v>21</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="E46" s="3" t="inlineStr"/>
       <c r="F46" s="3">
@@ -3051,10 +3051,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="F47" s="3">
         <f>IF(B47:B255="common", 4, IF(B47:B255="uncommon", 3, IF(B47:B255="rare", 0.792892156862745, 1)))</f>
@@ -3104,10 +3104,10 @@
         <v>46</v>
       </c>
       <c r="D48" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E48" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F48" s="3">
         <f>IF(B48:B256="common", 4, IF(B48:B256="uncommon", 3, IF(B48:B256="rare", 0.792892156862745, 1)))</f>
@@ -3157,10 +3157,10 @@
         <v>33</v>
       </c>
       <c r="D49" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>1.75</v>
+        <v>1.67</v>
       </c>
       <c r="F49" s="3">
         <f>IF(B49:B257="common", 4, IF(B49:B257="uncommon", 3, IF(B49:B257="rare", 0.792892156862745, 1)))</f>
@@ -3210,7 +3210,7 @@
         <v>188</v>
       </c>
       <c r="D50" s="3" t="n">
-        <v>20.09</v>
+        <v>20.11</v>
       </c>
       <c r="E50" s="3" t="inlineStr"/>
       <c r="F50" s="3">
@@ -3261,10 +3261,10 @@
         <v>21</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>1.41</v>
+        <v>1.37</v>
       </c>
       <c r="F51" s="3">
         <f>IF(B51:B259="common", 4, IF(B51:B259="uncommon", 3, IF(B51:B259="rare", 0.792892156862745, 1)))</f>
@@ -3317,7 +3317,7 @@
         <v>0.1</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F52" s="3">
         <f>IF(B52:B260="common", 4, IF(B52:B260="uncommon", 3, IF(B52:B260="rare", 0.792892156862745, 1)))</f>
@@ -3367,10 +3367,10 @@
         <v>46</v>
       </c>
       <c r="D53" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F53" s="3">
         <f>IF(B53:B261="common", 4, IF(B53:B261="uncommon", 3, IF(B53:B261="rare", 0.792892156862745, 1)))</f>
@@ -3420,10 +3420,10 @@
         <v>33</v>
       </c>
       <c r="D54" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>0.14</v>
+        <v>0.2</v>
       </c>
       <c r="F54" s="3">
         <f>IF(B54:B262="common", 4, IF(B54:B262="uncommon", 3, IF(B54:B262="rare", 0.792892156862745, 1)))</f>
@@ -3476,7 +3476,7 @@
         <v>0.12</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="F55" s="3">
         <f>IF(B55:B263="common", 4, IF(B55:B263="uncommon", 3, IF(B55:B263="rare", 0.792892156862745, 1)))</f>
@@ -3529,7 +3529,7 @@
         <v>0.06</v>
       </c>
       <c r="E56" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F56" s="3">
         <f>IF(B56:B264="common", 4, IF(B56:B264="uncommon", 3, IF(B56:B264="rare", 0.792892156862745, 1)))</f>
@@ -3632,10 +3632,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="E58" s="3" t="n">
-        <v>1.18</v>
+        <v>1.16</v>
       </c>
       <c r="F58" s="3">
         <f>IF(B58:B266="common", 4, IF(B58:B266="uncommon", 3, IF(B58:B266="rare", 0.792892156862745, 1)))</f>
@@ -3685,10 +3685,10 @@
         <v>33</v>
       </c>
       <c r="D59" s="3" t="n">
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>1.28</v>
+        <v>1.14</v>
       </c>
       <c r="F59" s="3">
         <f>IF(B59:B267="common", 4, IF(B59:B267="uncommon", 3, IF(B59:B267="rare", 0.792892156862745, 1)))</f>
@@ -3791,7 +3791,7 @@
         <v>248</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>5.88</v>
+        <v>5.56</v>
       </c>
       <c r="E61" s="3" t="inlineStr"/>
       <c r="F61" s="3">
@@ -3842,7 +3842,7 @@
         <v>225</v>
       </c>
       <c r="D62" s="3" t="n">
-        <v>13.84</v>
+        <v>13.57</v>
       </c>
       <c r="E62" s="3" t="inlineStr"/>
       <c r="F62" s="3">
@@ -3893,10 +3893,10 @@
         <v>46</v>
       </c>
       <c r="D63" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F63" s="3">
         <f>IF(B63:B271="common", 4, IF(B63:B271="uncommon", 3, IF(B63:B271="rare", 0.792892156862745, 1)))</f>
@@ -3946,10 +3946,10 @@
         <v>33</v>
       </c>
       <c r="D64" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E64" s="3" t="n">
-        <v>1.55</v>
+        <v>1.5</v>
       </c>
       <c r="F64" s="3">
         <f>IF(B64:B272="common", 4, IF(B64:B272="uncommon", 3, IF(B64:B272="rare", 0.792892156862745, 1)))</f>
@@ -4002,7 +4002,7 @@
         <v>0.05</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F65" s="3">
         <f>IF(B65:B273="common", 4, IF(B65:B273="uncommon", 3, IF(B65:B273="rare", 0.792892156862745, 1)))</f>
@@ -4052,10 +4052,10 @@
         <v>33</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="F66" s="3">
         <f>IF(B66:B274="common", 4, IF(B66:B274="uncommon", 3, IF(B66:B274="rare", 0.792892156862745, 1)))</f>
@@ -4105,10 +4105,10 @@
         <v>21</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>1.28</v>
+        <v>1.08</v>
       </c>
       <c r="F67" s="3">
         <f>IF(B67:B275="common", 4, IF(B67:B275="uncommon", 3, IF(B67:B275="rare", 0.792892156862745, 1)))</f>
@@ -4161,7 +4161,7 @@
         <v>0.08</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F68" s="3">
         <f>IF(B68:B276="common", 4, IF(B68:B276="uncommon", 3, IF(B68:B276="rare", 0.792892156862745, 1)))</f>
@@ -4211,10 +4211,10 @@
         <v>21</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>1.84</v>
+        <v>2</v>
       </c>
       <c r="F69" s="3">
         <f>IF(B69:B277="common", 4, IF(B69:B277="uncommon", 3, IF(B69:B277="rare", 0.792892156862745, 1)))</f>
@@ -4264,10 +4264,10 @@
         <v>46</v>
       </c>
       <c r="D70" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E70" s="3" t="n">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="F70" s="3">
         <f>IF(B70:B278="common", 4, IF(B70:B278="uncommon", 3, IF(B70:B278="rare", 0.792892156862745, 1)))</f>
@@ -4317,10 +4317,10 @@
         <v>33</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="F71" s="3">
         <f>IF(B71:B279="common", 4, IF(B71:B279="uncommon", 3, IF(B71:B279="rare", 0.792892156862745, 1)))</f>
@@ -4370,7 +4370,7 @@
         <v>248</v>
       </c>
       <c r="D72" s="3" t="n">
-        <v>5.54</v>
+        <v>4.99</v>
       </c>
       <c r="E72" s="3" t="inlineStr"/>
       <c r="F72" s="3">
@@ -4421,7 +4421,7 @@
         <v>225</v>
       </c>
       <c r="D73" s="3" t="n">
-        <v>13.18</v>
+        <v>12.98</v>
       </c>
       <c r="E73" s="3" t="inlineStr"/>
       <c r="F73" s="3">
@@ -4472,10 +4472,10 @@
         <v>33</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="F74" s="3">
         <f>IF(B74:B282="common", 4, IF(B74:B282="uncommon", 3, IF(B74:B282="rare", 0.792892156862745, 1)))</f>
@@ -4631,7 +4631,7 @@
         <v>33</v>
       </c>
       <c r="D77" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E77" s="3" t="n">
         <v>0.16</v>
@@ -4684,7 +4684,7 @@
         <v>90</v>
       </c>
       <c r="D78" s="3" t="n">
-        <v>0.61</v>
+        <v>0.63</v>
       </c>
       <c r="E78" s="3" t="inlineStr"/>
       <c r="F78" s="3">
@@ -4735,7 +4735,7 @@
         <v>248</v>
       </c>
       <c r="D79" s="3" t="n">
-        <v>5.37</v>
+        <v>5.26</v>
       </c>
       <c r="E79" s="3" t="inlineStr"/>
       <c r="F79" s="3">
@@ -4789,7 +4789,7 @@
         <v>0.12</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>0.64</v>
+        <v>0.6</v>
       </c>
       <c r="F80" s="3">
         <f>IF(B80:B288="common", 4, IF(B80:B288="uncommon", 3, IF(B80:B288="rare", 0.792892156862745, 1)))</f>
@@ -4842,7 +4842,7 @@
         <v>0.06</v>
       </c>
       <c r="E81" s="3" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="F81" s="3">
         <f>IF(B81:B289="common", 4, IF(B81:B289="uncommon", 3, IF(B81:B289="rare", 0.792892156862745, 1)))</f>
@@ -4892,10 +4892,10 @@
         <v>46</v>
       </c>
       <c r="D82" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E82" s="3" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="F82" s="3">
         <f>IF(B82:B290="common", 4, IF(B82:B290="uncommon", 3, IF(B82:B290="rare", 0.792892156862745, 1)))</f>
@@ -4948,7 +4948,7 @@
         <v>0.05</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="F83" s="3">
         <f>IF(B83:B291="common", 4, IF(B83:B291="uncommon", 3, IF(B83:B291="rare", 0.792892156862745, 1)))</f>
@@ -4998,10 +4998,10 @@
         <v>21</v>
       </c>
       <c r="D84" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
       <c r="F84" s="3">
         <f>IF(B84:B292="common", 4, IF(B84:B292="uncommon", 3, IF(B84:B292="rare", 0.792892156862745, 1)))</f>
@@ -5051,10 +5051,10 @@
         <v>33</v>
       </c>
       <c r="D85" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="F85" s="3">
         <f>IF(B85:B293="common", 4, IF(B85:B293="uncommon", 3, IF(B85:B293="rare", 0.792892156862745, 1)))</f>
@@ -5107,7 +5107,7 @@
         <v>0.11</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>1.24</v>
+        <v>1.2</v>
       </c>
       <c r="F86" s="3">
         <f>IF(B86:B294="common", 4, IF(B86:B294="uncommon", 3, IF(B86:B294="rare", 0.792892156862745, 1)))</f>
@@ -5157,10 +5157,10 @@
         <v>33</v>
       </c>
       <c r="D87" s="3" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="E87" s="3" t="n">
-        <v>1.16</v>
+        <v>1.22</v>
       </c>
       <c r="F87" s="3">
         <f>IF(B87:B295="common", 4, IF(B87:B295="uncommon", 3, IF(B87:B295="rare", 0.792892156862745, 1)))</f>
@@ -5210,7 +5210,7 @@
         <v>46</v>
       </c>
       <c r="D88" s="3" t="n">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="E88" s="3" t="n">
         <v>0.14</v>
@@ -5263,10 +5263,10 @@
         <v>33</v>
       </c>
       <c r="D89" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>1.18</v>
+        <v>1.05</v>
       </c>
       <c r="F89" s="3">
         <f>IF(B89:B297="common", 4, IF(B89:B297="uncommon", 3, IF(B89:B297="rare", 0.792892156862745, 1)))</f>
@@ -5319,7 +5319,7 @@
         <v>0.1</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>0.33</v>
+        <v>0.28</v>
       </c>
       <c r="F90" s="3">
         <f>IF(B90:B298="common", 4, IF(B90:B298="uncommon", 3, IF(B90:B298="rare", 0.792892156862745, 1)))</f>
@@ -5369,7 +5369,7 @@
         <v>188</v>
       </c>
       <c r="D91" s="3" t="n">
-        <v>27.43</v>
+        <v>27.57</v>
       </c>
       <c r="E91" s="3" t="inlineStr"/>
       <c r="F91" s="3">
@@ -5420,10 +5420,10 @@
         <v>46</v>
       </c>
       <c r="D92" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="F92" s="3">
         <f>IF(B92:B300="common", 4, IF(B92:B300="uncommon", 3, IF(B92:B300="rare", 0.792892156862745, 1)))</f>
@@ -5473,10 +5473,10 @@
         <v>21</v>
       </c>
       <c r="D93" s="3" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="E93" s="3" t="n">
-        <v>2.15</v>
+        <v>2.12</v>
       </c>
       <c r="F93" s="3">
         <f>IF(B93:B301="common", 4, IF(B93:B301="uncommon", 3, IF(B93:B301="rare", 0.792892156862745, 1)))</f>
@@ -5526,7 +5526,7 @@
         <v>90</v>
       </c>
       <c r="D94" s="3" t="n">
-        <v>1.06</v>
+        <v>0.82</v>
       </c>
       <c r="E94" s="3" t="inlineStr"/>
       <c r="F94" s="3">
@@ -5577,7 +5577,7 @@
         <v>248</v>
       </c>
       <c r="D95" s="3" t="n">
-        <v>4.34</v>
+        <v>4.23</v>
       </c>
       <c r="E95" s="3" t="inlineStr"/>
       <c r="F95" s="3">
@@ -5631,7 +5631,7 @@
         <v>0.08</v>
       </c>
       <c r="E96" s="3" t="n">
-        <v>1.3</v>
+        <v>1.26</v>
       </c>
       <c r="F96" s="3">
         <f>IF(B96:B304="common", 4, IF(B96:B304="uncommon", 3, IF(B96:B304="rare", 0.792892156862745, 1)))</f>
@@ -5681,10 +5681,10 @@
         <v>21</v>
       </c>
       <c r="D97" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>1.07</v>
+        <v>0.96</v>
       </c>
       <c r="F97" s="3">
         <f>IF(B97:B305="common", 4, IF(B97:B305="uncommon", 3, IF(B97:B305="rare", 0.792892156862745, 1)))</f>
@@ -5734,10 +5734,10 @@
         <v>33</v>
       </c>
       <c r="D98" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E98" s="3" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="F98" s="3">
         <f>IF(B98:B306="common", 4, IF(B98:B306="uncommon", 3, IF(B98:B306="rare", 0.792892156862745, 1)))</f>
@@ -5787,10 +5787,10 @@
         <v>46</v>
       </c>
       <c r="D99" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E99" s="3" t="n">
-        <v>1.82</v>
+        <v>1.64</v>
       </c>
       <c r="F99" s="3">
         <f>IF(B99:B307="common", 4, IF(B99:B307="uncommon", 3, IF(B99:B307="rare", 0.792892156862745, 1)))</f>
@@ -5840,7 +5840,7 @@
         <v>90</v>
       </c>
       <c r="D100" s="3" t="n">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="E100" s="3" t="inlineStr"/>
       <c r="F100" s="3">
@@ -5891,7 +5891,7 @@
         <v>248</v>
       </c>
       <c r="D101" s="3" t="n">
-        <v>4.81</v>
+        <v>4.89</v>
       </c>
       <c r="E101" s="3" t="inlineStr"/>
       <c r="F101" s="3">
@@ -5942,10 +5942,10 @@
         <v>33</v>
       </c>
       <c r="D102" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E102" s="3" t="n">
-        <v>1.26</v>
+        <v>1.41</v>
       </c>
       <c r="F102" s="3">
         <f>IF(B102:B310="common", 4, IF(B102:B310="uncommon", 3, IF(B102:B310="rare", 0.792892156862745, 1)))</f>
@@ -5995,10 +5995,10 @@
         <v>46</v>
       </c>
       <c r="D103" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E103" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F103" s="3">
         <f>IF(B103:B311="common", 4, IF(B103:B311="uncommon", 3, IF(B103:B311="rare", 0.792892156862745, 1)))</f>
@@ -6048,7 +6048,7 @@
         <v>46</v>
       </c>
       <c r="D104" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E104" s="3" t="n">
         <v>0.16</v>
@@ -6104,7 +6104,7 @@
         <v>0.09</v>
       </c>
       <c r="E105" s="3" t="n">
-        <v>1.49</v>
+        <v>1.28</v>
       </c>
       <c r="F105" s="3">
         <f>IF(B105:B313="common", 4, IF(B105:B313="uncommon", 3, IF(B105:B313="rare", 0.792892156862745, 1)))</f>
@@ -6154,10 +6154,10 @@
         <v>33</v>
       </c>
       <c r="D106" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E106" s="3" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="F106" s="3">
         <f>IF(B106:B314="common", 4, IF(B106:B314="uncommon", 3, IF(B106:B314="rare", 0.792892156862745, 1)))</f>
@@ -6207,7 +6207,7 @@
         <v>46</v>
       </c>
       <c r="D107" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E107" s="3" t="n">
         <v>0.14</v>
@@ -6263,7 +6263,7 @@
         <v>0.18</v>
       </c>
       <c r="E108" s="3" t="n">
-        <v>0.68</v>
+        <v>0.65</v>
       </c>
       <c r="F108" s="3">
         <f>IF(B108:B316="common", 4, IF(B108:B316="uncommon", 3, IF(B108:B316="rare", 0.792892156862745, 1)))</f>
@@ -6313,7 +6313,7 @@
         <v>33</v>
       </c>
       <c r="D109" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E109" s="3" t="n">
         <v>0.17</v>
@@ -6366,7 +6366,7 @@
         <v>188</v>
       </c>
       <c r="D110" s="3" t="n">
-        <v>9.800000000000001</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="E110" s="3" t="inlineStr"/>
       <c r="F110" s="3">
@@ -6420,7 +6420,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F111" s="3">
         <f>IF(B111:B319="common", 4, IF(B111:B319="uncommon", 3, IF(B111:B319="rare", 0.792892156862745, 1)))</f>
@@ -6470,10 +6470,10 @@
         <v>46</v>
       </c>
       <c r="D112" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E112" s="3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="F112" s="3">
         <f>IF(B112:B320="common", 4, IF(B112:B320="uncommon", 3, IF(B112:B320="rare", 0.792892156862745, 1)))</f>
@@ -6523,10 +6523,10 @@
         <v>46</v>
       </c>
       <c r="D113" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E113" s="3" t="n">
-        <v>1.06</v>
+        <v>0.96</v>
       </c>
       <c r="F113" s="3">
         <f>IF(B113:B321="common", 4, IF(B113:B321="uncommon", 3, IF(B113:B321="rare", 0.792892156862745, 1)))</f>
@@ -6576,10 +6576,10 @@
         <v>46</v>
       </c>
       <c r="D114" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E114" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F114" s="3">
         <f>IF(B114:B322="common", 4, IF(B114:B322="uncommon", 3, IF(B114:B322="rare", 0.792892156862745, 1)))</f>
@@ -6632,7 +6632,7 @@
         <v>0.09</v>
       </c>
       <c r="E115" s="3" t="n">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="F115" s="3">
         <f>IF(B115:B323="common", 4, IF(B115:B323="uncommon", 3, IF(B115:B323="rare", 0.792892156862745, 1)))</f>
@@ -6682,7 +6682,7 @@
         <v>46</v>
       </c>
       <c r="D116" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E116" s="3" t="n">
         <v>0.12</v>
@@ -6735,10 +6735,10 @@
         <v>21</v>
       </c>
       <c r="D117" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="E117" s="3" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="F117" s="3">
         <f>IF(B117:B325="common", 4, IF(B117:B325="uncommon", 3, IF(B117:B325="rare", 0.792892156862745, 1)))</f>
@@ -6791,7 +6791,7 @@
         <v>0.08</v>
       </c>
       <c r="E118" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F118" s="3">
         <f>IF(B118:B326="common", 4, IF(B118:B326="uncommon", 3, IF(B118:B326="rare", 0.792892156862745, 1)))</f>
@@ -6844,7 +6844,7 @@
         <v>0.1</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>2.18</v>
+        <v>2.61</v>
       </c>
       <c r="F119" s="3">
         <f>IF(B119:B327="common", 4, IF(B119:B327="uncommon", 3, IF(B119:B327="rare", 0.792892156862745, 1)))</f>
@@ -6894,7 +6894,7 @@
         <v>90</v>
       </c>
       <c r="D120" s="3" t="n">
-        <v>6.41</v>
+        <v>6.32</v>
       </c>
       <c r="E120" s="3" t="inlineStr"/>
       <c r="F120" s="3">
@@ -6945,7 +6945,7 @@
         <v>248</v>
       </c>
       <c r="D121" s="3" t="n">
-        <v>18.51</v>
+        <v>17.12</v>
       </c>
       <c r="E121" s="3" t="inlineStr"/>
       <c r="F121" s="3">
@@ -6996,7 +6996,7 @@
         <v>154</v>
       </c>
       <c r="D122" s="3" t="n">
-        <v>12.65</v>
+        <v>12</v>
       </c>
       <c r="E122" s="3" t="inlineStr"/>
       <c r="F122" s="3">
@@ -7047,7 +7047,7 @@
         <v>90</v>
       </c>
       <c r="D123" s="3" t="n">
-        <v>10.27</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E123" s="3" t="inlineStr"/>
       <c r="F123" s="3">
@@ -7098,10 +7098,10 @@
         <v>21</v>
       </c>
       <c r="D124" s="3" t="n">
-        <v>0.55</v>
+        <v>0.47</v>
       </c>
       <c r="E124" s="3" t="n">
-        <v>1.58</v>
+        <v>1.46</v>
       </c>
       <c r="F124" s="3">
         <f>IF(B124:B332="common", 4, IF(B124:B332="uncommon", 3, IF(B124:B332="rare", 0.792892156862745, 1)))</f>
@@ -7154,7 +7154,7 @@
         <v>0.24</v>
       </c>
       <c r="E125" s="3" t="n">
-        <v>0.74</v>
+        <v>0.63</v>
       </c>
       <c r="F125" s="3">
         <f>IF(B125:B333="common", 4, IF(B125:B333="uncommon", 3, IF(B125:B333="rare", 0.792892156862745, 1)))</f>
@@ -7204,10 +7204,10 @@
         <v>21</v>
       </c>
       <c r="D126" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E126" s="3" t="n">
-        <v>0.57</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F126" s="3">
         <f>IF(B126:B334="common", 4, IF(B126:B334="uncommon", 3, IF(B126:B334="rare", 0.792892156862745, 1)))</f>
@@ -7257,7 +7257,7 @@
         <v>188</v>
       </c>
       <c r="D127" s="3" t="n">
-        <v>5.65</v>
+        <v>5.29</v>
       </c>
       <c r="E127" s="3" t="inlineStr"/>
       <c r="F127" s="3">
@@ -7308,10 +7308,10 @@
         <v>33</v>
       </c>
       <c r="D128" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E128" s="3" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="F128" s="3">
         <f>IF(B128:B336="common", 4, IF(B128:B336="uncommon", 3, IF(B128:B336="rare", 0.792892156862745, 1)))</f>
@@ -7364,7 +7364,7 @@
         <v>0.16</v>
       </c>
       <c r="E129" s="3" t="n">
-        <v>0.76</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F129" s="3">
         <f>IF(B129:B337="common", 4, IF(B129:B337="uncommon", 3, IF(B129:B337="rare", 0.792892156862745, 1)))</f>
@@ -7414,7 +7414,7 @@
         <v>188</v>
       </c>
       <c r="D130" s="3" t="n">
-        <v>9.49</v>
+        <v>9.109999999999999</v>
       </c>
       <c r="E130" s="3" t="inlineStr"/>
       <c r="F130" s="3">
@@ -7468,7 +7468,7 @@
         <v>0.09</v>
       </c>
       <c r="E131" s="3" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="F131" s="3">
         <f>IF(B131:B339="common", 4, IF(B131:B339="uncommon", 3, IF(B131:B339="rare", 0.792892156862745, 1)))</f>
@@ -7518,10 +7518,10 @@
         <v>46</v>
       </c>
       <c r="D132" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="E132" s="3" t="n">
-        <v>1.67</v>
+        <v>1.46</v>
       </c>
       <c r="F132" s="3">
         <f>IF(B132:B340="common", 4, IF(B132:B340="uncommon", 3, IF(B132:B340="rare", 0.792892156862745, 1)))</f>
@@ -7574,7 +7574,7 @@
         <v>0.1</v>
       </c>
       <c r="E133" s="3" t="n">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="F133" s="3">
         <f>IF(B133:B341="common", 4, IF(B133:B341="uncommon", 3, IF(B133:B341="rare", 0.792892156862745, 1)))</f>
@@ -7680,7 +7680,7 @@
         <v>0.05</v>
       </c>
       <c r="E135" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F135" s="3">
         <f>IF(B135:B343="common", 4, IF(B135:B343="uncommon", 3, IF(B135:B343="rare", 0.792892156862745, 1)))</f>
@@ -7730,7 +7730,7 @@
         <v>90</v>
       </c>
       <c r="D136" s="3" t="n">
-        <v>1.13</v>
+        <v>1.02</v>
       </c>
       <c r="E136" s="3" t="inlineStr"/>
       <c r="F136" s="3">
@@ -7781,7 +7781,7 @@
         <v>248</v>
       </c>
       <c r="D137" s="3" t="n">
-        <v>7.37</v>
+        <v>7.43</v>
       </c>
       <c r="E137" s="3" t="inlineStr"/>
       <c r="F137" s="3">
@@ -7832,7 +7832,7 @@
         <v>46</v>
       </c>
       <c r="D138" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E138" s="3" t="n">
         <v>0.14</v>
@@ -7888,7 +7888,7 @@
         <v>0.09</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>1.84</v>
+        <v>1.69</v>
       </c>
       <c r="F139" s="3">
         <f>IF(B139:B347="common", 4, IF(B139:B347="uncommon", 3, IF(B139:B347="rare", 0.792892156862745, 1)))</f>
@@ -7938,7 +7938,7 @@
         <v>188</v>
       </c>
       <c r="D140" s="3" t="n">
-        <v>5.82</v>
+        <v>5.73</v>
       </c>
       <c r="E140" s="3" t="inlineStr"/>
       <c r="F140" s="3">
@@ -7989,10 +7989,10 @@
         <v>21</v>
       </c>
       <c r="D141" s="3" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="E141" s="3" t="n">
-        <v>0.68</v>
+        <v>0.57</v>
       </c>
       <c r="F141" s="3">
         <f>IF(B141:B349="common", 4, IF(B141:B349="uncommon", 3, IF(B141:B349="rare", 0.792892156862745, 1)))</f>
@@ -8042,10 +8042,10 @@
         <v>33</v>
       </c>
       <c r="D142" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E142" s="3" t="n">
-        <v>1.46</v>
+        <v>1.45</v>
       </c>
       <c r="F142" s="3">
         <f>IF(B142:B350="common", 4, IF(B142:B350="uncommon", 3, IF(B142:B350="rare", 0.792892156862745, 1)))</f>
@@ -8098,7 +8098,7 @@
         <v>0.05</v>
       </c>
       <c r="E143" s="3" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="F143" s="3">
         <f>IF(B143:B351="common", 4, IF(B143:B351="uncommon", 3, IF(B143:B351="rare", 0.792892156862745, 1)))</f>
@@ -8151,7 +8151,7 @@
         <v>0.06</v>
       </c>
       <c r="E144" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F144" s="3">
         <f>IF(B144:B352="common", 4, IF(B144:B352="uncommon", 3, IF(B144:B352="rare", 0.792892156862745, 1)))</f>
@@ -8201,10 +8201,10 @@
         <v>33</v>
       </c>
       <c r="D145" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F145" s="3">
         <f>IF(B145:B353="common", 4, IF(B145:B353="uncommon", 3, IF(B145:B353="rare", 0.792892156862745, 1)))</f>
@@ -8254,10 +8254,10 @@
         <v>33</v>
       </c>
       <c r="D146" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E146" s="3" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="F146" s="3">
         <f>IF(B146:B354="common", 4, IF(B146:B354="uncommon", 3, IF(B146:B354="rare", 0.792892156862745, 1)))</f>
@@ -8307,10 +8307,10 @@
         <v>46</v>
       </c>
       <c r="D147" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>2.07</v>
+        <v>2.4</v>
       </c>
       <c r="F147" s="3">
         <f>IF(B147:B355="common", 4, IF(B147:B355="uncommon", 3, IF(B147:B355="rare", 0.792892156862745, 1)))</f>
@@ -8363,7 +8363,7 @@
         <v>0.1</v>
       </c>
       <c r="E148" s="3" t="n">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
       <c r="F148" s="3">
         <f>IF(B148:B356="common", 4, IF(B148:B356="uncommon", 3, IF(B148:B356="rare", 0.792892156862745, 1)))</f>
@@ -8413,10 +8413,10 @@
         <v>46</v>
       </c>
       <c r="D149" s="3" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="E149" s="3" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="F149" s="3">
         <f>IF(B149:B357="common", 4, IF(B149:B357="uncommon", 3, IF(B149:B357="rare", 0.792892156862745, 1)))</f>
@@ -8466,7 +8466,7 @@
         <v>188</v>
       </c>
       <c r="D150" s="3" t="n">
-        <v>24.97</v>
+        <v>24.78</v>
       </c>
       <c r="E150" s="3" t="inlineStr"/>
       <c r="F150" s="3">
@@ -8517,10 +8517,10 @@
         <v>33</v>
       </c>
       <c r="D151" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>1.54</v>
+        <v>1.42</v>
       </c>
       <c r="F151" s="3">
         <f>IF(B151:B359="common", 4, IF(B151:B359="uncommon", 3, IF(B151:B359="rare", 0.792892156862745, 1)))</f>
@@ -8623,10 +8623,10 @@
         <v>46</v>
       </c>
       <c r="D153" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>1.85</v>
+        <v>1.79</v>
       </c>
       <c r="F153" s="3">
         <f>IF(B153:B361="common", 4, IF(B153:B361="uncommon", 3, IF(B153:B361="rare", 0.792892156862745, 1)))</f>
@@ -8676,7 +8676,7 @@
         <v>188</v>
       </c>
       <c r="D154" s="3" t="n">
-        <v>17.04</v>
+        <v>16.93</v>
       </c>
       <c r="E154" s="3" t="inlineStr"/>
       <c r="F154" s="3">
@@ -8727,10 +8727,10 @@
         <v>33</v>
       </c>
       <c r="D155" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E155" s="3" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="F155" s="3">
         <f>IF(B155:B363="common", 4, IF(B155:B363="uncommon", 3, IF(B155:B363="rare", 0.792892156862745, 1)))</f>
@@ -8783,7 +8783,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E156" s="3" t="n">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="F156" s="3">
         <f>IF(B156:B364="common", 4, IF(B156:B364="uncommon", 3, IF(B156:B364="rare", 0.792892156862745, 1)))</f>
@@ -8836,7 +8836,7 @@
         <v>0.06</v>
       </c>
       <c r="E157" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F157" s="3">
         <f>IF(B157:B365="common", 4, IF(B157:B365="uncommon", 3, IF(B157:B365="rare", 0.792892156862745, 1)))</f>
@@ -8886,7 +8886,7 @@
         <v>33</v>
       </c>
       <c r="D158" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E158" s="3" t="n">
         <v>0.16</v>
@@ -8939,10 +8939,10 @@
         <v>33</v>
       </c>
       <c r="D159" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="F159" s="3">
         <f>IF(B159:B367="common", 4, IF(B159:B367="uncommon", 3, IF(B159:B367="rare", 0.792892156862745, 1)))</f>
@@ -8992,10 +8992,10 @@
         <v>46</v>
       </c>
       <c r="D160" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E160" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F160" s="3">
         <f>IF(B160:B368="common", 4, IF(B160:B368="uncommon", 3, IF(B160:B368="rare", 0.792892156862745, 1)))</f>
@@ -9045,7 +9045,7 @@
         <v>188</v>
       </c>
       <c r="D161" s="3" t="n">
-        <v>18.79</v>
+        <v>18.6</v>
       </c>
       <c r="E161" s="3" t="inlineStr"/>
       <c r="F161" s="3">
@@ -9096,10 +9096,10 @@
         <v>21</v>
       </c>
       <c r="D162" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E162" s="3" t="n">
-        <v>1.19</v>
+        <v>1.21</v>
       </c>
       <c r="F162" s="3">
         <f>IF(B162:B370="common", 4, IF(B162:B370="uncommon", 3, IF(B162:B370="rare", 0.792892156862745, 1)))</f>
@@ -9149,10 +9149,10 @@
         <v>33</v>
       </c>
       <c r="D163" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F163" s="3">
         <f>IF(B163:B371="common", 4, IF(B163:B371="uncommon", 3, IF(B163:B371="rare", 0.792892156862745, 1)))</f>
@@ -9202,10 +9202,10 @@
         <v>33</v>
       </c>
       <c r="D164" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E164" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F164" s="3">
         <f>IF(B164:B372="common", 4, IF(B164:B372="uncommon", 3, IF(B164:B372="rare", 0.792892156862745, 1)))</f>
@@ -9258,7 +9258,7 @@
         <v>0.05</v>
       </c>
       <c r="E165" s="3" t="n">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="F165" s="3">
         <f>IF(B165:B373="common", 4, IF(B165:B373="uncommon", 3, IF(B165:B373="rare", 0.792892156862745, 1)))</f>
@@ -9308,10 +9308,10 @@
         <v>33</v>
       </c>
       <c r="D166" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E166" s="3" t="n">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="F166" s="3">
         <f>IF(B166:B374="common", 4, IF(B166:B374="uncommon", 3, IF(B166:B374="rare", 0.792892156862745, 1)))</f>
@@ -9361,10 +9361,10 @@
         <v>46</v>
       </c>
       <c r="D167" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E167" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F167" s="3">
         <f>IF(B167:B375="common", 4, IF(B167:B375="uncommon", 3, IF(B167:B375="rare", 0.792892156862745, 1)))</f>
@@ -9414,10 +9414,10 @@
         <v>33</v>
       </c>
       <c r="D168" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E168" s="3" t="n">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="F168" s="3">
         <f>IF(B168:B376="common", 4, IF(B168:B376="uncommon", 3, IF(B168:B376="rare", 0.792892156862745, 1)))</f>
@@ -9467,7 +9467,7 @@
         <v>46</v>
       </c>
       <c r="D169" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E169" s="3" t="n">
         <v>0.17</v>
@@ -9523,7 +9523,7 @@
         <v>0.05</v>
       </c>
       <c r="E170" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F170" s="3">
         <f>IF(B170:B378="common", 4, IF(B170:B378="uncommon", 3, IF(B170:B378="rare", 0.792892156862745, 1)))</f>
@@ -9573,10 +9573,10 @@
         <v>33</v>
       </c>
       <c r="D171" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>2.65</v>
+        <v>2.37</v>
       </c>
       <c r="F171" s="3">
         <f>IF(B171:B379="common", 4, IF(B171:B379="uncommon", 3, IF(B171:B379="rare", 0.792892156862745, 1)))</f>
@@ -9626,10 +9626,10 @@
         <v>33</v>
       </c>
       <c r="D172" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E172" s="3" t="n">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="F172" s="3">
         <f>IF(B172:B380="common", 4, IF(B172:B380="uncommon", 3, IF(B172:B380="rare", 0.792892156862745, 1)))</f>
@@ -9679,10 +9679,10 @@
         <v>33</v>
       </c>
       <c r="D173" s="3" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="F173" s="3">
         <f>IF(B173:B381="common", 4, IF(B173:B381="uncommon", 3, IF(B173:B381="rare", 0.792892156862745, 1)))</f>
@@ -9785,10 +9785,10 @@
         <v>46</v>
       </c>
       <c r="D175" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>0.17</v>
+        <v>0.13</v>
       </c>
       <c r="F175" s="3">
         <f>IF(B175:B383="common", 4, IF(B175:B383="uncommon", 3, IF(B175:B383="rare", 0.792892156862745, 1)))</f>
@@ -9838,10 +9838,10 @@
         <v>33</v>
       </c>
       <c r="D176" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E176" s="3" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="F176" s="3">
         <f>IF(B176:B384="common", 4, IF(B176:B384="uncommon", 3, IF(B176:B384="rare", 0.792892156862745, 1)))</f>
@@ -9891,10 +9891,10 @@
         <v>46</v>
       </c>
       <c r="D177" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>0.13</v>
+        <v>0.17</v>
       </c>
       <c r="F177" s="3">
         <f>IF(B177:B385="common", 4, IF(B177:B385="uncommon", 3, IF(B177:B385="rare", 0.792892156862745, 1)))</f>
@@ -9944,10 +9944,10 @@
         <v>33</v>
       </c>
       <c r="D178" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E178" s="3" t="n">
-        <v>1.22</v>
+        <v>1.18</v>
       </c>
       <c r="F178" s="3">
         <f>IF(B178:B386="common", 4, IF(B178:B386="uncommon", 3, IF(B178:B386="rare", 0.792892156862745, 1)))</f>
@@ -9997,10 +9997,10 @@
         <v>46</v>
       </c>
       <c r="D179" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>0.83</v>
+        <v>1.07</v>
       </c>
       <c r="F179" s="3">
         <f>IF(B179:B387="common", 4, IF(B179:B387="uncommon", 3, IF(B179:B387="rare", 0.792892156862745, 1)))</f>
@@ -10050,7 +10050,7 @@
         <v>46</v>
       </c>
       <c r="D180" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E180" s="3" t="n">
         <v>0.18</v>
@@ -10103,7 +10103,7 @@
         <v>188</v>
       </c>
       <c r="D181" s="3" t="n">
-        <v>40</v>
+        <v>38.56</v>
       </c>
       <c r="E181" s="3" t="inlineStr"/>
       <c r="F181" s="3">
@@ -10157,7 +10157,7 @@
         <v>0.16</v>
       </c>
       <c r="E182" s="3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.57</v>
       </c>
       <c r="F182" s="3">
         <f>IF(B182:B390="common", 4, IF(B182:B390="uncommon", 3, IF(B182:B390="rare", 0.792892156862745, 1)))</f>
@@ -10207,10 +10207,10 @@
         <v>46</v>
       </c>
       <c r="D183" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E183" s="3" t="n">
-        <v>0.14</v>
+        <v>0.18</v>
       </c>
       <c r="F183" s="3">
         <f>IF(B183:B391="common", 4, IF(B183:B391="uncommon", 3, IF(B183:B391="rare", 0.792892156862745, 1)))</f>
@@ -10260,7 +10260,7 @@
         <v>154</v>
       </c>
       <c r="D184" s="3" t="n">
-        <v>2.85</v>
+        <v>2.19</v>
       </c>
       <c r="E184" s="3" t="inlineStr"/>
       <c r="F184" s="3">
@@ -10311,10 +10311,10 @@
         <v>46</v>
       </c>
       <c r="D185" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E185" s="3" t="n">
-        <v>0.14</v>
+        <v>0.17</v>
       </c>
       <c r="F185" s="3">
         <f>IF(B185:B393="common", 4, IF(B185:B393="uncommon", 3, IF(B185:B393="rare", 0.792892156862745, 1)))</f>
@@ -10364,7 +10364,7 @@
         <v>188</v>
       </c>
       <c r="D186" s="3" t="n">
-        <v>6.7</v>
+        <v>6.47</v>
       </c>
       <c r="E186" s="3" t="inlineStr"/>
       <c r="F186" s="3">
@@ -10418,7 +10418,7 @@
         <v>0.1</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>0.87</v>
+        <v>0.85</v>
       </c>
       <c r="F187" s="3">
         <f>IF(B187:B395="common", 4, IF(B187:B395="uncommon", 3, IF(B187:B395="rare", 0.792892156862745, 1)))</f>
@@ -10471,7 +10471,7 @@
         <v>0.06</v>
       </c>
       <c r="E188" s="3" t="n">
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="F188" s="3">
         <f>IF(B188:B396="common", 4, IF(B188:B396="uncommon", 3, IF(B188:B396="rare", 0.792892156862745, 1)))</f>
@@ -10521,10 +10521,10 @@
         <v>33</v>
       </c>
       <c r="D189" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E189" s="3" t="n">
-        <v>0.14</v>
+        <v>0.17</v>
       </c>
       <c r="F189" s="3">
         <f>IF(B189:B397="common", 4, IF(B189:B397="uncommon", 3, IF(B189:B397="rare", 0.792892156862745, 1)))</f>
@@ -10574,10 +10574,10 @@
         <v>21</v>
       </c>
       <c r="D190" s="3" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E190" s="3" t="n">
-        <v>1.46</v>
+        <v>1.31</v>
       </c>
       <c r="F190" s="3">
         <f>IF(B190:B398="common", 4, IF(B190:B398="uncommon", 3, IF(B190:B398="rare", 0.792892156862745, 1)))</f>
@@ -10627,10 +10627,10 @@
         <v>33</v>
       </c>
       <c r="D191" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="F191" s="3">
         <f>IF(B191:B399="common", 4, IF(B191:B399="uncommon", 3, IF(B191:B399="rare", 0.792892156862745, 1)))</f>
@@ -10680,10 +10680,10 @@
         <v>46</v>
       </c>
       <c r="D192" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E192" s="3" t="n">
-        <v>0.13</v>
+        <v>0.17</v>
       </c>
       <c r="F192" s="3">
         <f>IF(B192:B400="common", 4, IF(B192:B400="uncommon", 3, IF(B192:B400="rare", 0.792892156862745, 1)))</f>
@@ -10733,7 +10733,7 @@
         <v>90</v>
       </c>
       <c r="D193" s="3" t="n">
-        <v>0.55</v>
+        <v>0.73</v>
       </c>
       <c r="E193" s="3" t="inlineStr"/>
       <c r="F193" s="3">
@@ -10784,7 +10784,7 @@
         <v>248</v>
       </c>
       <c r="D194" s="3" t="n">
-        <v>9.69</v>
+        <v>9.470000000000001</v>
       </c>
       <c r="E194" s="3" t="inlineStr"/>
       <c r="F194" s="3">
@@ -10835,7 +10835,7 @@
         <v>225</v>
       </c>
       <c r="D195" s="3" t="n">
-        <v>57.96</v>
+        <v>57.55</v>
       </c>
       <c r="E195" s="3" t="inlineStr"/>
       <c r="F195" s="3">
@@ -10939,7 +10939,7 @@
         <v>21</v>
       </c>
       <c r="D197" s="3" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="E197" s="3" t="n">
         <v>0.77</v>
@@ -10995,7 +10995,7 @@
         <v>0.06</v>
       </c>
       <c r="E198" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F198" s="3">
         <f>IF(B198:B406="common", 4, IF(B198:B406="uncommon", 3, IF(B198:B406="rare", 0.792892156862745, 1)))</f>
@@ -11045,10 +11045,10 @@
         <v>46</v>
       </c>
       <c r="D199" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E199" s="3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="F199" s="3">
         <f>IF(B199:B407="common", 4, IF(B199:B407="uncommon", 3, IF(B199:B407="rare", 0.792892156862745, 1)))</f>
@@ -11101,7 +11101,7 @@
         <v>0.1</v>
       </c>
       <c r="E200" s="3" t="n">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="F200" s="3">
         <f>IF(B200:B408="common", 4, IF(B200:B408="uncommon", 3, IF(B200:B408="rare", 0.792892156862745, 1)))</f>
@@ -11151,7 +11151,7 @@
         <v>188</v>
       </c>
       <c r="D201" s="3" t="n">
-        <v>24.22</v>
+        <v>23.06</v>
       </c>
       <c r="E201" s="3" t="inlineStr"/>
       <c r="F201" s="3">
@@ -11255,10 +11255,10 @@
         <v>46</v>
       </c>
       <c r="D203" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E203" s="3" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="F203" s="3">
         <f>IF(B203:B411="common", 4, IF(B203:B411="uncommon", 3, IF(B203:B411="rare", 0.792892156862745, 1)))</f>
@@ -11311,7 +11311,7 @@
         <v>0.13</v>
       </c>
       <c r="E204" s="3" t="n">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="F204" s="3">
         <f>IF(B204:B412="common", 4, IF(B204:B412="uncommon", 3, IF(B204:B412="rare", 0.792892156862745, 1)))</f>
@@ -11361,7 +11361,7 @@
         <v>90</v>
       </c>
       <c r="D205" s="3" t="n">
-        <v>0.64</v>
+        <v>0.74</v>
       </c>
       <c r="E205" s="3" t="inlineStr"/>
       <c r="F205" s="3">
@@ -11412,7 +11412,7 @@
         <v>248</v>
       </c>
       <c r="D206" s="3" t="n">
-        <v>6.9</v>
+        <v>6.27</v>
       </c>
       <c r="E206" s="3" t="inlineStr"/>
       <c r="F206" s="3">
@@ -11463,7 +11463,7 @@
         <v>90</v>
       </c>
       <c r="D207" s="3" t="n">
-        <v>0.76</v>
+        <v>0.8</v>
       </c>
       <c r="E207" s="3" t="inlineStr"/>
       <c r="F207" s="3">
@@ -11514,7 +11514,7 @@
         <v>248</v>
       </c>
       <c r="D208" s="3" t="n">
-        <v>7.15</v>
+        <v>7.23</v>
       </c>
       <c r="E208" s="3" t="inlineStr"/>
       <c r="F208" s="3">
@@ -11565,7 +11565,7 @@
         <v>225</v>
       </c>
       <c r="D209" s="3" t="n">
-        <v>46.15</v>
+        <v>47.08</v>
       </c>
       <c r="E209" s="3" t="inlineStr"/>
       <c r="F209" s="3">
@@ -18308,7 +18308,7 @@
         </is>
       </c>
       <c r="B2" s="13" t="n">
-        <v>0.4304347826086957</v>
+        <v>0.4008695652173913</v>
       </c>
     </row>
     <row r="3">
@@ -18318,7 +18318,7 @@
         </is>
       </c>
       <c r="B3" s="13" t="n">
-        <v>0.4881818181818181</v>
+        <v>0.4536363636363635</v>
       </c>
     </row>
     <row r="4">
@@ -18328,7 +18328,7 @@
         </is>
       </c>
       <c r="B4" s="13" t="n">
-        <v>0.2016211484593838</v>
+        <v>0.1925595238095238</v>
       </c>
     </row>
     <row r="5">
@@ -18338,7 +18338,7 @@
         </is>
       </c>
       <c r="B5" s="13" t="n">
-        <v>5.329323789133571</v>
+        <v>5.212912706255096</v>
       </c>
     </row>
     <row r="6">
@@ -18378,7 +18378,7 @@
         </is>
       </c>
       <c r="B9" s="13" t="n">
-        <v>1.740372340425532</v>
+        <v>1.716223404255319</v>
       </c>
     </row>
     <row r="10">
@@ -18388,7 +18388,7 @@
         </is>
       </c>
       <c r="B10" s="13" t="n">
-        <v>1.954666666666667</v>
+        <v>1.917866666666667</v>
       </c>
     </row>
     <row r="11">
@@ -18398,7 +18398,7 @@
         </is>
       </c>
       <c r="B11" s="13" t="n">
-        <v>0.3157777777777778</v>
+        <v>0.3143333333333334</v>
       </c>
     </row>
     <row r="12">
@@ -18408,7 +18408,7 @@
         </is>
       </c>
       <c r="B12" s="13" t="n">
-        <v>0.1305844155844156</v>
+        <v>0.121038961038961</v>
       </c>
     </row>
     <row r="13">
@@ -18418,7 +18418,7 @@
         </is>
       </c>
       <c r="B13" s="13" t="n">
-        <v>0.5363709677419355</v>
+        <v>0.5255241935483871</v>
       </c>
     </row>
     <row r="14">
@@ -18448,7 +18448,7 @@
         </is>
       </c>
       <c r="B16" s="13" t="n">
-        <v>4.677772168196328</v>
+        <v>4.594986558842668</v>
       </c>
     </row>
     <row r="17">
@@ -18458,7 +18458,7 @@
         </is>
       </c>
       <c r="B17" s="13" t="n">
-        <v>11.12733370657979</v>
+        <v>10.85496471776104</v>
       </c>
     </row>
     <row r="18">
@@ -18468,7 +18468,7 @@
         </is>
       </c>
       <c r="B18" s="13" t="n">
-        <v>1.397333706579793</v>
+        <v>0.9649647177610419</v>
       </c>
     </row>
     <row r="19">
@@ -18478,7 +18478,7 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>1.14361086398559</v>
+        <v>1.097569738904049</v>
       </c>
     </row>
     <row r="20">
@@ -18488,7 +18488,7 @@
         </is>
       </c>
       <c r="B20" s="15" t="n">
-        <v>0.1436108639855902</v>
+        <v>0.09756973890404863</v>
       </c>
     </row>
     <row r="21">

</xml_diff>